<commit_message>
process results of SPEC run
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE5B6C2-C597-604F-BBF6-EF495ED79A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D58AE3-6BD5-DC4E-8919-8A456D14B05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -213,6 +213,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -608,9 +611,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -666,6 +666,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -985,7 +988,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G18" sqref="G18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,40 +1017,40 @@
     </row>
     <row r="4" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="37" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="40" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="41"/>
+      <c r="E5" s="40"/>
       <c r="F5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="41"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="21" t="s">
         <v>16</v>
       </c>
@@ -1091,21 +1094,25 @@
       <c r="C7" s="13">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <v>10930</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="27">
         <v>0.16200000000000001</v>
       </c>
       <c r="F7" s="18">
         <f>D7/$B7</f>
         <v>3.5707285200914733</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="G7" s="26">
+        <v>12673</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="I7" s="18">
         <f>G7/$B7</f>
-        <v>0</v>
+        <v>4.14015027768703</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1118,21 +1125,25 @@
       <c r="C8" s="15">
         <v>1.17</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>9301</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>0.42799999999999999</v>
       </c>
       <c r="F8" s="19">
         <f t="shared" ref="F8:F16" si="0">D8/$B8</f>
         <v>2.7436578171091446</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="28">
+        <v>10375</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.38400000000000001</v>
+      </c>
       <c r="I8" s="19">
         <f t="shared" ref="I8:I16" si="1">G8/$B8</f>
-        <v>0</v>
+        <v>3.0604719764011801</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1145,21 +1156,25 @@
       <c r="C9" s="15">
         <v>1.48</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>3654</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>1.29</v>
       </c>
       <c r="F9" s="19">
         <f t="shared" si="0"/>
         <v>1.1483343808925204</v>
       </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+      <c r="G9" s="28">
+        <v>4774</v>
+      </c>
+      <c r="H9" s="29">
+        <v>0.98899999999999999</v>
+      </c>
       <c r="I9" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5003142677561283</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1172,21 +1187,25 @@
       <c r="C10" s="15">
         <v>0.63300000000000001</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>8210</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>0.19900000000000001</v>
       </c>
       <c r="F10" s="19">
         <f t="shared" si="0"/>
         <v>3.1871118012422359</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="G10" s="28">
+        <v>10257</v>
+      </c>
+      <c r="H10" s="29">
+        <v>0.159</v>
+      </c>
       <c r="I10" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.9817546583850931</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1199,21 +1218,25 @@
       <c r="C11" s="15">
         <v>0.82799999999999996</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="28">
         <v>4563</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>0.311</v>
       </c>
       <c r="F11" s="19">
         <f t="shared" si="0"/>
         <v>2.6668614845119811</v>
       </c>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
+      <c r="G11" s="28">
+        <v>5285</v>
+      </c>
+      <c r="H11" s="29">
+        <v>0.26800000000000002</v>
+      </c>
       <c r="I11" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.0888369374634714</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1226,21 +1249,25 @@
       <c r="C12" s="15">
         <v>0.60399999999999998</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="28">
         <v>4333</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>0.40699999999999997</v>
       </c>
       <c r="F12" s="19">
         <f t="shared" si="0"/>
         <v>1.4833960972269771</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
+      <c r="G12" s="28">
+        <v>4305</v>
+      </c>
+      <c r="H12" s="29">
+        <v>0.41</v>
+      </c>
       <c r="I12" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4738103389250257</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1253,21 +1280,25 @@
       <c r="C13" s="15">
         <v>0.58299999999999996</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>10330</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <v>0.13900000000000001</v>
       </c>
       <c r="F13" s="19">
         <f t="shared" si="0"/>
         <v>4.2008946726311507</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
+      <c r="G13" s="28">
+        <v>10327</v>
+      </c>
+      <c r="H13" s="29">
+        <v>0.13900000000000001</v>
+      </c>
       <c r="I13" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.1996746644977634</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1280,21 +1311,25 @@
       <c r="C14" s="15">
         <v>0.53800000000000003</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>7517</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <v>0.22700000000000001</v>
       </c>
       <c r="F14" s="19">
         <f t="shared" si="0"/>
         <v>2.3705455692210657</v>
       </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="30"/>
+      <c r="G14" s="28">
+        <v>6737</v>
+      </c>
+      <c r="H14" s="29">
+        <v>0.253</v>
+      </c>
       <c r="I14" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.1245663828445287</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1307,21 +1342,25 @@
       <c r="C15" s="15">
         <v>1.33</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>4891</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <v>0.60099999999999998</v>
       </c>
       <c r="F15" s="19">
         <f t="shared" si="0"/>
         <v>2.2101220063262539</v>
       </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
+      <c r="G15" s="28">
+        <v>4807</v>
+      </c>
+      <c r="H15" s="29">
+        <v>0.61199999999999999</v>
+      </c>
       <c r="I15" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.1721644826028017</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1334,59 +1373,68 @@
       <c r="C16" s="17">
         <v>0.69299999999999995</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="30">
         <v>12625</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <v>0.49</v>
       </c>
       <c r="F16" s="20">
         <f t="shared" si="0"/>
         <v>1.4161525518788558</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="G16" s="30">
+        <v>13272</v>
+      </c>
+      <c r="H16" s="31">
+        <v>0.46600000000000003</v>
+      </c>
       <c r="I16" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4887268648345484</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="42" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="43"/>
+      <c r="H17" s="42"/>
       <c r="I17" s="25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="48">
+      <c r="B18" s="47">
         <v>0.78810000000000002</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="33">
+      <c r="C18" s="48"/>
+      <c r="D18" s="32">
         <v>0.3337</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="26">
+      <c r="E18" s="33"/>
+      <c r="F18" s="49">
         <f>$B$18/D18</f>
         <v>2.3617021276595747</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="26"/>
+      <c r="G18" s="32">
+        <v>0.31390000000000001</v>
+      </c>
+      <c r="H18" s="33"/>
+      <c r="I18" s="49">
+        <f>$B$18/G18</f>
+        <v>2.5106721885950938</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">

</xml_diff>

<commit_message>
include results in overview
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D58AE3-6BD5-DC4E-8919-8A456D14B05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1147B47B-B1C2-3740-B695-74660B4E4247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Benchmark</t>
   </si>
@@ -208,13 +208,28 @@
       <t>&lt;last git version tag&gt;–&lt;no. of commits between HEAD &amp; last tag&gt; (latest commit hash)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>v1.2.2-12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (b904a345)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -284,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -560,11 +575,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -572,11 +650,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,6 +690,9 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,9 +744,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2E7EA3-8BF5-F743-9E89-1A0A4F76CDF3}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:H18"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,443 +1093,618 @@
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="36" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
-    </row>
-    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="33"/>
+      <c r="L4" s="34"/>
+    </row>
+    <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="39" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="21" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="J5" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="36"/>
+      <c r="L5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="J6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="7">
         <v>3061</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="21">
         <v>10930</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="22">
         <v>0.16200000000000001</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="13">
         <f>D7/$B7</f>
         <v>3.5707285200914733</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="21">
         <v>12673</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="22">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="13">
         <f>G7/$B7</f>
         <v>4.14015027768703</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="J7" s="21">
+        <v>10971</v>
+      </c>
+      <c r="K7" s="22">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="L7" s="13">
+        <f>J7/$B7</f>
+        <v>3.584122835674616</v>
+      </c>
+      <c r="M7" s="47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="9">
         <v>3390</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="10">
         <v>1.17</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="23">
         <v>9301</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="24">
         <v>0.42799999999999999</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="14">
         <f t="shared" ref="F8:F16" si="0">D8/$B8</f>
         <v>2.7436578171091446</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="23">
         <v>10375</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="24">
         <v>0.38400000000000001</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="14">
         <f t="shared" ref="I8:I16" si="1">G8/$B8</f>
         <v>3.0604719764011801</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="J8" s="23">
+        <v>8693</v>
+      </c>
+      <c r="K8" s="24">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" ref="L8:L16" si="2">J8/$B8</f>
+        <v>2.5643067846607668</v>
+      </c>
+      <c r="M8" s="48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="9">
         <v>3182</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="10">
         <v>1.48</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="23">
         <v>3654</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="24">
         <v>1.29</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>1.1483343808925204</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="23">
         <v>4774</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="24">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="14">
         <f t="shared" si="1"/>
         <v>1.5003142677561283</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="J9" s="23">
+        <v>3558</v>
+      </c>
+      <c r="K9" s="24">
+        <v>1.33</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="2"/>
+        <v>1.1181646763042112</v>
+      </c>
+      <c r="M9" s="48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="9">
         <v>2576</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="10">
         <v>0.63300000000000001</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="23">
         <v>8210</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="24">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
         <v>3.1871118012422359</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="23">
         <v>10257</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="24">
         <v>0.159</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="14">
         <f t="shared" si="1"/>
         <v>3.9817546583850931</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="J10" s="23">
+        <v>7892</v>
+      </c>
+      <c r="K10" s="24">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="2"/>
+        <v>3.0636645962732918</v>
+      </c>
+      <c r="M10" s="48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="9">
         <v>1711</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="10">
         <v>0.82799999999999996</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="23">
         <v>4563</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="24">
         <v>0.311</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="14">
         <f t="shared" si="0"/>
         <v>2.6668614845119811</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="23">
         <v>5285</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="24">
         <v>0.26800000000000002</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="14">
         <f t="shared" si="1"/>
         <v>3.0888369374634714</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="J11" s="23">
+        <v>4313</v>
+      </c>
+      <c r="K11" s="24">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="2"/>
+        <v>2.5207481005260082</v>
+      </c>
+      <c r="M11" s="48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="9">
         <v>2921</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="10">
         <v>0.60399999999999998</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="23">
         <v>4333</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="24">
         <v>0.40699999999999997</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
         <v>1.4833960972269771</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="23">
         <v>4305</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="24">
         <v>0.41</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="14">
         <f t="shared" si="1"/>
         <v>1.4738103389250257</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="J12" s="23">
+        <v>4009</v>
+      </c>
+      <c r="K12" s="24">
+        <v>0.44</v>
+      </c>
+      <c r="L12" s="14">
+        <f t="shared" si="2"/>
+        <v>1.3724751797329682</v>
+      </c>
+      <c r="M12" s="48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="9">
         <v>2459</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="10">
         <v>0.58299999999999996</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="23">
         <v>10330</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="24">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="14">
         <f t="shared" si="0"/>
         <v>4.2008946726311507</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="23">
         <v>10327</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="24">
         <v>0.13900000000000001</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="14">
         <f t="shared" si="1"/>
         <v>4.1996746644977634</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="J13" s="23">
+        <v>10089</v>
+      </c>
+      <c r="K13" s="24">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" si="2"/>
+        <v>4.1028873525823508</v>
+      </c>
+      <c r="M13" s="48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="9">
         <v>3171</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="10">
         <v>0.53800000000000003</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="23">
         <v>7517</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="24">
         <v>0.22700000000000001</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="14">
         <f t="shared" si="0"/>
         <v>2.3705455692210657</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="23">
         <v>6737</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="24">
         <v>0.253</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="14">
         <f t="shared" si="1"/>
         <v>2.1245663828445287</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="J14" s="23">
+        <v>6716</v>
+      </c>
+      <c r="K14" s="24">
+        <v>0.254</v>
+      </c>
+      <c r="L14" s="14">
+        <f t="shared" si="2"/>
+        <v>2.1179438662882371</v>
+      </c>
+      <c r="M14" s="48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="9">
         <v>2213</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="10">
         <v>1.33</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="23">
         <v>4891</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="24">
         <v>0.60099999999999998</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="14">
         <f t="shared" si="0"/>
         <v>2.2101220063262539</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="23">
         <v>4807</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="24">
         <v>0.61199999999999999</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="14">
         <f t="shared" si="1"/>
         <v>2.1721644826028017</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="J15" s="23">
+        <v>4849</v>
+      </c>
+      <c r="K15" s="24">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="2"/>
+        <v>2.1911432444645276</v>
+      </c>
+      <c r="M15" s="48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="11">
         <v>8915</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="12">
         <v>0.69299999999999995</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="25">
         <v>12625</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="26">
         <v>0.49</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="15">
         <f t="shared" si="0"/>
         <v>1.4161525518788558</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="25">
         <v>13272</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="26">
         <v>0.46600000000000003</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="15">
         <f t="shared" si="1"/>
         <v>1.4887268648345484</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="s">
+      <c r="J16" s="25">
+        <v>12543</v>
+      </c>
+      <c r="K16" s="26">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="L16" s="15">
+        <f t="shared" si="2"/>
+        <v>1.4069545709478408</v>
+      </c>
+      <c r="M16" s="49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="B17" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="41" t="s">
+      <c r="C17" s="42"/>
+      <c r="D17" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="25" t="s">
+      <c r="E17" s="38"/>
+      <c r="F17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="25" t="s">
+      <c r="H17" s="38"/>
+      <c r="I17" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="47">
+      <c r="J17" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="38"/>
+      <c r="L17" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="43">
         <v>0.78810000000000002</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="32">
+      <c r="C18" s="44"/>
+      <c r="D18" s="28">
         <v>0.3337</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="49">
+      <c r="E18" s="29"/>
+      <c r="F18" s="27">
         <f>$B$18/D18</f>
         <v>2.3617021276595747</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="28">
         <v>0.31390000000000001</v>
       </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="49">
+      <c r="H18" s="29"/>
+      <c r="I18" s="27">
         <f>$B$18/G18</f>
         <v>2.5106721885950938</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="28">
+        <v>0.35489999999999999</v>
+      </c>
+      <c r="K18" s="29"/>
+      <c r="L18" s="27">
+        <f>$B$18/J18</f>
+        <v>2.2206255283178362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1445,7 +1713,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1454,7 +1722,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1731,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -1472,7 +1740,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1481,13 +1749,13 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1496,20 +1764,24 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:F4"/>
@@ -1524,6 +1796,18 @@
     <mergeCell ref="D18:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:I16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1535,7 +1819,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:I16">
+  <conditionalFormatting sqref="L7:L16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
add SPEC pattern matching results to overview
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1147B47B-B1C2-3740-B695-74660B4E4247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB69ECE-6C1F-8344-9BCF-5616689A640C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Benchmark</t>
   </si>
@@ -221,6 +221,21 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (b904a345)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>v1.2.2-67</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (b47ad7cf)</t>
     </r>
   </si>
 </sst>
@@ -693,57 +708,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -764,6 +728,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,10 +1093,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2E7EA3-8BF5-F743-9E89-1A0A4F76CDF3}">
-  <dimension ref="A1:M30"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1094,80 +1112,92 @@
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="50"/>
+      <c r="D4" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="32" t="s">
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="32" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="34"/>
-    </row>
-    <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="K4" s="45"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="45"/>
+      <c r="O4" s="46"/>
+    </row>
+    <row r="5" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="35" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="36"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="36"/>
+      <c r="K5" s="48"/>
       <c r="L5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="48"/>
+      <c r="O5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1203,12 +1233,21 @@
       <c r="L6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="46" t="s">
+      <c r="M6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52" t="s">
+    <row r="7" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="7">
@@ -1247,12 +1286,22 @@
         <f>J7/$B7</f>
         <v>3.584122835674616</v>
       </c>
-      <c r="M7" s="47" t="s">
+      <c r="M7" s="21">
+        <v>10939</v>
+      </c>
+      <c r="N7" s="22">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="O7" s="13">
+        <f>M7/$B7</f>
+        <v>3.5736687357072854</v>
+      </c>
+      <c r="P7" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="53" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="9">
@@ -1291,12 +1340,22 @@
         <f t="shared" ref="L8:L16" si="2">J8/$B8</f>
         <v>2.5643067846607668</v>
       </c>
-      <c r="M8" s="48" t="s">
+      <c r="M8" s="23">
+        <v>8686</v>
+      </c>
+      <c r="N8" s="24">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" ref="O8:O16" si="3">M8/$B8</f>
+        <v>2.5622418879056048</v>
+      </c>
+      <c r="P8" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="9">
@@ -1335,12 +1394,22 @@
         <f t="shared" si="2"/>
         <v>1.1181646763042112</v>
       </c>
-      <c r="M9" s="48" t="s">
+      <c r="M9" s="23">
+        <v>3548</v>
+      </c>
+      <c r="N9" s="24">
+        <v>1.33</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="3"/>
+        <v>1.1150219987429291</v>
+      </c>
+      <c r="P9" s="31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="9">
@@ -1379,12 +1448,22 @@
         <f t="shared" si="2"/>
         <v>3.0636645962732918</v>
       </c>
-      <c r="M10" s="48" t="s">
+      <c r="M10" s="23">
+        <v>7991</v>
+      </c>
+      <c r="N10" s="24">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1020962732919255</v>
+      </c>
+      <c r="P10" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="53" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="9">
@@ -1423,12 +1502,22 @@
         <f t="shared" si="2"/>
         <v>2.5207481005260082</v>
       </c>
-      <c r="M11" s="48" t="s">
+      <c r="M11" s="23">
+        <v>4392</v>
+      </c>
+      <c r="N11" s="24">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="3"/>
+        <v>2.5669199298655756</v>
+      </c>
+      <c r="P11" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="9">
@@ -1467,12 +1556,22 @@
         <f t="shared" si="2"/>
         <v>1.3724751797329682</v>
       </c>
-      <c r="M12" s="48" t="s">
+      <c r="M12" s="23">
+        <v>4017</v>
+      </c>
+      <c r="N12" s="24">
+        <v>0.439</v>
+      </c>
+      <c r="O12" s="14">
+        <f t="shared" si="3"/>
+        <v>1.3752139678192399</v>
+      </c>
+      <c r="P12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="53" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="9">
@@ -1511,12 +1610,22 @@
         <f t="shared" si="2"/>
         <v>4.1028873525823508</v>
       </c>
-      <c r="M13" s="48" t="s">
+      <c r="M13" s="23">
+        <v>10104</v>
+      </c>
+      <c r="N13" s="24">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="O13" s="14">
+        <f t="shared" si="3"/>
+        <v>4.1089873932492882</v>
+      </c>
+      <c r="P13" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="53" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="9">
@@ -1555,12 +1664,22 @@
         <f t="shared" si="2"/>
         <v>2.1179438662882371</v>
       </c>
-      <c r="M14" s="48" t="s">
+      <c r="M14" s="23">
+        <v>7568</v>
+      </c>
+      <c r="N14" s="24">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="O14" s="14">
+        <f t="shared" si="3"/>
+        <v>2.3866288237149162</v>
+      </c>
+      <c r="P14" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="9">
@@ -1599,12 +1718,22 @@
         <f t="shared" si="2"/>
         <v>2.1911432444645276</v>
       </c>
-      <c r="M15" s="48" t="s">
+      <c r="M15" s="23">
+        <v>4763</v>
+      </c>
+      <c r="N15" s="24">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="O15" s="14">
+        <f t="shared" si="3"/>
+        <v>2.1522819701762312</v>
+      </c>
+      <c r="P15" s="31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+    <row r="16" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="11">
@@ -1643,68 +1772,93 @@
         <f t="shared" si="2"/>
         <v>1.4069545709478408</v>
       </c>
-      <c r="M16" s="49" t="s">
+      <c r="M16" s="25">
+        <v>14671</v>
+      </c>
+      <c r="N16" s="26">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="O16" s="15">
+        <f t="shared" si="3"/>
+        <v>1.6456533931575996</v>
+      </c>
+      <c r="P16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+    <row r="17" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="B17" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="37" t="s">
+      <c r="C17" s="54"/>
+      <c r="D17" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="38"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="37" t="s">
+      <c r="J17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="38"/>
+      <c r="K17" s="41"/>
       <c r="L17" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43">
+      <c r="M17" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="N17" s="41"/>
+      <c r="O17" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="38">
         <v>0.78810000000000002</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="28">
+      <c r="C18" s="39"/>
+      <c r="D18" s="42">
         <v>0.3337</v>
       </c>
-      <c r="E18" s="29"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="27">
         <f>$B$18/D18</f>
         <v>2.3617021276595747</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="42">
         <v>0.31390000000000001</v>
       </c>
-      <c r="H18" s="29"/>
+      <c r="H18" s="43"/>
       <c r="I18" s="27">
         <f>$B$18/G18</f>
         <v>2.5106721885950938</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="42">
         <v>0.35489999999999999</v>
       </c>
-      <c r="K18" s="29"/>
+      <c r="K18" s="43"/>
       <c r="L18" s="27">
         <f>$B$18/J18</f>
         <v>2.2206255283178362</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" s="42">
+        <v>0.34489999999999998</v>
+      </c>
+      <c r="N18" s="43"/>
+      <c r="O18" s="27">
+        <f>$B$18/M18</f>
+        <v>2.2850101478689475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1713,7 +1867,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1722,7 +1876,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1731,7 +1885,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -1740,7 +1894,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1749,13 +1903,13 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1764,25 +1918,31 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="J4:L4"/>
+  <mergeCells count="20">
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:I4"/>
@@ -1791,11 +1951,21 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J4:L4"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:I16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1807,7 +1977,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:I16">
+  <conditionalFormatting sqref="L7:L16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1819,7 +1989,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:L16">
+  <conditionalFormatting sqref="O7:O16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1832,6 +2002,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add native results to table
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB69ECE-6C1F-8344-9BCF-5616689A640C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E428BC1-AB2C-0C4A-9B04-988C638E81AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Benchmark</t>
   </si>
@@ -237,6 +237,9 @@
       </rPr>
       <t xml:space="preserve"> (b47ad7cf)</t>
     </r>
+  </si>
+  <si>
+    <t>Native</t>
   </si>
 </sst>
 </file>
@@ -728,24 +731,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -754,12 +763,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1096,107 +1099,123 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="12" max="15" width="13.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="14" max="17" width="13.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="49" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="50"/>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="47"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="46"/>
-    </row>
-    <row r="5" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48"/>
+    </row>
+    <row r="5" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="47" t="s">
+      <c r="E5" s="52"/>
+      <c r="F5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="48"/>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="39"/>
+      <c r="H5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="I5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="39"/>
+      <c r="K5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="L5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="48"/>
-      <c r="L5" s="16" t="s">
+      <c r="M5" s="39"/>
+      <c r="N5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="47" t="s">
+      <c r="O5" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="48"/>
-      <c r="O5" s="16" t="s">
+      <c r="P5" s="39"/>
+      <c r="Q5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="R5" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
@@ -1206,754 +1225,838 @@
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="J6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="K6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="M6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="N6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="O6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="P6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="Q6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="29" t="s">
+      <c r="R6" s="29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="7">
+        <v>724</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="D7" s="7">
         <v>3061</v>
       </c>
-      <c r="C7" s="8">
+      <c r="E7" s="8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D7" s="21">
+      <c r="F7" s="21">
         <v>10930</v>
       </c>
-      <c r="E7" s="22">
+      <c r="G7" s="22">
         <v>0.16200000000000001</v>
       </c>
-      <c r="F7" s="13">
-        <f>D7/$B7</f>
+      <c r="H7" s="13">
+        <f>F7/$D7</f>
         <v>3.5707285200914733</v>
       </c>
-      <c r="G7" s="21">
+      <c r="I7" s="21">
         <v>12673</v>
       </c>
-      <c r="H7" s="22">
+      <c r="J7" s="22">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I7" s="13">
-        <f>G7/$B7</f>
+      <c r="K7" s="13">
+        <f>I7/$D7</f>
         <v>4.14015027768703</v>
       </c>
-      <c r="J7" s="21">
+      <c r="L7" s="21">
         <v>10971</v>
       </c>
-      <c r="K7" s="22">
+      <c r="M7" s="22">
         <v>0.16200000000000001</v>
       </c>
-      <c r="L7" s="13">
-        <f>J7/$B7</f>
+      <c r="N7" s="13">
+        <f>L7/$D7</f>
         <v>3.584122835674616</v>
       </c>
-      <c r="M7" s="21">
+      <c r="O7" s="21">
         <v>10939</v>
       </c>
-      <c r="N7" s="22">
+      <c r="P7" s="22">
         <v>0.16200000000000001</v>
       </c>
-      <c r="O7" s="13">
-        <f>M7/$B7</f>
+      <c r="Q7" s="13">
+        <f>O7/$D7</f>
         <v>3.5736687357072854</v>
       </c>
-      <c r="P7" s="30" t="s">
+      <c r="R7" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="9">
+        <v>1002</v>
+      </c>
+      <c r="C8" s="10">
+        <v>3.98</v>
+      </c>
+      <c r="D8" s="9">
         <v>3390</v>
       </c>
-      <c r="C8" s="10">
+      <c r="E8" s="10">
         <v>1.17</v>
       </c>
-      <c r="D8" s="23">
+      <c r="F8" s="23">
         <v>9301</v>
       </c>
-      <c r="E8" s="24">
+      <c r="G8" s="24">
         <v>0.42799999999999999</v>
       </c>
-      <c r="F8" s="14">
-        <f t="shared" ref="F8:F16" si="0">D8/$B8</f>
+      <c r="H8" s="14">
+        <f t="shared" ref="H8:H16" si="0">F8/$D8</f>
         <v>2.7436578171091446</v>
       </c>
-      <c r="G8" s="23">
+      <c r="I8" s="23">
         <v>10375</v>
       </c>
-      <c r="H8" s="24">
+      <c r="J8" s="24">
         <v>0.38400000000000001</v>
       </c>
-      <c r="I8" s="14">
-        <f t="shared" ref="I8:I16" si="1">G8/$B8</f>
+      <c r="K8" s="14">
+        <f t="shared" ref="K8:K16" si="1">I8/$D8</f>
         <v>3.0604719764011801</v>
       </c>
-      <c r="J8" s="23">
+      <c r="L8" s="23">
         <v>8693</v>
       </c>
-      <c r="K8" s="24">
+      <c r="M8" s="24">
         <v>0.45800000000000002</v>
       </c>
-      <c r="L8" s="14">
-        <f t="shared" ref="L8:L16" si="2">J8/$B8</f>
+      <c r="N8" s="14">
+        <f t="shared" ref="N8:N16" si="2">L8/$D8</f>
         <v>2.5643067846607668</v>
       </c>
-      <c r="M8" s="23">
+      <c r="O8" s="23">
         <v>8686</v>
       </c>
-      <c r="N8" s="24">
+      <c r="P8" s="24">
         <v>0.45800000000000002</v>
       </c>
-      <c r="O8" s="14">
-        <f t="shared" ref="O8:O16" si="3">M8/$B8</f>
+      <c r="Q8" s="14">
+        <f t="shared" ref="Q8:Q16" si="3">O8/$D8</f>
         <v>2.5622418879056048</v>
       </c>
-      <c r="P8" s="31" t="s">
+      <c r="R8" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="9">
+        <v>1406</v>
+      </c>
+      <c r="C9" s="10">
+        <v>3.36</v>
+      </c>
+      <c r="D9" s="9">
         <v>3182</v>
       </c>
-      <c r="C9" s="10">
+      <c r="E9" s="10">
         <v>1.48</v>
       </c>
-      <c r="D9" s="23">
+      <c r="F9" s="23">
         <v>3654</v>
       </c>
-      <c r="E9" s="24">
+      <c r="G9" s="24">
         <v>1.29</v>
       </c>
-      <c r="F9" s="14">
+      <c r="H9" s="14">
         <f t="shared" si="0"/>
         <v>1.1483343808925204</v>
       </c>
-      <c r="G9" s="23">
+      <c r="I9" s="23">
         <v>4774</v>
       </c>
-      <c r="H9" s="24">
+      <c r="J9" s="24">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I9" s="14">
+      <c r="K9" s="14">
         <f t="shared" si="1"/>
         <v>1.5003142677561283</v>
       </c>
-      <c r="J9" s="23">
+      <c r="L9" s="23">
         <v>3558</v>
       </c>
-      <c r="K9" s="24">
+      <c r="M9" s="24">
         <v>1.33</v>
       </c>
-      <c r="L9" s="14">
+      <c r="N9" s="14">
         <f t="shared" si="2"/>
         <v>1.1181646763042112</v>
       </c>
-      <c r="M9" s="23">
+      <c r="O9" s="23">
         <v>3548</v>
       </c>
-      <c r="N9" s="24">
+      <c r="P9" s="24">
         <v>1.33</v>
       </c>
-      <c r="O9" s="14">
+      <c r="Q9" s="14">
         <f t="shared" si="3"/>
         <v>1.1150219987429291</v>
       </c>
-      <c r="P9" s="31" t="s">
+      <c r="R9" s="31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="9">
+        <v>886</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1.84</v>
+      </c>
+      <c r="D10" s="9">
         <v>2576</v>
       </c>
-      <c r="C10" s="10">
+      <c r="E10" s="10">
         <v>0.63300000000000001</v>
       </c>
-      <c r="D10" s="23">
+      <c r="F10" s="23">
         <v>8210</v>
       </c>
-      <c r="E10" s="24">
+      <c r="G10" s="24">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F10" s="14">
+      <c r="H10" s="14">
         <f t="shared" si="0"/>
         <v>3.1871118012422359</v>
       </c>
-      <c r="G10" s="23">
+      <c r="I10" s="23">
         <v>10257</v>
       </c>
-      <c r="H10" s="24">
+      <c r="J10" s="24">
         <v>0.159</v>
       </c>
-      <c r="I10" s="14">
+      <c r="K10" s="14">
         <f t="shared" si="1"/>
         <v>3.9817546583850931</v>
       </c>
-      <c r="J10" s="23">
+      <c r="L10" s="23">
         <v>7892</v>
       </c>
-      <c r="K10" s="24">
+      <c r="M10" s="24">
         <v>0.20699999999999999</v>
       </c>
-      <c r="L10" s="14">
+      <c r="N10" s="14">
         <f t="shared" si="2"/>
         <v>3.0636645962732918</v>
       </c>
-      <c r="M10" s="23">
+      <c r="O10" s="23">
         <v>7991</v>
       </c>
-      <c r="N10" s="24">
+      <c r="P10" s="24">
         <v>0.20399999999999999</v>
       </c>
-      <c r="O10" s="14">
+      <c r="Q10" s="14">
         <f t="shared" si="3"/>
         <v>3.1020962732919255</v>
       </c>
-      <c r="P10" s="31" t="s">
+      <c r="R10" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="9">
+        <v>627</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="D11" s="9">
         <v>1711</v>
       </c>
-      <c r="C11" s="10">
+      <c r="E11" s="10">
         <v>0.82799999999999996</v>
       </c>
-      <c r="D11" s="23">
+      <c r="F11" s="23">
         <v>4563</v>
       </c>
-      <c r="E11" s="24">
+      <c r="G11" s="24">
         <v>0.311</v>
       </c>
-      <c r="F11" s="14">
+      <c r="H11" s="14">
         <f t="shared" si="0"/>
         <v>2.6668614845119811</v>
       </c>
-      <c r="G11" s="23">
+      <c r="I11" s="23">
         <v>5285</v>
       </c>
-      <c r="H11" s="24">
+      <c r="J11" s="24">
         <v>0.26800000000000002</v>
       </c>
-      <c r="I11" s="14">
+      <c r="K11" s="14">
         <f t="shared" si="1"/>
         <v>3.0888369374634714</v>
       </c>
-      <c r="J11" s="23">
+      <c r="L11" s="23">
         <v>4313</v>
       </c>
-      <c r="K11" s="24">
+      <c r="M11" s="24">
         <v>0.32900000000000001</v>
       </c>
-      <c r="L11" s="14">
+      <c r="N11" s="14">
         <f t="shared" si="2"/>
         <v>2.5207481005260082</v>
       </c>
-      <c r="M11" s="23">
+      <c r="O11" s="23">
         <v>4392</v>
       </c>
-      <c r="N11" s="24">
+      <c r="P11" s="24">
         <v>0.32300000000000001</v>
       </c>
-      <c r="O11" s="14">
+      <c r="Q11" s="14">
         <f t="shared" si="3"/>
         <v>2.5669199298655756</v>
       </c>
-      <c r="P11" s="31" t="s">
+      <c r="R11" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="9">
+        <v>1080</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1.63</v>
+      </c>
+      <c r="D12" s="9">
         <v>2921</v>
       </c>
-      <c r="C12" s="10">
+      <c r="E12" s="10">
         <v>0.60399999999999998</v>
       </c>
-      <c r="D12" s="23">
+      <c r="F12" s="23">
         <v>4333</v>
       </c>
-      <c r="E12" s="24">
+      <c r="G12" s="24">
         <v>0.40699999999999997</v>
       </c>
-      <c r="F12" s="14">
+      <c r="H12" s="14">
         <f t="shared" si="0"/>
         <v>1.4833960972269771</v>
       </c>
-      <c r="G12" s="23">
+      <c r="I12" s="23">
         <v>4305</v>
       </c>
-      <c r="H12" s="24">
+      <c r="J12" s="24">
         <v>0.41</v>
       </c>
-      <c r="I12" s="14">
+      <c r="K12" s="14">
         <f t="shared" si="1"/>
         <v>1.4738103389250257</v>
       </c>
-      <c r="J12" s="23">
+      <c r="L12" s="23">
         <v>4009</v>
       </c>
-      <c r="K12" s="24">
+      <c r="M12" s="24">
         <v>0.44</v>
       </c>
-      <c r="L12" s="14">
+      <c r="N12" s="14">
         <f t="shared" si="2"/>
         <v>1.3724751797329682</v>
       </c>
-      <c r="M12" s="23">
+      <c r="O12" s="23">
         <v>4017</v>
       </c>
-      <c r="N12" s="24">
+      <c r="P12" s="24">
         <v>0.439</v>
       </c>
-      <c r="O12" s="14">
+      <c r="Q12" s="14">
         <f t="shared" si="3"/>
         <v>1.3752139678192399</v>
       </c>
-      <c r="P12" s="31" t="s">
+      <c r="R12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="9">
+        <v>770</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1.86</v>
+      </c>
+      <c r="D13" s="9">
         <v>2459</v>
       </c>
-      <c r="C13" s="10">
+      <c r="E13" s="10">
         <v>0.58299999999999996</v>
       </c>
-      <c r="D13" s="23">
+      <c r="F13" s="23">
         <v>10330</v>
       </c>
-      <c r="E13" s="24">
+      <c r="G13" s="24">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F13" s="14">
+      <c r="H13" s="14">
         <f t="shared" si="0"/>
         <v>4.2008946726311507</v>
       </c>
-      <c r="G13" s="23">
+      <c r="I13" s="23">
         <v>10327</v>
       </c>
-      <c r="H13" s="24">
+      <c r="J13" s="24">
         <v>0.13900000000000001</v>
       </c>
-      <c r="I13" s="14">
+      <c r="K13" s="14">
         <f t="shared" si="1"/>
         <v>4.1996746644977634</v>
       </c>
-      <c r="J13" s="23">
+      <c r="L13" s="23">
         <v>10089</v>
       </c>
-      <c r="K13" s="24">
+      <c r="M13" s="24">
         <v>0.14199999999999999</v>
       </c>
-      <c r="L13" s="14">
+      <c r="N13" s="14">
         <f t="shared" si="2"/>
         <v>4.1028873525823508</v>
       </c>
-      <c r="M13" s="23">
+      <c r="O13" s="23">
         <v>10104</v>
       </c>
-      <c r="N13" s="24">
+      <c r="P13" s="24">
         <v>0.14199999999999999</v>
       </c>
-      <c r="O13" s="14">
+      <c r="Q13" s="14">
         <f t="shared" si="3"/>
         <v>4.1089873932492882</v>
       </c>
-      <c r="P13" s="31" t="s">
+      <c r="R13" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="9">
+        <v>1362</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="D14" s="9">
         <v>3171</v>
       </c>
-      <c r="C14" s="10">
+      <c r="E14" s="10">
         <v>0.53800000000000003</v>
       </c>
-      <c r="D14" s="23">
+      <c r="F14" s="23">
         <v>7517</v>
       </c>
-      <c r="E14" s="24">
+      <c r="G14" s="24">
         <v>0.22700000000000001</v>
       </c>
-      <c r="F14" s="14">
+      <c r="H14" s="14">
         <f t="shared" si="0"/>
         <v>2.3705455692210657</v>
       </c>
-      <c r="G14" s="23">
+      <c r="I14" s="23">
         <v>6737</v>
       </c>
-      <c r="H14" s="24">
+      <c r="J14" s="24">
         <v>0.253</v>
       </c>
-      <c r="I14" s="14">
+      <c r="K14" s="14">
         <f t="shared" si="1"/>
         <v>2.1245663828445287</v>
       </c>
-      <c r="J14" s="23">
+      <c r="L14" s="23">
         <v>6716</v>
       </c>
-      <c r="K14" s="24">
+      <c r="M14" s="24">
         <v>0.254</v>
       </c>
-      <c r="L14" s="14">
+      <c r="N14" s="14">
         <f t="shared" si="2"/>
         <v>2.1179438662882371</v>
       </c>
-      <c r="M14" s="23">
+      <c r="O14" s="23">
         <v>7568</v>
       </c>
-      <c r="N14" s="24">
+      <c r="P14" s="24">
         <v>0.22500000000000001</v>
       </c>
-      <c r="O14" s="14">
+      <c r="Q14" s="14">
         <f t="shared" si="3"/>
         <v>2.3866288237149162</v>
       </c>
-      <c r="P14" s="31" t="s">
+      <c r="R14" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="9">
+        <v>624</v>
+      </c>
+      <c r="C15" s="10">
+        <v>4.71</v>
+      </c>
+      <c r="D15" s="9">
         <v>2213</v>
       </c>
-      <c r="C15" s="10">
+      <c r="E15" s="10">
         <v>1.33</v>
       </c>
-      <c r="D15" s="23">
+      <c r="F15" s="23">
         <v>4891</v>
       </c>
-      <c r="E15" s="24">
+      <c r="G15" s="24">
         <v>0.60099999999999998</v>
       </c>
-      <c r="F15" s="14">
+      <c r="H15" s="14">
         <f t="shared" si="0"/>
         <v>2.2101220063262539</v>
       </c>
-      <c r="G15" s="23">
+      <c r="I15" s="23">
         <v>4807</v>
       </c>
-      <c r="H15" s="24">
+      <c r="J15" s="24">
         <v>0.61199999999999999</v>
       </c>
-      <c r="I15" s="14">
+      <c r="K15" s="14">
         <f t="shared" si="1"/>
         <v>2.1721644826028017</v>
       </c>
-      <c r="J15" s="23">
+      <c r="L15" s="23">
         <v>4849</v>
       </c>
-      <c r="K15" s="24">
+      <c r="M15" s="24">
         <v>0.60599999999999998</v>
       </c>
-      <c r="L15" s="14">
+      <c r="N15" s="14">
         <f t="shared" si="2"/>
         <v>2.1911432444645276</v>
       </c>
-      <c r="M15" s="23">
+      <c r="O15" s="23">
         <v>4763</v>
       </c>
-      <c r="N15" s="24">
+      <c r="P15" s="24">
         <v>0.61699999999999999</v>
       </c>
-      <c r="O15" s="14">
+      <c r="Q15" s="14">
         <f t="shared" si="3"/>
         <v>2.1522819701762312</v>
       </c>
-      <c r="P15" s="31" t="s">
+      <c r="R15" s="31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="11">
+        <v>4681</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1.32</v>
+      </c>
+      <c r="D16" s="11">
         <v>8915</v>
       </c>
-      <c r="C16" s="12">
+      <c r="E16" s="12">
         <v>0.69299999999999995</v>
       </c>
-      <c r="D16" s="25">
+      <c r="F16" s="25">
         <v>12625</v>
       </c>
-      <c r="E16" s="26">
+      <c r="G16" s="26">
         <v>0.49</v>
       </c>
-      <c r="F16" s="15">
+      <c r="H16" s="15">
         <f t="shared" si="0"/>
         <v>1.4161525518788558</v>
       </c>
-      <c r="G16" s="25">
+      <c r="I16" s="25">
         <v>13272</v>
       </c>
-      <c r="H16" s="26">
+      <c r="J16" s="26">
         <v>0.46600000000000003</v>
       </c>
-      <c r="I16" s="15">
+      <c r="K16" s="15">
         <f t="shared" si="1"/>
         <v>1.4887268648345484</v>
       </c>
-      <c r="J16" s="25">
+      <c r="L16" s="25">
         <v>12543</v>
       </c>
-      <c r="K16" s="26">
+      <c r="M16" s="26">
         <v>0.49299999999999999</v>
       </c>
-      <c r="L16" s="15">
+      <c r="N16" s="15">
         <f t="shared" si="2"/>
         <v>1.4069545709478408</v>
       </c>
-      <c r="M16" s="25">
+      <c r="O16" s="25">
         <v>14671</v>
       </c>
-      <c r="N16" s="26">
+      <c r="P16" s="26">
         <v>0.42099999999999999</v>
       </c>
-      <c r="O16" s="15">
+      <c r="Q16" s="15">
         <f t="shared" si="3"/>
         <v>1.6456533931575996</v>
       </c>
-      <c r="P16" s="32" t="s">
+      <c r="R16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="B17" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="54"/>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="54"/>
+      <c r="F17" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="20" t="s">
+      <c r="G17" s="41"/>
+      <c r="H17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="40" t="s">
+      <c r="I17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="20" t="s">
+      <c r="J17" s="41"/>
+      <c r="K17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="L17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="41"/>
-      <c r="L17" s="20" t="s">
+      <c r="M17" s="41"/>
+      <c r="N17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="40" t="s">
+      <c r="O17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="20" t="s">
+      <c r="P17" s="41"/>
+      <c r="Q17" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="38">
+    <row r="18" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="44">
         <v>0.78810000000000002</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="42">
+      <c r="E18" s="45"/>
+      <c r="F18" s="42">
         <v>0.3337</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="27">
-        <f>$B$18/D18</f>
+      <c r="G18" s="43"/>
+      <c r="H18" s="27">
+        <f>$D$18/F18</f>
         <v>2.3617021276595747</v>
       </c>
-      <c r="G18" s="42">
+      <c r="I18" s="42">
         <v>0.31390000000000001</v>
       </c>
-      <c r="H18" s="43"/>
-      <c r="I18" s="27">
-        <f>$B$18/G18</f>
+      <c r="J18" s="43"/>
+      <c r="K18" s="27">
+        <f>$D$18/I18</f>
         <v>2.5106721885950938</v>
       </c>
-      <c r="J18" s="42">
+      <c r="L18" s="42">
         <v>0.35489999999999999</v>
       </c>
-      <c r="K18" s="43"/>
-      <c r="L18" s="27">
-        <f>$B$18/J18</f>
+      <c r="M18" s="43"/>
+      <c r="N18" s="27">
+        <f>$D$18/L18</f>
         <v>2.2206255283178362</v>
       </c>
-      <c r="M18" s="42">
+      <c r="O18" s="42">
         <v>0.34489999999999998</v>
       </c>
-      <c r="N18" s="43"/>
-      <c r="O18" s="27">
-        <f>$B$18/M18</f>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="27">
+        <f>$D$18/O18</f>
         <v>2.2850101478689475</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C24" s="3"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G30" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="G18:H18"/>
+  <mergeCells count="24">
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="D17:E17"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="I18:J18"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
   </mergeCells>
-  <conditionalFormatting sqref="F7:F16">
+  <conditionalFormatting sqref="H7:H16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1965,7 +2068,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:I16">
+  <conditionalFormatting sqref="K7:K16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1977,7 +2080,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:L16">
+  <conditionalFormatting sqref="N7:N16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1989,7 +2092,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O7:O16">
+  <conditionalFormatting sqref="Q7:Q16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2002,6 +2105,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add results to overview
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E428BC1-AB2C-0C4A-9B04-988C638E81AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E64066-F541-3B4B-8229-E85724D995FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="127, 128" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>Benchmark</t>
   </si>
@@ -240,6 +241,21 @@
   </si>
   <si>
     <t>Native</t>
+  </si>
+  <si>
+    <r>
+      <t>v1.2.2-78</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (0390bce3)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -731,50 +747,50 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1099,10 +1115,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:C17"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1112,110 +1128,125 @@
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" customWidth="1"/>
-    <col min="14" max="17" width="13.33203125" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="18" max="20" width="13.33203125" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="49" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="46" t="s">
+      <c r="E4" s="52"/>
+      <c r="F4" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="46" t="s">
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="46" t="s">
+      <c r="J4" s="45"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="47"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="46" t="s">
+      <c r="M4" s="45"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="48"/>
-    </row>
-    <row r="5" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="45"/>
+      <c r="T4" s="46"/>
+    </row>
+    <row r="5" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="51" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="38" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="39"/>
+      <c r="J5" s="48"/>
       <c r="K5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="39"/>
+      <c r="M5" s="48"/>
       <c r="N5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="39"/>
+      <c r="P5" s="48"/>
       <c r="Q5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="28" t="s">
+      <c r="R5" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="48"/>
+      <c r="T5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
@@ -1267,11 +1298,20 @@
       <c r="Q6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="29" t="s">
+      <c r="R6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" s="29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>3</v>
       </c>
@@ -1327,11 +1367,21 @@
         <f>O7/$D7</f>
         <v>3.5736687357072854</v>
       </c>
-      <c r="R7" s="30" t="s">
+      <c r="R7" s="21">
+        <v>2222</v>
+      </c>
+      <c r="S7" s="22">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="T7" s="13">
+        <f>R7/$D7</f>
+        <v>0.72590656648154195</v>
+      </c>
+      <c r="U7" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
@@ -1387,11 +1437,21 @@
         <f t="shared" ref="Q8:Q16" si="3">O8/$D8</f>
         <v>2.5622418879056048</v>
       </c>
-      <c r="R8" s="31" t="s">
+      <c r="R8" s="23">
+        <v>1956</v>
+      </c>
+      <c r="S8" s="24">
+        <v>2.04</v>
+      </c>
+      <c r="T8" s="14">
+        <f t="shared" ref="T8:T16" si="4">R8/$D8</f>
+        <v>0.57699115044247784</v>
+      </c>
+      <c r="U8" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
@@ -1447,11 +1507,21 @@
         <f t="shared" si="3"/>
         <v>1.1150219987429291</v>
       </c>
-      <c r="R9" s="31" t="s">
+      <c r="R9" s="23">
+        <v>2695</v>
+      </c>
+      <c r="S9" s="24">
+        <v>1.75</v>
+      </c>
+      <c r="T9" s="14">
+        <f t="shared" si="4"/>
+        <v>0.84695160276555626</v>
+      </c>
+      <c r="U9" s="31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
@@ -1507,11 +1577,21 @@
         <f t="shared" si="3"/>
         <v>3.1020962732919255</v>
       </c>
-      <c r="R10" s="31" t="s">
+      <c r="R10" s="23">
+        <v>1768</v>
+      </c>
+      <c r="S10" s="24">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="T10" s="14">
+        <f t="shared" si="4"/>
+        <v>0.68633540372670809</v>
+      </c>
+      <c r="U10" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -1567,11 +1647,21 @@
         <f t="shared" si="3"/>
         <v>2.5669199298655756</v>
       </c>
-      <c r="R11" s="31" t="s">
+      <c r="R11" s="23">
+        <v>1178</v>
+      </c>
+      <c r="S11" s="24">
+        <v>1.2</v>
+      </c>
+      <c r="T11" s="14">
+        <f t="shared" si="4"/>
+        <v>0.68848626534190527</v>
+      </c>
+      <c r="U11" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
@@ -1627,11 +1717,21 @@
         <f t="shared" si="3"/>
         <v>1.3752139678192399</v>
       </c>
-      <c r="R12" s="31" t="s">
+      <c r="R12" s="23">
+        <v>2590</v>
+      </c>
+      <c r="S12" s="24">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="T12" s="14">
+        <f t="shared" si="4"/>
+        <v>0.88668264293050325</v>
+      </c>
+      <c r="U12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
@@ -1687,11 +1787,21 @@
         <f t="shared" si="3"/>
         <v>4.1089873932492882</v>
       </c>
-      <c r="R13" s="31" t="s">
+      <c r="R13" s="23">
+        <v>1603</v>
+      </c>
+      <c r="S13" s="24">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="T13" s="14">
+        <f t="shared" si="4"/>
+        <v>0.65189101260675075</v>
+      </c>
+      <c r="U13" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
@@ -1747,11 +1857,21 @@
         <f t="shared" si="3"/>
         <v>2.3866288237149162</v>
       </c>
-      <c r="R14" s="31" t="s">
+      <c r="R14" s="23">
+        <v>2080</v>
+      </c>
+      <c r="S14" s="24">
+        <v>0.82</v>
+      </c>
+      <c r="T14" s="14">
+        <f t="shared" si="4"/>
+        <v>0.65594449700409962</v>
+      </c>
+      <c r="U14" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
@@ -1807,11 +1927,21 @@
         <f t="shared" si="3"/>
         <v>2.1522819701762312</v>
       </c>
-      <c r="R15" s="31" t="s">
+      <c r="R15" s="23">
+        <v>1575</v>
+      </c>
+      <c r="S15" s="24">
+        <v>1.87</v>
+      </c>
+      <c r="T15" s="14">
+        <f t="shared" si="4"/>
+        <v>0.71170356981473115</v>
+      </c>
+      <c r="U15" s="31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
@@ -1867,11 +1997,21 @@
         <f t="shared" si="3"/>
         <v>1.6456533931575996</v>
       </c>
-      <c r="R16" s="32" t="s">
+      <c r="R16" s="25">
+        <v>11083</v>
+      </c>
+      <c r="S16" s="26">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="T16" s="15">
+        <f t="shared" si="4"/>
+        <v>1.2431856421761076</v>
+      </c>
+      <c r="U16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="19" x14ac:dyDescent="0.25">
       <c r="B17" s="53" t="s">
         <v>15</v>
       </c>
@@ -1908,16 +2048,23 @@
       <c r="Q17" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="44">
+      <c r="R17" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="S17" s="41"/>
+      <c r="T17" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="38">
         <v>2.2400000000000002</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="44">
+      <c r="C18" s="39"/>
+      <c r="D18" s="38">
         <v>0.78810000000000002</v>
       </c>
-      <c r="E18" s="45"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="42">
         <v>0.3337</v>
       </c>
@@ -1950,8 +2097,16 @@
         <f>$D$18/O18</f>
         <v>2.2850101478689475</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18" s="42">
+        <v>1.05</v>
+      </c>
+      <c r="S18" s="43"/>
+      <c r="T18" s="27">
+        <f>$D$18/R18</f>
+        <v>0.75057142857142856</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1961,7 +2116,7 @@
       <c r="C20" s="3"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1971,7 +2126,7 @@
       <c r="C21" s="3"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1981,7 +2136,7 @@
       <c r="C22" s="3"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -1991,7 +2146,7 @@
       <c r="C23" s="3"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2001,13 +2156,13 @@
       <c r="C24" s="3"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -2017,20 +2172,20 @@
       <c r="C26" s="3"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="I30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="28">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B4:C4"/>
@@ -2047,16 +2202,32 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R18:S18"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="I18:J18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
   </mergeCells>
   <conditionalFormatting sqref="H7:H16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7:K16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2068,7 +2239,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:K16">
+  <conditionalFormatting sqref="N7:N16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2080,7 +2251,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N7:N16">
+  <conditionalFormatting sqref="Q7:Q16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2092,7 +2263,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q7:Q16">
+  <conditionalFormatting sqref="T7:T16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2105,6 +2276,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update native results for use in graphics
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E64066-F541-3B4B-8229-E85724D995FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCBC3B5-434C-0D4B-8F6C-5F24DDF59065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="127, 128" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -747,12 +746,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -763,39 +795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1118,7 +1117,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,84 +1160,84 @@
     </row>
     <row r="4" spans="1:21" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="51" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="44" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="44" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="44" t="s">
+      <c r="J4" s="47"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="45"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="44" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="44" t="s">
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="45"/>
-      <c r="T4" s="46"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="48"/>
     </row>
     <row r="5" spans="1:21" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="49" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="47" t="s">
+      <c r="E5" s="39"/>
+      <c r="F5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="48"/>
+      <c r="G5" s="50"/>
       <c r="H5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="48"/>
+      <c r="J5" s="50"/>
       <c r="K5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="47" t="s">
+      <c r="L5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="48"/>
+      <c r="M5" s="50"/>
       <c r="N5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="47" t="s">
+      <c r="O5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="48"/>
+      <c r="P5" s="50"/>
       <c r="Q5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="47" t="s">
+      <c r="R5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="48"/>
+      <c r="S5" s="50"/>
       <c r="T5" s="16" t="s">
         <v>16</v>
       </c>
@@ -1316,10 +1315,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="7">
-        <v>724</v>
+        <v>654</v>
       </c>
       <c r="C7" s="8">
-        <v>2.4500000000000002</v>
+        <v>2.71</v>
       </c>
       <c r="D7" s="7">
         <v>3061</v>
@@ -1386,10 +1385,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="9">
-        <v>1002</v>
+        <v>953</v>
       </c>
       <c r="C8" s="10">
-        <v>3.98</v>
+        <v>4.18</v>
       </c>
       <c r="D8" s="9">
         <v>3390</v>
@@ -1456,10 +1455,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="9">
-        <v>1406</v>
+        <v>1409</v>
       </c>
       <c r="C9" s="10">
-        <v>3.36</v>
+        <v>3.35</v>
       </c>
       <c r="D9" s="9">
         <v>3182</v>
@@ -1526,10 +1525,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="9">
-        <v>886</v>
+        <v>779</v>
       </c>
       <c r="C10" s="10">
-        <v>1.84</v>
+        <v>2.09</v>
       </c>
       <c r="D10" s="9">
         <v>2576</v>
@@ -1596,10 +1595,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="9">
-        <v>627</v>
+        <v>533</v>
       </c>
       <c r="C11" s="10">
-        <v>2.2599999999999998</v>
+        <v>2.66</v>
       </c>
       <c r="D11" s="9">
         <v>1711</v>
@@ -1666,10 +1665,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="9">
-        <v>1080</v>
+        <v>554</v>
       </c>
       <c r="C12" s="10">
-        <v>1.63</v>
+        <v>3.19</v>
       </c>
       <c r="D12" s="9">
         <v>2921</v>
@@ -1736,10 +1735,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="9">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="C13" s="10">
-        <v>1.86</v>
+        <v>1.85</v>
       </c>
       <c r="D13" s="9">
         <v>2459</v>
@@ -1806,10 +1805,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="9">
-        <v>1362</v>
+        <v>1045</v>
       </c>
       <c r="C14" s="10">
-        <v>1.25</v>
+        <v>1.63</v>
       </c>
       <c r="D14" s="9">
         <v>3171</v>
@@ -1876,10 +1875,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="9">
-        <v>624</v>
+        <v>780</v>
       </c>
       <c r="C15" s="10">
-        <v>4.71</v>
+        <v>3.77</v>
       </c>
       <c r="D15" s="9">
         <v>2213</v>
@@ -1946,10 +1945,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="11">
-        <v>4681</v>
+        <v>4665</v>
       </c>
       <c r="C16" s="12">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
       <c r="D16" s="11">
         <v>8915</v>
@@ -2012,95 +2011,95 @@
       </c>
     </row>
     <row r="17" spans="1:20" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="53" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="54"/>
-      <c r="F17" s="40" t="s">
+      <c r="E17" s="45"/>
+      <c r="F17" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="41"/>
+      <c r="G17" s="52"/>
       <c r="H17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="41"/>
+      <c r="J17" s="52"/>
       <c r="K17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="40" t="s">
+      <c r="L17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="41"/>
+      <c r="M17" s="52"/>
       <c r="N17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="40" t="s">
+      <c r="O17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="P17" s="41"/>
+      <c r="P17" s="52"/>
       <c r="Q17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="R17" s="40" t="s">
+      <c r="R17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="S17" s="41"/>
+      <c r="S17" s="52"/>
       <c r="T17" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="38">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="38">
+      <c r="B18" s="40">
+        <v>2.52</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="40">
         <v>0.78810000000000002</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="42">
+      <c r="E18" s="41"/>
+      <c r="F18" s="53">
         <v>0.3337</v>
       </c>
-      <c r="G18" s="43"/>
+      <c r="G18" s="54"/>
       <c r="H18" s="27">
         <f>$D$18/F18</f>
         <v>2.3617021276595747</v>
       </c>
-      <c r="I18" s="42">
+      <c r="I18" s="53">
         <v>0.31390000000000001</v>
       </c>
-      <c r="J18" s="43"/>
+      <c r="J18" s="54"/>
       <c r="K18" s="27">
         <f>$D$18/I18</f>
         <v>2.5106721885950938</v>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="53">
         <v>0.35489999999999999</v>
       </c>
-      <c r="M18" s="43"/>
+      <c r="M18" s="54"/>
       <c r="N18" s="27">
         <f>$D$18/L18</f>
         <v>2.2206255283178362</v>
       </c>
-      <c r="O18" s="42">
+      <c r="O18" s="53">
         <v>0.34489999999999998</v>
       </c>
-      <c r="P18" s="43"/>
+      <c r="P18" s="54"/>
       <c r="Q18" s="27">
         <f>$D$18/O18</f>
         <v>2.2850101478689475</v>
       </c>
-      <c r="R18" s="42">
+      <c r="R18" s="53">
         <v>1.05</v>
       </c>
-      <c r="S18" s="43"/>
+      <c r="S18" s="54"/>
       <c r="T18" s="27">
         <f>$D$18/R18</f>
         <v>0.75057142857142856</v>
@@ -2186,6 +2185,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="I18:J18"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B4:C4"/>
@@ -2202,18 +2213,6 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="I18:J18"/>
   </mergeCells>
   <conditionalFormatting sqref="H7:H16">
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
update QEMU run with new settings
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCBC3B5-434C-0D4B-8F6C-5F24DDF59065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAF989B-E8FD-F549-9F90-836464AA55D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
   <si>
     <t>Benchmark</t>
   </si>
@@ -255,6 +255,9 @@
       </rPr>
       <t xml:space="preserve"> (0390bce3)</t>
     </r>
+  </si>
+  <si>
+    <t>rv8</t>
   </si>
 </sst>
 </file>
@@ -746,28 +749,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1114,10 +1117,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:C17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,127 +1128,142 @@
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="8.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="17" width="13.33203125" hidden="1" customWidth="1"/>
-    <col min="18" max="20" width="13.33203125" customWidth="1"/>
-    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="19" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="20" max="22" width="13.33203125" customWidth="1"/>
+    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:21" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:23" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:23" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="46" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="47"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="47"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="47"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="46" t="s">
+      <c r="R4" s="47"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="47"/>
-      <c r="T4" s="48"/>
-    </row>
-    <row r="5" spans="1:21" ht="19" x14ac:dyDescent="0.25">
+      <c r="U4" s="47"/>
+      <c r="V4" s="48"/>
+    </row>
+    <row r="5" spans="1:23" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="41"/>
+      <c r="F5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="49" t="s">
+      <c r="G5" s="41"/>
+      <c r="H5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="16" t="s">
+      <c r="I5" s="50"/>
+      <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="49" t="s">
+      <c r="K5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="16" t="s">
+      <c r="L5" s="50"/>
+      <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="N5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="50"/>
-      <c r="N5" s="16" t="s">
+      <c r="O5" s="50"/>
+      <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="49" t="s">
+      <c r="Q5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="16" t="s">
+      <c r="R5" s="50"/>
+      <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="49" t="s">
+      <c r="T5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="50"/>
-      <c r="T5" s="16" t="s">
+      <c r="U5" s="50"/>
+      <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="U5" s="28" t="s">
+      <c r="W5" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
@@ -1261,56 +1279,62 @@
       <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="L6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="M6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="N6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="O6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="P6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="Q6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="R6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="S6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="17" t="s">
+      <c r="T6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="U6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="V6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="U6" s="29" t="s">
+      <c r="W6" s="29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>3</v>
       </c>
@@ -1320,67 +1344,69 @@
       <c r="C7" s="8">
         <v>2.71</v>
       </c>
-      <c r="D7" s="7">
-        <v>3061</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7">
+        <v>3090</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="H7" s="21">
         <v>10930</v>
       </c>
-      <c r="G7" s="22">
+      <c r="I7" s="22">
         <v>0.16200000000000001</v>
       </c>
-      <c r="H7" s="13">
-        <f>F7/$D7</f>
-        <v>3.5707285200914733</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="J7" s="13">
+        <f>H7/$F7</f>
+        <v>3.5372168284789645</v>
+      </c>
+      <c r="K7" s="21">
         <v>12673</v>
       </c>
-      <c r="J7" s="22">
+      <c r="L7" s="22">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K7" s="13">
-        <f>I7/$D7</f>
-        <v>4.14015027768703</v>
-      </c>
-      <c r="L7" s="21">
+      <c r="M7" s="13">
+        <f>K7/$F7</f>
+        <v>4.1012944983818773</v>
+      </c>
+      <c r="N7" s="21">
         <v>10971</v>
       </c>
-      <c r="M7" s="22">
+      <c r="O7" s="22">
         <v>0.16200000000000001</v>
       </c>
-      <c r="N7" s="13">
-        <f>L7/$D7</f>
-        <v>3.584122835674616</v>
-      </c>
-      <c r="O7" s="21">
+      <c r="P7" s="13">
+        <f>N7/$F7</f>
+        <v>3.5504854368932039</v>
+      </c>
+      <c r="Q7" s="21">
         <v>10939</v>
       </c>
-      <c r="P7" s="22">
+      <c r="R7" s="22">
         <v>0.16200000000000001</v>
       </c>
-      <c r="Q7" s="13">
-        <f>O7/$D7</f>
-        <v>3.5736687357072854</v>
-      </c>
-      <c r="R7" s="21">
+      <c r="S7" s="13">
+        <f>Q7/$F7</f>
+        <v>3.5401294498381879</v>
+      </c>
+      <c r="T7" s="21">
         <v>2222</v>
       </c>
-      <c r="S7" s="22">
+      <c r="U7" s="22">
         <v>0.79900000000000004</v>
       </c>
-      <c r="T7" s="13">
-        <f>R7/$D7</f>
-        <v>0.72590656648154195</v>
-      </c>
-      <c r="U7" s="30" t="s">
+      <c r="V7" s="13">
+        <f>T7/$F7</f>
+        <v>0.71909385113268609</v>
+      </c>
+      <c r="W7" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
@@ -1390,67 +1416,69 @@
       <c r="C8" s="10">
         <v>4.18</v>
       </c>
-      <c r="D8" s="9">
-        <v>3390</v>
-      </c>
-      <c r="E8" s="10">
-        <v>1.17</v>
-      </c>
-      <c r="F8" s="23">
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9">
+        <v>3379</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1.18</v>
+      </c>
+      <c r="H8" s="23">
         <v>9301</v>
       </c>
-      <c r="G8" s="24">
+      <c r="I8" s="24">
         <v>0.42799999999999999</v>
       </c>
-      <c r="H8" s="14">
-        <f t="shared" ref="H8:H16" si="0">F8/$D8</f>
-        <v>2.7436578171091446</v>
-      </c>
-      <c r="I8" s="23">
+      <c r="J8" s="14">
+        <f t="shared" ref="J8:J16" si="0">H8/$F8</f>
+        <v>2.7525895235276709</v>
+      </c>
+      <c r="K8" s="23">
         <v>10375</v>
       </c>
-      <c r="J8" s="24">
+      <c r="L8" s="24">
         <v>0.38400000000000001</v>
       </c>
-      <c r="K8" s="14">
-        <f t="shared" ref="K8:K16" si="1">I8/$D8</f>
-        <v>3.0604719764011801</v>
-      </c>
-      <c r="L8" s="23">
+      <c r="M8" s="14">
+        <f t="shared" ref="M8:M16" si="1">K8/$F8</f>
+        <v>3.0704350399526485</v>
+      </c>
+      <c r="N8" s="23">
         <v>8693</v>
       </c>
-      <c r="M8" s="24">
+      <c r="O8" s="24">
         <v>0.45800000000000002</v>
       </c>
-      <c r="N8" s="14">
-        <f t="shared" ref="N8:N16" si="2">L8/$D8</f>
-        <v>2.5643067846607668</v>
-      </c>
-      <c r="O8" s="23">
+      <c r="P8" s="14">
+        <f t="shared" ref="P8:P16" si="2">N8/$F8</f>
+        <v>2.5726546315477954</v>
+      </c>
+      <c r="Q8" s="23">
         <v>8686</v>
       </c>
-      <c r="P8" s="24">
+      <c r="R8" s="24">
         <v>0.45800000000000002</v>
       </c>
-      <c r="Q8" s="14">
-        <f t="shared" ref="Q8:Q16" si="3">O8/$D8</f>
-        <v>2.5622418879056048</v>
-      </c>
-      <c r="R8" s="23">
+      <c r="S8" s="14">
+        <f t="shared" ref="S8:S16" si="3">Q8/$F8</f>
+        <v>2.5705830127256584</v>
+      </c>
+      <c r="T8" s="23">
         <v>1956</v>
       </c>
-      <c r="S8" s="24">
+      <c r="U8" s="24">
         <v>2.04</v>
       </c>
-      <c r="T8" s="14">
-        <f t="shared" ref="T8:T16" si="4">R8/$D8</f>
-        <v>0.57699115044247784</v>
-      </c>
-      <c r="U8" s="31" t="s">
+      <c r="V8" s="14">
+        <f t="shared" ref="V8:V16" si="4">T8/$F8</f>
+        <v>0.57886948801420535</v>
+      </c>
+      <c r="W8" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
@@ -1460,67 +1488,69 @@
       <c r="C9" s="10">
         <v>3.35</v>
       </c>
-      <c r="D9" s="9">
-        <v>3182</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1.48</v>
-      </c>
-      <c r="F9" s="23">
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9">
+        <v>3225</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1.46</v>
+      </c>
+      <c r="H9" s="23">
         <v>3654</v>
       </c>
-      <c r="G9" s="24">
+      <c r="I9" s="24">
         <v>1.29</v>
       </c>
-      <c r="H9" s="14">
+      <c r="J9" s="14">
         <f t="shared" si="0"/>
-        <v>1.1483343808925204</v>
-      </c>
-      <c r="I9" s="23">
+        <v>1.1330232558139535</v>
+      </c>
+      <c r="K9" s="23">
         <v>4774</v>
       </c>
-      <c r="J9" s="24">
+      <c r="L9" s="24">
         <v>0.98899999999999999</v>
       </c>
-      <c r="K9" s="14">
+      <c r="M9" s="14">
         <f t="shared" si="1"/>
-        <v>1.5003142677561283</v>
-      </c>
-      <c r="L9" s="23">
+        <v>1.4803100775193798</v>
+      </c>
+      <c r="N9" s="23">
         <v>3558</v>
       </c>
-      <c r="M9" s="24">
+      <c r="O9" s="24">
         <v>1.33</v>
       </c>
-      <c r="N9" s="14">
+      <c r="P9" s="14">
         <f t="shared" si="2"/>
-        <v>1.1181646763042112</v>
-      </c>
-      <c r="O9" s="23">
+        <v>1.1032558139534883</v>
+      </c>
+      <c r="Q9" s="23">
         <v>3548</v>
       </c>
-      <c r="P9" s="24">
+      <c r="R9" s="24">
         <v>1.33</v>
       </c>
-      <c r="Q9" s="14">
+      <c r="S9" s="14">
         <f t="shared" si="3"/>
-        <v>1.1150219987429291</v>
-      </c>
-      <c r="R9" s="23">
+        <v>1.1001550387596899</v>
+      </c>
+      <c r="T9" s="23">
         <v>2695</v>
       </c>
-      <c r="S9" s="24">
+      <c r="U9" s="24">
         <v>1.75</v>
       </c>
-      <c r="T9" s="14">
+      <c r="V9" s="14">
         <f t="shared" si="4"/>
-        <v>0.84695160276555626</v>
-      </c>
-      <c r="U9" s="31" t="s">
+        <v>0.83565891472868215</v>
+      </c>
+      <c r="W9" s="31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
@@ -1530,67 +1560,69 @@
       <c r="C10" s="10">
         <v>2.09</v>
       </c>
-      <c r="D10" s="9">
-        <v>2576</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9">
+        <v>2604</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.626</v>
+      </c>
+      <c r="H10" s="23">
         <v>8210</v>
       </c>
-      <c r="G10" s="24">
+      <c r="I10" s="24">
         <v>0.19900000000000001</v>
       </c>
-      <c r="H10" s="14">
+      <c r="J10" s="14">
         <f t="shared" si="0"/>
-        <v>3.1871118012422359</v>
-      </c>
-      <c r="I10" s="23">
+        <v>3.1528417818740397</v>
+      </c>
+      <c r="K10" s="23">
         <v>10257</v>
       </c>
-      <c r="J10" s="24">
+      <c r="L10" s="24">
         <v>0.159</v>
       </c>
-      <c r="K10" s="14">
+      <c r="M10" s="14">
         <f t="shared" si="1"/>
-        <v>3.9817546583850931</v>
-      </c>
-      <c r="L10" s="23">
+        <v>3.9389400921658986</v>
+      </c>
+      <c r="N10" s="23">
         <v>7892</v>
       </c>
-      <c r="M10" s="24">
+      <c r="O10" s="24">
         <v>0.20699999999999999</v>
       </c>
-      <c r="N10" s="14">
+      <c r="P10" s="14">
         <f t="shared" si="2"/>
-        <v>3.0636645962732918</v>
-      </c>
-      <c r="O10" s="23">
+        <v>3.0307219662058373</v>
+      </c>
+      <c r="Q10" s="23">
         <v>7991</v>
       </c>
-      <c r="P10" s="24">
+      <c r="R10" s="24">
         <v>0.20399999999999999</v>
       </c>
-      <c r="Q10" s="14">
+      <c r="S10" s="14">
         <f t="shared" si="3"/>
-        <v>3.1020962732919255</v>
-      </c>
-      <c r="R10" s="23">
+        <v>3.0687403993855606</v>
+      </c>
+      <c r="T10" s="23">
         <v>1768</v>
       </c>
-      <c r="S10" s="24">
+      <c r="U10" s="24">
         <v>0.92200000000000004</v>
       </c>
-      <c r="T10" s="14">
+      <c r="V10" s="14">
         <f t="shared" si="4"/>
-        <v>0.68633540372670809</v>
-      </c>
-      <c r="U10" s="31" t="s">
+        <v>0.67895545314900152</v>
+      </c>
+      <c r="W10" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -1600,67 +1632,69 @@
       <c r="C11" s="10">
         <v>2.66</v>
       </c>
-      <c r="D11" s="9">
-        <v>1711</v>
-      </c>
-      <c r="E11" s="10">
-        <v>0.82799999999999996</v>
-      </c>
-      <c r="F11" s="23">
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9">
+        <v>1651</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="H11" s="23">
         <v>4563</v>
       </c>
-      <c r="G11" s="24">
+      <c r="I11" s="24">
         <v>0.311</v>
       </c>
-      <c r="H11" s="14">
+      <c r="J11" s="14">
         <f t="shared" si="0"/>
-        <v>2.6668614845119811</v>
-      </c>
-      <c r="I11" s="23">
+        <v>2.7637795275590551</v>
+      </c>
+      <c r="K11" s="23">
         <v>5285</v>
       </c>
-      <c r="J11" s="24">
+      <c r="L11" s="24">
         <v>0.26800000000000002</v>
       </c>
-      <c r="K11" s="14">
+      <c r="M11" s="14">
         <f t="shared" si="1"/>
-        <v>3.0888369374634714</v>
-      </c>
-      <c r="L11" s="23">
+        <v>3.2010902483343426</v>
+      </c>
+      <c r="N11" s="23">
         <v>4313</v>
       </c>
-      <c r="M11" s="24">
+      <c r="O11" s="24">
         <v>0.32900000000000001</v>
       </c>
-      <c r="N11" s="14">
+      <c r="P11" s="14">
         <f t="shared" si="2"/>
-        <v>2.5207481005260082</v>
-      </c>
-      <c r="O11" s="23">
+        <v>2.6123561477892188</v>
+      </c>
+      <c r="Q11" s="23">
         <v>4392</v>
       </c>
-      <c r="P11" s="24">
+      <c r="R11" s="24">
         <v>0.32300000000000001</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="S11" s="14">
         <f t="shared" si="3"/>
-        <v>2.5669199298655756</v>
-      </c>
-      <c r="R11" s="23">
+        <v>2.6602059357964869</v>
+      </c>
+      <c r="T11" s="23">
         <v>1178</v>
       </c>
-      <c r="S11" s="24">
+      <c r="U11" s="24">
         <v>1.2</v>
       </c>
-      <c r="T11" s="14">
+      <c r="V11" s="14">
         <f t="shared" si="4"/>
-        <v>0.68848626534190527</v>
-      </c>
-      <c r="U11" s="31" t="s">
+        <v>0.71350696547546943</v>
+      </c>
+      <c r="W11" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
@@ -1670,67 +1704,69 @@
       <c r="C12" s="10">
         <v>3.19</v>
       </c>
-      <c r="D12" s="9">
-        <v>2921</v>
-      </c>
-      <c r="E12" s="10">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="9">
+        <v>2926</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="H12" s="23">
         <v>4333</v>
       </c>
-      <c r="G12" s="24">
+      <c r="I12" s="24">
         <v>0.40699999999999997</v>
       </c>
-      <c r="H12" s="14">
+      <c r="J12" s="14">
         <f t="shared" si="0"/>
-        <v>1.4833960972269771</v>
-      </c>
-      <c r="I12" s="23">
+        <v>1.4808612440191387</v>
+      </c>
+      <c r="K12" s="23">
         <v>4305</v>
       </c>
-      <c r="J12" s="24">
+      <c r="L12" s="24">
         <v>0.41</v>
       </c>
-      <c r="K12" s="14">
+      <c r="M12" s="14">
         <f t="shared" si="1"/>
-        <v>1.4738103389250257</v>
-      </c>
-      <c r="L12" s="23">
+        <v>1.4712918660287082</v>
+      </c>
+      <c r="N12" s="23">
         <v>4009</v>
       </c>
-      <c r="M12" s="24">
+      <c r="O12" s="24">
         <v>0.44</v>
       </c>
-      <c r="N12" s="14">
+      <c r="P12" s="14">
         <f t="shared" si="2"/>
-        <v>1.3724751797329682</v>
-      </c>
-      <c r="O12" s="23">
+        <v>1.3701298701298701</v>
+      </c>
+      <c r="Q12" s="23">
         <v>4017</v>
       </c>
-      <c r="P12" s="24">
+      <c r="R12" s="24">
         <v>0.439</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="S12" s="14">
         <f t="shared" si="3"/>
-        <v>1.3752139678192399</v>
-      </c>
-      <c r="R12" s="23">
+        <v>1.3728639781271361</v>
+      </c>
+      <c r="T12" s="23">
         <v>2590</v>
       </c>
-      <c r="S12" s="24">
+      <c r="U12" s="24">
         <v>0.68100000000000005</v>
       </c>
-      <c r="T12" s="14">
+      <c r="V12" s="14">
         <f t="shared" si="4"/>
-        <v>0.88668264293050325</v>
-      </c>
-      <c r="U12" s="31" t="s">
+        <v>0.88516746411483249</v>
+      </c>
+      <c r="W12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
@@ -1740,67 +1776,69 @@
       <c r="C13" s="10">
         <v>1.85</v>
       </c>
-      <c r="D13" s="9">
-        <v>2459</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="F13" s="23">
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9">
+        <v>2443</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="H13" s="23">
         <v>10330</v>
       </c>
-      <c r="G13" s="24">
+      <c r="I13" s="24">
         <v>0.13900000000000001</v>
       </c>
-      <c r="H13" s="14">
+      <c r="J13" s="14">
         <f t="shared" si="0"/>
-        <v>4.2008946726311507</v>
-      </c>
-      <c r="I13" s="23">
+        <v>4.228407695456406</v>
+      </c>
+      <c r="K13" s="23">
         <v>10327</v>
       </c>
-      <c r="J13" s="24">
+      <c r="L13" s="24">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K13" s="14">
+      <c r="M13" s="14">
         <f t="shared" si="1"/>
-        <v>4.1996746644977634</v>
-      </c>
-      <c r="L13" s="23">
+        <v>4.227179697093737</v>
+      </c>
+      <c r="N13" s="23">
         <v>10089</v>
       </c>
-      <c r="M13" s="24">
+      <c r="O13" s="24">
         <v>0.14199999999999999</v>
       </c>
-      <c r="N13" s="14">
+      <c r="P13" s="14">
         <f t="shared" si="2"/>
-        <v>4.1028873525823508</v>
-      </c>
-      <c r="O13" s="23">
+        <v>4.1297584936553422</v>
+      </c>
+      <c r="Q13" s="23">
         <v>10104</v>
       </c>
-      <c r="P13" s="24">
+      <c r="R13" s="24">
         <v>0.14199999999999999</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="S13" s="14">
         <f t="shared" si="3"/>
-        <v>4.1089873932492882</v>
-      </c>
-      <c r="R13" s="23">
+        <v>4.1358984854686858</v>
+      </c>
+      <c r="T13" s="23">
         <v>1603</v>
       </c>
-      <c r="S13" s="24">
+      <c r="U13" s="24">
         <v>0.89400000000000002</v>
       </c>
-      <c r="T13" s="14">
+      <c r="V13" s="14">
         <f t="shared" si="4"/>
-        <v>0.65189101260675075</v>
-      </c>
-      <c r="U13" s="31" t="s">
+        <v>0.65616045845272208</v>
+      </c>
+      <c r="W13" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
@@ -1810,67 +1848,69 @@
       <c r="C14" s="10">
         <v>1.63</v>
       </c>
-      <c r="D14" s="9">
-        <v>3171</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="F14" s="23">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="9">
+        <v>3176</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="H14" s="23">
         <v>7517</v>
       </c>
-      <c r="G14" s="24">
+      <c r="I14" s="24">
         <v>0.22700000000000001</v>
       </c>
-      <c r="H14" s="14">
+      <c r="J14" s="14">
         <f t="shared" si="0"/>
-        <v>2.3705455692210657</v>
-      </c>
-      <c r="I14" s="23">
+        <v>2.3668136020151134</v>
+      </c>
+      <c r="K14" s="23">
         <v>6737</v>
       </c>
-      <c r="J14" s="24">
+      <c r="L14" s="24">
         <v>0.253</v>
       </c>
-      <c r="K14" s="14">
+      <c r="M14" s="14">
         <f t="shared" si="1"/>
-        <v>2.1245663828445287</v>
-      </c>
-      <c r="L14" s="23">
+        <v>2.1212216624685141</v>
+      </c>
+      <c r="N14" s="23">
         <v>6716</v>
       </c>
-      <c r="M14" s="24">
+      <c r="O14" s="24">
         <v>0.254</v>
       </c>
-      <c r="N14" s="14">
+      <c r="P14" s="14">
         <f t="shared" si="2"/>
-        <v>2.1179438662882371</v>
-      </c>
-      <c r="O14" s="23">
+        <v>2.1146095717884132</v>
+      </c>
+      <c r="Q14" s="23">
         <v>7568</v>
       </c>
-      <c r="P14" s="24">
+      <c r="R14" s="24">
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="S14" s="14">
         <f t="shared" si="3"/>
-        <v>2.3866288237149162</v>
-      </c>
-      <c r="R14" s="23">
+        <v>2.3828715365239295</v>
+      </c>
+      <c r="T14" s="23">
         <v>2080</v>
       </c>
-      <c r="S14" s="24">
+      <c r="U14" s="24">
         <v>0.82</v>
       </c>
-      <c r="T14" s="14">
+      <c r="V14" s="14">
         <f t="shared" si="4"/>
-        <v>0.65594449700409962</v>
-      </c>
-      <c r="U14" s="31" t="s">
+        <v>0.65491183879093195</v>
+      </c>
+      <c r="W14" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
@@ -1880,67 +1920,69 @@
       <c r="C15" s="10">
         <v>3.77</v>
       </c>
-      <c r="D15" s="9">
-        <v>2213</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9">
+        <v>2214</v>
+      </c>
+      <c r="G15" s="10">
         <v>1.33</v>
       </c>
-      <c r="F15" s="23">
+      <c r="H15" s="23">
         <v>4891</v>
       </c>
-      <c r="G15" s="24">
+      <c r="I15" s="24">
         <v>0.60099999999999998</v>
       </c>
-      <c r="H15" s="14">
+      <c r="J15" s="14">
         <f t="shared" si="0"/>
-        <v>2.2101220063262539</v>
-      </c>
-      <c r="I15" s="23">
+        <v>2.2091237579042455</v>
+      </c>
+      <c r="K15" s="23">
         <v>4807</v>
       </c>
-      <c r="J15" s="24">
+      <c r="L15" s="24">
         <v>0.61199999999999999</v>
       </c>
-      <c r="K15" s="14">
+      <c r="M15" s="14">
         <f t="shared" si="1"/>
-        <v>2.1721644826028017</v>
-      </c>
-      <c r="L15" s="23">
+        <v>2.1711833785004515</v>
+      </c>
+      <c r="N15" s="23">
         <v>4849</v>
       </c>
-      <c r="M15" s="24">
+      <c r="O15" s="24">
         <v>0.60599999999999998</v>
       </c>
-      <c r="N15" s="14">
+      <c r="P15" s="14">
         <f t="shared" si="2"/>
-        <v>2.1911432444645276</v>
-      </c>
-      <c r="O15" s="23">
+        <v>2.1901535682023487</v>
+      </c>
+      <c r="Q15" s="23">
         <v>4763</v>
       </c>
-      <c r="P15" s="24">
+      <c r="R15" s="24">
         <v>0.61699999999999999</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="S15" s="14">
         <f t="shared" si="3"/>
-        <v>2.1522819701762312</v>
-      </c>
-      <c r="R15" s="23">
+        <v>2.1513098464317975</v>
+      </c>
+      <c r="T15" s="23">
         <v>1575</v>
       </c>
-      <c r="S15" s="24">
+      <c r="U15" s="24">
         <v>1.87</v>
       </c>
-      <c r="T15" s="14">
+      <c r="V15" s="14">
         <f t="shared" si="4"/>
-        <v>0.71170356981473115</v>
-      </c>
-      <c r="U15" s="31" t="s">
+        <v>0.71138211382113825</v>
+      </c>
+      <c r="W15" s="31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
@@ -1950,162 +1992,170 @@
       <c r="C16" s="12">
         <v>1.33</v>
       </c>
-      <c r="D16" s="11">
-        <v>8915</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="11">
+        <v>8919</v>
+      </c>
+      <c r="G16" s="12">
         <v>0.69299999999999995</v>
       </c>
-      <c r="F16" s="25">
+      <c r="H16" s="25">
         <v>12625</v>
       </c>
-      <c r="G16" s="26">
+      <c r="I16" s="26">
         <v>0.49</v>
       </c>
-      <c r="H16" s="15">
+      <c r="J16" s="15">
         <f t="shared" si="0"/>
-        <v>1.4161525518788558</v>
-      </c>
-      <c r="I16" s="25">
+        <v>1.4155174346899877</v>
+      </c>
+      <c r="K16" s="25">
         <v>13272</v>
       </c>
-      <c r="J16" s="26">
+      <c r="L16" s="26">
         <v>0.46600000000000003</v>
       </c>
-      <c r="K16" s="15">
+      <c r="M16" s="15">
         <f t="shared" si="1"/>
-        <v>1.4887268648345484</v>
-      </c>
-      <c r="L16" s="25">
+        <v>1.4880591994618231</v>
+      </c>
+      <c r="N16" s="25">
         <v>12543</v>
       </c>
-      <c r="M16" s="26">
+      <c r="O16" s="26">
         <v>0.49299999999999999</v>
       </c>
-      <c r="N16" s="15">
+      <c r="P16" s="15">
         <f t="shared" si="2"/>
-        <v>1.4069545709478408</v>
-      </c>
-      <c r="O16" s="25">
+        <v>1.4063235788765556</v>
+      </c>
+      <c r="Q16" s="25">
         <v>14671</v>
       </c>
-      <c r="P16" s="26">
+      <c r="R16" s="26">
         <v>0.42099999999999999</v>
       </c>
-      <c r="Q16" s="15">
+      <c r="S16" s="15">
         <f t="shared" si="3"/>
-        <v>1.6456533931575996</v>
-      </c>
-      <c r="R16" s="25">
+        <v>1.6449153492544006</v>
+      </c>
+      <c r="T16" s="25">
         <v>11083</v>
       </c>
-      <c r="S16" s="26">
+      <c r="U16" s="26">
         <v>0.55800000000000005</v>
       </c>
-      <c r="T16" s="15">
+      <c r="V16" s="15">
         <f t="shared" si="4"/>
-        <v>1.2431856421761076</v>
-      </c>
-      <c r="U16" s="32" t="s">
+        <v>1.2426280973203274</v>
+      </c>
+      <c r="W16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+    <row r="17" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="44" t="s">
+      <c r="C17" s="43"/>
+      <c r="D17" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="51" t="s">
+      <c r="E17" s="43"/>
+      <c r="F17" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="20" t="s">
+      <c r="I17" s="52"/>
+      <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="51" t="s">
+      <c r="K17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="52"/>
-      <c r="K17" s="20" t="s">
+      <c r="L17" s="52"/>
+      <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="51" t="s">
+      <c r="N17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="52"/>
-      <c r="N17" s="20" t="s">
+      <c r="O17" s="52"/>
+      <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="51" t="s">
+      <c r="Q17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="20" t="s">
+      <c r="R17" s="52"/>
+      <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="R17" s="51" t="s">
+      <c r="T17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="S17" s="52"/>
-      <c r="T17" s="20" t="s">
+      <c r="U17" s="52"/>
+      <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="40">
+    <row r="18" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44">
         <v>2.52</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="40">
-        <v>0.78810000000000002</v>
-      </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="53">
+      <c r="C18" s="45"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="44">
+        <v>0.78869999999999996</v>
+      </c>
+      <c r="G18" s="45"/>
+      <c r="H18" s="53">
         <v>0.3337</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="27">
-        <f>$D$18/F18</f>
-        <v>2.3617021276595747</v>
-      </c>
-      <c r="I18" s="53">
+      <c r="I18" s="54"/>
+      <c r="J18" s="27">
+        <f>$F$18/H18</f>
+        <v>2.3635001498351813</v>
+      </c>
+      <c r="K18" s="53">
         <v>0.31390000000000001</v>
       </c>
-      <c r="J18" s="54"/>
-      <c r="K18" s="27">
-        <f>$D$18/I18</f>
-        <v>2.5106721885950938</v>
-      </c>
-      <c r="L18" s="53">
+      <c r="L18" s="54"/>
+      <c r="M18" s="27">
+        <f>$F$18/K18</f>
+        <v>2.5125836253583942</v>
+      </c>
+      <c r="N18" s="53">
         <v>0.35489999999999999</v>
       </c>
-      <c r="M18" s="54"/>
-      <c r="N18" s="27">
-        <f>$D$18/L18</f>
-        <v>2.2206255283178362</v>
-      </c>
-      <c r="O18" s="53">
+      <c r="O18" s="54"/>
+      <c r="P18" s="27">
+        <f>$F$18/N18</f>
+        <v>2.2223161453930684</v>
+      </c>
+      <c r="Q18" s="53">
         <v>0.34489999999999998</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="27">
-        <f>$D$18/O18</f>
-        <v>2.2850101478689475</v>
-      </c>
-      <c r="R18" s="53">
+      <c r="R18" s="54"/>
+      <c r="S18" s="27">
+        <f>$F$18/Q18</f>
+        <v>2.2867497825456655</v>
+      </c>
+      <c r="T18" s="53">
         <v>1.05</v>
       </c>
-      <c r="S18" s="54"/>
-      <c r="T18" s="27">
-        <f>$D$18/R18</f>
-        <v>0.75057142857142856</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U18" s="54"/>
+      <c r="V18" s="27">
+        <f>$F$18/T18</f>
+        <v>0.75114285714285711</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2113,9 +2163,11 @@
         <v>18</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -2123,9 +2175,11 @@
         <v>20</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -2133,9 +2187,11 @@
         <v>22</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2143,9 +2199,11 @@
         <v>37</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2153,15 +2211,17 @@
         <v>24</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -2169,52 +2229,58 @@
         <v>29</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="I30" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="D18:E18"/>
+  <mergeCells count="32">
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
-  <conditionalFormatting sqref="H7:H16">
+  <conditionalFormatting sqref="J7:J16">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2226,7 +2292,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:K16">
+  <conditionalFormatting sqref="M7:M16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2238,7 +2304,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N7:N16">
+  <conditionalFormatting sqref="P7:P16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2250,7 +2316,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q7:Q16">
+  <conditionalFormatting sqref="S7:S16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2262,7 +2328,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T7:T16">
+  <conditionalFormatting sqref="V7:V16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
add new benchmark results to table
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAF989B-E8FD-F549-9F90-836464AA55D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CC7777-1E0D-2A4B-8EA9-AFD7CB140284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
   <si>
     <t>Benchmark</t>
   </si>
@@ -258,6 +258,33 @@
   </si>
   <si>
     <t>rv8</t>
+  </si>
+  <si>
+    <t>Base Score*</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <t>v1.2.3-51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (f44daeb5)</t>
+    </r>
+  </si>
+  <si>
+    <t>after lazy_replace</t>
+  </si>
+  <si>
+    <t>after new allocation</t>
   </si>
 </sst>
 </file>
@@ -678,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -749,6 +776,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,31 +827,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1117,18 +1156,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="5" width="8.1640625" hidden="1" customWidth="1"/>
+    <col min="3" max="5" width="8.1640625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
@@ -1140,10 +1178,13 @@
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="19" width="13.33203125" hidden="1" customWidth="1"/>
     <col min="20" max="22" width="13.33203125" customWidth="1"/>
-    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5" customWidth="1"/>
+    <col min="24" max="24" width="12.1640625" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1152,7 +1193,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -1161,109 +1202,131 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:23" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+    </row>
+    <row r="4" spans="1:26" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="38" t="s">
+      <c r="C4" s="48"/>
+      <c r="D4" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="38" t="s">
+      <c r="E4" s="48"/>
+      <c r="F4" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="46" t="s">
+      <c r="G4" s="48"/>
+      <c r="H4" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="46" t="s">
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="47"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="46" t="s">
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="46" t="s">
+      <c r="O4" s="39"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="47"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="46" t="s">
+      <c r="R4" s="39"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="47"/>
-      <c r="V4" s="48"/>
-    </row>
-    <row r="5" spans="1:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="U4" s="39"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="40"/>
+    </row>
+    <row r="5" spans="1:26" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="40" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="40" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="49" t="s">
+      <c r="G5" s="50"/>
+      <c r="H5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="50"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="50"/>
+      <c r="L5" s="42"/>
       <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="49" t="s">
+      <c r="N5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="50"/>
+      <c r="O5" s="42"/>
       <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="49" t="s">
+      <c r="Q5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="50"/>
+      <c r="R5" s="42"/>
       <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="49" t="s">
+      <c r="T5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="50"/>
+      <c r="U5" s="42"/>
       <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="28" t="s">
+      <c r="W5" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="42"/>
+      <c r="Y5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
@@ -1330,11 +1393,20 @@
       <c r="V6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="29" t="s">
+      <c r="W6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z6" s="29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>3</v>
       </c>
@@ -1344,8 +1416,12 @@
       <c r="C7" s="8">
         <v>2.71</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>44</v>
+      </c>
       <c r="F7" s="7">
         <v>3090</v>
       </c>
@@ -1402,11 +1478,21 @@
         <f>T7/$F7</f>
         <v>0.71909385113268609</v>
       </c>
-      <c r="W7" s="30" t="s">
+      <c r="W7" s="21">
+        <v>2196</v>
+      </c>
+      <c r="X7" s="22">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="Y7" s="13">
+        <f>W7/$F7</f>
+        <v>0.71067961165048543</v>
+      </c>
+      <c r="Z7" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
@@ -1416,8 +1502,12 @@
       <c r="C8" s="10">
         <v>4.18</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>44</v>
+      </c>
       <c r="F8" s="9">
         <v>3379</v>
       </c>
@@ -1474,11 +1564,21 @@
         <f t="shared" ref="V8:V16" si="4">T8/$F8</f>
         <v>0.57886948801420535</v>
       </c>
-      <c r="W8" s="31" t="s">
+      <c r="W8" s="23">
+        <v>1926</v>
+      </c>
+      <c r="X8" s="24">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="Y8" s="14">
+        <f t="shared" ref="Y8:Y16" si="5">W8/$F8</f>
+        <v>0.56999112163361942</v>
+      </c>
+      <c r="Z8" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
@@ -1488,8 +1588,12 @@
       <c r="C9" s="10">
         <v>3.35</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>44</v>
+      </c>
       <c r="F9" s="9">
         <v>3225</v>
       </c>
@@ -1546,11 +1650,21 @@
         <f t="shared" si="4"/>
         <v>0.83565891472868215</v>
       </c>
-      <c r="W9" s="31" t="s">
+      <c r="W9" s="23">
+        <v>2672</v>
+      </c>
+      <c r="X9" s="24">
+        <v>1.77</v>
+      </c>
+      <c r="Y9" s="14">
+        <f t="shared" si="5"/>
+        <v>0.82852713178294579</v>
+      </c>
+      <c r="Z9" s="31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
@@ -1560,8 +1674,12 @@
       <c r="C10" s="10">
         <v>2.09</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>44</v>
+      </c>
       <c r="F10" s="9">
         <v>2604</v>
       </c>
@@ -1618,11 +1736,21 @@
         <f t="shared" si="4"/>
         <v>0.67895545314900152</v>
       </c>
-      <c r="W10" s="31" t="s">
+      <c r="W10" s="23">
+        <v>1757</v>
+      </c>
+      <c r="X10" s="24">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="Y10" s="14">
+        <f t="shared" si="5"/>
+        <v>0.67473118279569888</v>
+      </c>
+      <c r="Z10" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -1632,8 +1760,12 @@
       <c r="C11" s="10">
         <v>2.66</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>44</v>
+      </c>
       <c r="F11" s="9">
         <v>1651</v>
       </c>
@@ -1690,11 +1822,21 @@
         <f t="shared" si="4"/>
         <v>0.71350696547546943</v>
       </c>
-      <c r="W11" s="31" t="s">
+      <c r="W11" s="23">
+        <v>1105</v>
+      </c>
+      <c r="X11" s="24">
+        <v>1.28</v>
+      </c>
+      <c r="Y11" s="14">
+        <f t="shared" si="5"/>
+        <v>0.6692913385826772</v>
+      </c>
+      <c r="Z11" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
@@ -1704,8 +1846,12 @@
       <c r="C12" s="10">
         <v>3.19</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
+      <c r="D12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>44</v>
+      </c>
       <c r="F12" s="9">
         <v>2926</v>
       </c>
@@ -1762,11 +1908,21 @@
         <f t="shared" si="4"/>
         <v>0.88516746411483249</v>
       </c>
-      <c r="W12" s="31" t="s">
+      <c r="W12" s="23">
+        <v>2766</v>
+      </c>
+      <c r="X12" s="24">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="Y12" s="14">
+        <f t="shared" si="5"/>
+        <v>0.94531784005468211</v>
+      </c>
+      <c r="Z12" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
@@ -1776,8 +1932,12 @@
       <c r="C13" s="10">
         <v>1.85</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>44</v>
+      </c>
       <c r="F13" s="9">
         <v>2443</v>
       </c>
@@ -1834,11 +1994,21 @@
         <f t="shared" si="4"/>
         <v>0.65616045845272208</v>
       </c>
-      <c r="W13" s="31" t="s">
+      <c r="W13" s="23">
+        <v>1564</v>
+      </c>
+      <c r="X13" s="24">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="Y13" s="14">
+        <f t="shared" si="5"/>
+        <v>0.64019647973802707</v>
+      </c>
+      <c r="Z13" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
@@ -1848,8 +2018,12 @@
       <c r="C14" s="10">
         <v>1.63</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>44</v>
+      </c>
       <c r="F14" s="9">
         <v>3176</v>
       </c>
@@ -1906,11 +2080,21 @@
         <f t="shared" si="4"/>
         <v>0.65491183879093195</v>
       </c>
-      <c r="W14" s="31" t="s">
+      <c r="W14" s="23">
+        <v>1952</v>
+      </c>
+      <c r="X14" s="24">
+        <v>0.874</v>
+      </c>
+      <c r="Y14" s="14">
+        <f t="shared" si="5"/>
+        <v>0.61460957178841313</v>
+      </c>
+      <c r="Z14" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
@@ -1920,8 +2104,12 @@
       <c r="C15" s="10">
         <v>3.77</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="9">
+        <v>2171</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.35</v>
+      </c>
       <c r="F15" s="9">
         <v>2214</v>
       </c>
@@ -1978,11 +2166,21 @@
         <f t="shared" si="4"/>
         <v>0.71138211382113825</v>
       </c>
-      <c r="W15" s="31" t="s">
+      <c r="W15" s="23">
+        <v>1580</v>
+      </c>
+      <c r="X15" s="24">
+        <v>1.86</v>
+      </c>
+      <c r="Y15" s="14">
+        <f t="shared" si="5"/>
+        <v>0.71364046973803075</v>
+      </c>
+      <c r="Z15" s="31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
@@ -1992,8 +2190,12 @@
       <c r="C16" s="12">
         <v>1.33</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
+      <c r="D16" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>44</v>
+      </c>
       <c r="F16" s="11">
         <v>8919</v>
       </c>
@@ -2050,112 +2252,139 @@
         <f t="shared" si="4"/>
         <v>1.2426280973203274</v>
       </c>
-      <c r="W16" s="32" t="s">
+      <c r="W16" s="25">
+        <v>7575</v>
+      </c>
+      <c r="X16" s="26">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="Y16" s="15">
+        <f t="shared" si="5"/>
+        <v>0.84931046081399264</v>
+      </c>
+      <c r="Z16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+    <row r="17" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="B17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="42" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="52"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="51" t="s">
+      <c r="K17" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="52"/>
+      <c r="L17" s="44"/>
       <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="51" t="s">
+      <c r="N17" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="52"/>
+      <c r="O17" s="44"/>
       <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="51" t="s">
+      <c r="Q17" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="52"/>
+      <c r="R17" s="44"/>
       <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="51" t="s">
+      <c r="T17" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="52"/>
+      <c r="U17" s="44"/>
       <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="44">
+      <c r="W17" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="X17" s="44"/>
+      <c r="Y17" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="53">
         <v>2.52</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="44">
+      <c r="C18" s="54"/>
+      <c r="D18" s="53">
+        <v>1.35</v>
+      </c>
+      <c r="E18" s="54"/>
+      <c r="F18" s="53">
         <v>0.78869999999999996</v>
       </c>
-      <c r="G18" s="45"/>
-      <c r="H18" s="53">
+      <c r="G18" s="54"/>
+      <c r="H18" s="45">
         <v>0.3337</v>
       </c>
-      <c r="I18" s="54"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="27">
         <f>$F$18/H18</f>
         <v>2.3635001498351813</v>
       </c>
-      <c r="K18" s="53">
+      <c r="K18" s="45">
         <v>0.31390000000000001</v>
       </c>
-      <c r="L18" s="54"/>
+      <c r="L18" s="46"/>
       <c r="M18" s="27">
         <f>$F$18/K18</f>
         <v>2.5125836253583942</v>
       </c>
-      <c r="N18" s="53">
+      <c r="N18" s="45">
         <v>0.35489999999999999</v>
       </c>
-      <c r="O18" s="54"/>
+      <c r="O18" s="46"/>
       <c r="P18" s="27">
         <f>$F$18/N18</f>
         <v>2.2223161453930684</v>
       </c>
-      <c r="Q18" s="53">
+      <c r="Q18" s="45">
         <v>0.34489999999999998</v>
       </c>
-      <c r="R18" s="54"/>
+      <c r="R18" s="46"/>
       <c r="S18" s="27">
         <f>$F$18/Q18</f>
         <v>2.2867497825456655</v>
       </c>
-      <c r="T18" s="53">
+      <c r="T18" s="45">
         <v>1.05</v>
       </c>
-      <c r="U18" s="54"/>
+      <c r="U18" s="46"/>
       <c r="V18" s="27">
         <f>$F$18/T18</f>
         <v>0.75114285714285711</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W18" s="45">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="27">
+        <f>$F$18/W18</f>
+        <v>0.71054054054054039</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2167,7 +2396,7 @@
       <c r="E20" s="3"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -2179,7 +2408,7 @@
       <c r="E21" s="3"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -2191,7 +2420,7 @@
       <c r="E22" s="3"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2203,7 +2432,7 @@
       <c r="E23" s="3"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2215,13 +2444,13 @@
       <c r="E24" s="3"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -2233,20 +2462,46 @@
       <c r="E26" s="3"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="K30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="38">
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="T17:U17"/>
@@ -2259,28 +2514,20 @@
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:M16">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2292,7 +2539,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7:M16">
+  <conditionalFormatting sqref="P7:P16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2304,7 +2551,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:P16">
+  <conditionalFormatting sqref="S7:S16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2316,7 +2563,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S7:S16">
+  <conditionalFormatting sqref="V7:V16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2328,7 +2575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V7:V16">
+  <conditionalFormatting sqref="Y7:Y16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2341,6 +2588,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="76" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add results so far to overview
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CC7777-1E0D-2A4B-8EA9-AFD7CB140284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED369A8-1473-A14D-98CB-A729810C1C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
   <si>
     <t>Benchmark</t>
   </si>
@@ -260,9 +260,6 @@
     <t>rv8</t>
   </si>
   <si>
-    <t>Base Score*</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -286,6 +283,59 @@
   <si>
     <t>after new allocation</t>
   </si>
+  <si>
+    <r>
+      <t>v1.3.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (cfeedc41)</t>
+    </r>
+  </si>
+  <si>
+    <t>finalized</t>
+  </si>
+  <si>
+    <t>finalized no-fusion</t>
+  </si>
+  <si>
+    <r>
+      <t>v1.3.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (cfeedc41)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --optimize=no-fusion</t>
+    </r>
+  </si>
+  <si>
+    <t>1,22 (invalid - miscompare)</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
 </sst>
 </file>
 
@@ -294,7 +344,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +391,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -705,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -776,6 +833,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,42 +896,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,10 +1216,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:AI30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1180,11 +1240,11 @@
     <col min="20" max="22" width="13.33203125" customWidth="1"/>
     <col min="23" max="23" width="12.5" customWidth="1"/>
     <col min="24" max="24" width="12.1640625" customWidth="1"/>
-    <col min="25" max="25" width="13.33203125" customWidth="1"/>
-    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="31" width="13.33203125" customWidth="1"/>
+    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:34" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1193,7 +1253,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -1202,131 +1262,165 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="T3" s="58" t="s">
+      <c r="T3" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+    </row>
+    <row r="4" spans="1:34" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="47"/>
+      <c r="F4" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="47"/>
+      <c r="H4" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="51"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="51"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="51"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="51"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
+      <c r="AA4" s="51"/>
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="52"/>
     </row>
-    <row r="4" spans="1:26" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="39"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="39"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4" s="39"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="U4" s="39"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="40"/>
-    </row>
-    <row r="5" spans="1:26" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="49" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="49" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="41" t="s">
+      <c r="G5" s="43"/>
+      <c r="H5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="42"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="42"/>
+      <c r="L5" s="54"/>
       <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="41" t="s">
+      <c r="N5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="42"/>
+      <c r="O5" s="54"/>
       <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="41" t="s">
+      <c r="Q5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="42"/>
+      <c r="R5" s="54"/>
       <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="41" t="s">
+      <c r="T5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="42"/>
+      <c r="U5" s="54"/>
       <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="41" t="s">
+      <c r="W5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="42"/>
+      <c r="X5" s="54"/>
       <c r="Y5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Z5" s="28" t="s">
+      <c r="Z5" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC5" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="54"/>
+      <c r="AE5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
@@ -1402,11 +1496,30 @@
       <c r="Y6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="Z6" s="29" t="s">
+      <c r="Z6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF6" s="29" t="s">
         <v>0</v>
       </c>
+      <c r="AH6" s="61"/>
     </row>
-    <row r="7" spans="1:26" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>3</v>
       </c>
@@ -1417,10 +1530,10 @@
         <v>2.71</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>43</v>
       </c>
       <c r="F7" s="7">
         <v>3090</v>
@@ -1488,11 +1601,32 @@
         <f>W7/$F7</f>
         <v>0.71067961165048543</v>
       </c>
-      <c r="Z7" s="30" t="s">
+      <c r="Z7" s="21">
+        <v>1994</v>
+      </c>
+      <c r="AA7" s="22">
+        <v>0.89</v>
+      </c>
+      <c r="AB7" s="13">
+        <f>Z7/$F7</f>
+        <v>0.64530744336569579</v>
+      </c>
+      <c r="AC7" s="21">
+        <v>1997</v>
+      </c>
+      <c r="AD7" s="22">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="AE7" s="13">
+        <f>AC7/$F7</f>
+        <v>0.6462783171521036</v>
+      </c>
+      <c r="AF7" s="30" t="s">
         <v>3</v>
       </c>
+      <c r="AH7" s="61"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
@@ -1503,10 +1637,10 @@
         <v>4.18</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="F8" s="9">
         <v>3379</v>
@@ -1574,11 +1708,32 @@
         <f t="shared" ref="Y8:Y16" si="5">W8/$F8</f>
         <v>0.56999112163361942</v>
       </c>
-      <c r="Z8" s="31" t="s">
+      <c r="Z8" s="23">
+        <v>1785</v>
+      </c>
+      <c r="AA8" s="24">
+        <v>2.23</v>
+      </c>
+      <c r="AB8" s="14">
+        <f t="shared" ref="AB8:AB16" si="6">Z8/$F8</f>
+        <v>0.52826279964486533</v>
+      </c>
+      <c r="AC8" s="23">
+        <v>1790</v>
+      </c>
+      <c r="AD8" s="24">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AE8" s="14">
+        <f t="shared" ref="AE8:AE16" si="7">AC8/$F8</f>
+        <v>0.52974252737496297</v>
+      </c>
+      <c r="AF8" s="31" t="s">
         <v>4</v>
       </c>
+      <c r="AH8" s="61"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
@@ -1589,10 +1744,10 @@
         <v>3.35</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="F9" s="9">
         <v>3225</v>
@@ -1660,11 +1815,32 @@
         <f t="shared" si="5"/>
         <v>0.82852713178294579</v>
       </c>
-      <c r="Z9" s="31" t="s">
+      <c r="Z9" s="23">
+        <v>2510</v>
+      </c>
+      <c r="AA9" s="24">
+        <v>1.88</v>
+      </c>
+      <c r="AB9" s="14">
+        <f t="shared" si="6"/>
+        <v>0.77829457364341081</v>
+      </c>
+      <c r="AC9" s="23">
+        <v>2495</v>
+      </c>
+      <c r="AD9" s="24">
+        <v>1.89</v>
+      </c>
+      <c r="AE9" s="14">
+        <f t="shared" si="7"/>
+        <v>0.77364341085271315</v>
+      </c>
+      <c r="AF9" s="31" t="s">
         <v>5</v>
       </c>
+      <c r="AH9" s="61"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
@@ -1675,10 +1851,10 @@
         <v>2.09</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="F10" s="9">
         <v>2604</v>
@@ -1746,11 +1922,32 @@
         <f t="shared" si="5"/>
         <v>0.67473118279569888</v>
       </c>
-      <c r="Z10" s="31" t="s">
+      <c r="Z10" s="23">
+        <v>1669</v>
+      </c>
+      <c r="AA10" s="24">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="AB10" s="14">
+        <f t="shared" si="6"/>
+        <v>0.64093701996927799</v>
+      </c>
+      <c r="AC10" s="23">
+        <v>1671</v>
+      </c>
+      <c r="AD10" s="24">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AE10" s="14">
+        <f t="shared" si="7"/>
+        <v>0.64170506912442393</v>
+      </c>
+      <c r="AF10" s="31" t="s">
         <v>6</v>
       </c>
+      <c r="AH10" s="61"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -1761,10 +1958,10 @@
         <v>2.66</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="F11" s="9">
         <v>1651</v>
@@ -1832,11 +2029,32 @@
         <f t="shared" si="5"/>
         <v>0.6692913385826772</v>
       </c>
-      <c r="Z11" s="31" t="s">
+      <c r="Z11" s="23">
+        <v>981</v>
+      </c>
+      <c r="AA11" s="24">
+        <v>1.44</v>
+      </c>
+      <c r="AB11" s="14">
+        <f t="shared" si="6"/>
+        <v>0.59418534221683827</v>
+      </c>
+      <c r="AC11" s="23">
+        <v>975</v>
+      </c>
+      <c r="AD11" s="24">
+        <v>1.45</v>
+      </c>
+      <c r="AE11" s="14">
+        <f t="shared" si="7"/>
+        <v>0.59055118110236215</v>
+      </c>
+      <c r="AF11" s="31" t="s">
         <v>7</v>
       </c>
+      <c r="AH11" s="61"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
@@ -1847,10 +2065,10 @@
         <v>3.19</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="F12" s="9">
         <v>2926</v>
@@ -1918,11 +2136,32 @@
         <f t="shared" si="5"/>
         <v>0.94531784005468211</v>
       </c>
-      <c r="Z12" s="31" t="s">
+      <c r="Z12" s="23">
+        <v>2735</v>
+      </c>
+      <c r="AA12" s="24">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="AB12" s="14">
+        <f t="shared" si="6"/>
+        <v>0.93472317156527684</v>
+      </c>
+      <c r="AC12" s="23">
+        <v>2738</v>
+      </c>
+      <c r="AD12" s="24">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AE12" s="14">
+        <f t="shared" si="7"/>
+        <v>0.93574846206425155</v>
+      </c>
+      <c r="AF12" s="31" t="s">
         <v>8</v>
       </c>
+      <c r="AH12" s="61"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
@@ -1933,10 +2172,10 @@
         <v>1.85</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="F13" s="9">
         <v>2443</v>
@@ -2004,11 +2243,32 @@
         <f t="shared" si="5"/>
         <v>0.64019647973802707</v>
       </c>
-      <c r="Z13" s="31" t="s">
+      <c r="Z13" s="23">
+        <v>1492</v>
+      </c>
+      <c r="AA13" s="24">
+        <v>0.96</v>
+      </c>
+      <c r="AB13" s="14">
+        <f t="shared" si="6"/>
+        <v>0.61072451903397462</v>
+      </c>
+      <c r="AC13" s="23">
+        <v>1516</v>
+      </c>
+      <c r="AD13" s="24">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AE13" s="14">
+        <f t="shared" si="7"/>
+        <v>0.6205485059353254</v>
+      </c>
+      <c r="AF13" s="31" t="s">
         <v>9</v>
       </c>
+      <c r="AH13" s="61"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
@@ -2019,10 +2279,10 @@
         <v>1.63</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="F14" s="9">
         <v>3176</v>
@@ -2090,11 +2350,32 @@
         <f t="shared" si="5"/>
         <v>0.61460957178841313</v>
       </c>
-      <c r="Z14" s="31" t="s">
+      <c r="Z14" s="23">
+        <v>1867</v>
+      </c>
+      <c r="AA14" s="24">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="AB14" s="14">
+        <f t="shared" si="6"/>
+        <v>0.5878463476070529</v>
+      </c>
+      <c r="AC14" s="23">
+        <v>1892</v>
+      </c>
+      <c r="AD14" s="24">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="AE14" s="14">
+        <f t="shared" si="7"/>
+        <v>0.59571788413098237</v>
+      </c>
+      <c r="AF14" s="31" t="s">
         <v>10</v>
       </c>
+      <c r="AH14" s="61"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
@@ -2176,11 +2457,32 @@
         <f t="shared" si="5"/>
         <v>0.71364046973803075</v>
       </c>
-      <c r="Z15" s="31" t="s">
+      <c r="Z15" s="23">
+        <v>1461</v>
+      </c>
+      <c r="AA15" s="24">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AB15" s="14">
+        <f t="shared" si="6"/>
+        <v>0.65989159891598914</v>
+      </c>
+      <c r="AC15" s="23">
+        <v>1463</v>
+      </c>
+      <c r="AD15" s="24">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AE15" s="14">
+        <f t="shared" si="7"/>
+        <v>0.66079494128274618</v>
+      </c>
+      <c r="AF15" s="31" t="s">
         <v>11</v>
       </c>
+      <c r="AH15" s="61"/>
     </row>
-    <row r="16" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
@@ -2191,10 +2493,10 @@
         <v>1.33</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="F16" s="11">
         <v>8919</v>
@@ -2262,129 +2564,180 @@
         <f t="shared" si="5"/>
         <v>0.84931046081399264</v>
       </c>
-      <c r="Z16" s="32" t="s">
+      <c r="Z16" s="25">
+        <v>7385</v>
+      </c>
+      <c r="AA16" s="26">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="AB16" s="15">
+        <f t="shared" si="6"/>
+        <v>0.82800762417311358</v>
+      </c>
+      <c r="AC16" s="59">
+        <v>7746</v>
+      </c>
+      <c r="AD16" s="60">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="15">
+        <f t="shared" si="7"/>
+        <v>0.86848301379078374</v>
+      </c>
+      <c r="AF16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="51" t="s">
+    <row r="17" spans="1:35" ht="19" x14ac:dyDescent="0.25">
+      <c r="B17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="51" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="43" t="s">
+      <c r="E17" s="49"/>
+      <c r="F17" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="49"/>
+      <c r="H17" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="44"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="43" t="s">
+      <c r="K17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="44"/>
+      <c r="L17" s="56"/>
       <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="43" t="s">
+      <c r="N17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="44"/>
+      <c r="O17" s="56"/>
       <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="43" t="s">
+      <c r="Q17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="44"/>
+      <c r="R17" s="56"/>
       <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="43" t="s">
+      <c r="T17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="44"/>
+      <c r="U17" s="56"/>
       <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="W17" s="43" t="s">
+      <c r="W17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="44"/>
+      <c r="X17" s="56"/>
       <c r="Y17" s="20" t="s">
         <v>31</v>
       </c>
+      <c r="Z17" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA17" s="56"/>
+      <c r="AB17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC17" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD17" s="56"/>
+      <c r="AE17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH17" s="61"/>
+      <c r="AI17" s="61"/>
     </row>
-    <row r="18" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="53">
+    <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44">
         <v>2.52</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="53">
+      <c r="C18" s="45"/>
+      <c r="D18" s="44">
         <v>1.35</v>
       </c>
-      <c r="E18" s="54"/>
-      <c r="F18" s="53">
+      <c r="E18" s="45"/>
+      <c r="F18" s="44">
         <v>0.78869999999999996</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="45">
+      <c r="G18" s="45"/>
+      <c r="H18" s="57">
         <v>0.3337</v>
       </c>
-      <c r="I18" s="46"/>
+      <c r="I18" s="58"/>
       <c r="J18" s="27">
         <f>$F$18/H18</f>
         <v>2.3635001498351813</v>
       </c>
-      <c r="K18" s="45">
+      <c r="K18" s="57">
         <v>0.31390000000000001</v>
       </c>
-      <c r="L18" s="46"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="27">
         <f>$F$18/K18</f>
         <v>2.5125836253583942</v>
       </c>
-      <c r="N18" s="45">
+      <c r="N18" s="57">
         <v>0.35489999999999999</v>
       </c>
-      <c r="O18" s="46"/>
+      <c r="O18" s="58"/>
       <c r="P18" s="27">
         <f>$F$18/N18</f>
         <v>2.2223161453930684</v>
       </c>
-      <c r="Q18" s="45">
+      <c r="Q18" s="57">
         <v>0.34489999999999998</v>
       </c>
-      <c r="R18" s="46"/>
+      <c r="R18" s="58"/>
       <c r="S18" s="27">
         <f>$F$18/Q18</f>
         <v>2.2867497825456655</v>
       </c>
-      <c r="T18" s="45">
+      <c r="T18" s="57">
         <v>1.05</v>
       </c>
-      <c r="U18" s="46"/>
+      <c r="U18" s="58"/>
       <c r="V18" s="27">
         <f>$F$18/T18</f>
         <v>0.75114285714285711</v>
       </c>
-      <c r="W18" s="45">
+      <c r="W18" s="57">
         <v>1.1100000000000001</v>
       </c>
-      <c r="X18" s="46"/>
+      <c r="X18" s="58"/>
       <c r="Y18" s="27">
         <f>$F$18/W18</f>
         <v>0.71054054054054039</v>
       </c>
+      <c r="Z18" s="57">
+        <v>1.18</v>
+      </c>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="27">
+        <f>$F$18/Z18</f>
+        <v>0.66838983050847456</v>
+      </c>
+      <c r="AC18" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="27" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2396,7 +2749,7 @@
       <c r="E20" s="3"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -2408,7 +2761,7 @@
       <c r="E21" s="3"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -2420,7 +2773,7 @@
       <c r="E22" s="3"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2432,7 +2785,7 @@
       <c r="E23" s="3"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2444,13 +2797,13 @@
       <c r="E24" s="3"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -2462,20 +2815,52 @@
       <c r="E26" s="3"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="K30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="48">
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="W3:Y3"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="B5:C5"/>
@@ -2492,30 +2877,32 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J16">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:M16">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P7:P16">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2527,7 +2914,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7:M16">
+  <conditionalFormatting sqref="S7:S16">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2539,7 +2926,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:P16">
+  <conditionalFormatting sqref="V7:V16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2551,7 +2938,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S7:S16">
+  <conditionalFormatting sqref="Y7:Y16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2563,7 +2950,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V7:V16">
+  <conditionalFormatting sqref="AB7:AB16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2575,7 +2962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y7:Y16">
+  <conditionalFormatting sqref="AE7:AE16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
include results in overview table
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED369A8-1473-A14D-98CB-A729810C1C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1B66D-E91C-F846-980A-85ADBB14A817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="59">
   <si>
     <t>Benchmark</t>
   </si>
@@ -299,12 +299,6 @@
     </r>
   </si>
   <si>
-    <t>finalized</t>
-  </si>
-  <si>
-    <t>finalized no-fusion</t>
-  </si>
-  <si>
     <r>
       <t>v1.3.0</t>
     </r>
@@ -336,6 +330,134 @@
   <si>
     <t>invalid</t>
   </si>
+  <si>
+    <t>buggy</t>
+  </si>
+  <si>
+    <t>buggy no-fusion</t>
+  </si>
+  <si>
+    <r>
+      <t>v1.3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (523411b3)</t>
+    </r>
+  </si>
+  <si>
+    <t>finalized…</t>
+  </si>
+  <si>
+    <r>
+      <t>v1.3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (523411b3)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --optimize=no-fusion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>v1.3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (523411b3)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --optimize=no-ras</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>v1.3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (523411b3)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --optimize=no-jump-no-ras</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>v1.3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (523411b3)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --optimize=none</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -344,7 +466,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,8 +520,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +561,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -758,11 +907,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -842,63 +1004,80 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,10 +1395,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AI30"/>
+  <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH5" sqref="AH5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="57" workbookViewId="0">
+      <selection activeCell="AL24" sqref="AL24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1236,15 +1415,21 @@
     <col min="13" max="13" width="13.33203125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="12.1640625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="19" width="13.33203125" hidden="1" customWidth="1"/>
-    <col min="20" max="22" width="13.33203125" customWidth="1"/>
-    <col min="23" max="23" width="12.5" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" customWidth="1"/>
-    <col min="25" max="31" width="13.33203125" customWidth="1"/>
-    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="22" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="25" max="31" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="32" max="40" width="13.33203125" customWidth="1"/>
+    <col min="41" max="41" width="15.5" customWidth="1"/>
+    <col min="42" max="42" width="15.6640625" customWidth="1"/>
+    <col min="43" max="43" width="16.5" customWidth="1"/>
+    <col min="44" max="44" width="12.5" customWidth="1"/>
+    <col min="45" max="45" width="13.33203125" customWidth="1"/>
+    <col min="46" max="46" width="12.1640625" customWidth="1"/>
+    <col min="47" max="47" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:49" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1253,7 +1438,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:34" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -1262,165 +1447,242 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:34" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="T3" s="41" t="s">
+      <c r="T3" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41" t="s">
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="41"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41" t="s">
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="53"/>
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="53"/>
+      <c r="AM3" s="53"/>
+      <c r="AN3" s="53"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="53"/>
+      <c r="AQ3" s="53"/>
+      <c r="AR3" s="53"/>
+      <c r="AS3" s="53"/>
+      <c r="AT3" s="53"/>
+    </row>
+    <row r="4" spans="1:49" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="68"/>
+      <c r="D4" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="F4" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="68"/>
+      <c r="H4" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="60"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="60"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="60"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="60"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA4" s="60"/>
+      <c r="AB4" s="61"/>
+      <c r="AC4" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD3" s="41"/>
-      <c r="AE3" s="41"/>
+      <c r="AD4" s="60"/>
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ4" s="60"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM4" s="60"/>
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP4" s="55"/>
+      <c r="AQ4" s="62"/>
+      <c r="AR4" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS4" s="55"/>
+      <c r="AT4" s="56"/>
     </row>
-    <row r="4" spans="1:34" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4" s="51"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="U4" s="51"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD4" s="51"/>
-      <c r="AE4" s="52"/>
-    </row>
-    <row r="5" spans="1:34" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="42" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="42" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="53" t="s">
+      <c r="G5" s="64"/>
+      <c r="H5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="54"/>
+      <c r="I5" s="58"/>
       <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="54"/>
+      <c r="L5" s="58"/>
       <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="53" t="s">
+      <c r="N5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="54"/>
+      <c r="O5" s="58"/>
       <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="53" t="s">
+      <c r="Q5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="54"/>
+      <c r="R5" s="58"/>
       <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="53" t="s">
+      <c r="T5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="54"/>
+      <c r="U5" s="58"/>
       <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="53" t="s">
+      <c r="W5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="54"/>
+      <c r="X5" s="58"/>
       <c r="Y5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Z5" s="53" t="s">
+      <c r="Z5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="54"/>
+      <c r="AA5" s="58"/>
       <c r="AB5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" s="53" t="s">
+      <c r="AC5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="54"/>
+      <c r="AD5" s="58"/>
       <c r="AE5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="28" t="s">
+      <c r="AF5" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI5" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL5" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO5" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR5" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU5" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>0</v>
       </c>
@@ -1514,12 +1776,57 @@
       <c r="AE6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AF6" s="29" t="s">
+      <c r="AF6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="AH6" s="61"/>
+      <c r="AW6" s="43"/>
     </row>
-    <row r="7" spans="1:34" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:49" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>3</v>
       </c>
@@ -1621,12 +1928,50 @@
         <f>AC7/$F7</f>
         <v>0.6462783171521036</v>
       </c>
-      <c r="AF7" s="30" t="s">
+      <c r="AF7" s="21">
+        <v>2028</v>
+      </c>
+      <c r="AG7" s="22">
+        <v>0.875</v>
+      </c>
+      <c r="AH7" s="13">
+        <f>AF7/$F7</f>
+        <v>0.65631067961165046</v>
+      </c>
+      <c r="AI7" s="21">
+        <v>2108</v>
+      </c>
+      <c r="AJ7" s="22">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="AK7" s="13">
+        <f>AI7/$F7</f>
+        <v>0.68220064724919094</v>
+      </c>
+      <c r="AL7" s="21"/>
+      <c r="AM7" s="22"/>
+      <c r="AN7" s="13">
+        <f>AL7/$F7</f>
+        <v>0</v>
+      </c>
+      <c r="AO7" s="21"/>
+      <c r="AP7" s="22"/>
+      <c r="AQ7" s="13">
+        <f>AO7/$F7</f>
+        <v>0</v>
+      </c>
+      <c r="AR7" s="21"/>
+      <c r="AS7" s="22"/>
+      <c r="AT7" s="13">
+        <f>AR7/$F7</f>
+        <v>0</v>
+      </c>
+      <c r="AU7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="AH7" s="61"/>
+      <c r="AW7" s="43"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
@@ -1728,12 +2073,50 @@
         <f t="shared" ref="AE8:AE16" si="7">AC8/$F8</f>
         <v>0.52974252737496297</v>
       </c>
-      <c r="AF8" s="31" t="s">
+      <c r="AF8" s="23">
+        <v>1784</v>
+      </c>
+      <c r="AG8" s="24">
+        <v>2.23</v>
+      </c>
+      <c r="AH8" s="14">
+        <f t="shared" ref="AH8:AH16" si="8">AF8/$F8</f>
+        <v>0.52796685409884581</v>
+      </c>
+      <c r="AI8" s="23">
+        <v>1800</v>
+      </c>
+      <c r="AJ8" s="24">
+        <v>2.21</v>
+      </c>
+      <c r="AK8" s="14">
+        <f t="shared" ref="AK8:AK16" si="9">AI8/$F8</f>
+        <v>0.53270198283515835</v>
+      </c>
+      <c r="AL8" s="23"/>
+      <c r="AM8" s="24"/>
+      <c r="AN8" s="14">
+        <f t="shared" ref="AN8:AN16" si="10">AL8/$F8</f>
+        <v>0</v>
+      </c>
+      <c r="AO8" s="23"/>
+      <c r="AP8" s="24"/>
+      <c r="AQ8" s="14">
+        <f t="shared" ref="AQ8:AQ16" si="11">AO8/$F8</f>
+        <v>0</v>
+      </c>
+      <c r="AR8" s="23"/>
+      <c r="AS8" s="24"/>
+      <c r="AT8" s="14">
+        <f t="shared" ref="AT8:AT16" si="12">AR8/$F8</f>
+        <v>0</v>
+      </c>
+      <c r="AU8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AH8" s="61"/>
+      <c r="AW8" s="43"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
@@ -1835,12 +2218,50 @@
         <f t="shared" si="7"/>
         <v>0.77364341085271315</v>
       </c>
-      <c r="AF9" s="31" t="s">
+      <c r="AF9" s="23">
+        <v>2484</v>
+      </c>
+      <c r="AG9" s="24">
+        <v>1.9</v>
+      </c>
+      <c r="AH9" s="14">
+        <f t="shared" si="8"/>
+        <v>0.77023255813953484</v>
+      </c>
+      <c r="AI9" s="23">
+        <v>2532</v>
+      </c>
+      <c r="AJ9" s="24">
+        <v>1.86</v>
+      </c>
+      <c r="AK9" s="14">
+        <f t="shared" si="9"/>
+        <v>0.78511627906976744</v>
+      </c>
+      <c r="AL9" s="23"/>
+      <c r="AM9" s="24"/>
+      <c r="AN9" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO9" s="23"/>
+      <c r="AP9" s="24"/>
+      <c r="AQ9" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR9" s="23"/>
+      <c r="AS9" s="24"/>
+      <c r="AT9" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AH9" s="61"/>
+      <c r="AW9" s="43"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
@@ -1942,12 +2363,50 @@
         <f t="shared" si="7"/>
         <v>0.64170506912442393</v>
       </c>
-      <c r="AF10" s="31" t="s">
+      <c r="AF10" s="23">
+        <v>1640</v>
+      </c>
+      <c r="AG10" s="24">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="AH10" s="14">
+        <f t="shared" si="8"/>
+        <v>0.62980030721966207</v>
+      </c>
+      <c r="AI10" s="23">
+        <v>1679</v>
+      </c>
+      <c r="AJ10" s="24">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="AK10" s="14">
+        <f t="shared" si="9"/>
+        <v>0.64477726574500771</v>
+      </c>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="24"/>
+      <c r="AN10" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO10" s="23"/>
+      <c r="AP10" s="24"/>
+      <c r="AQ10" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR10" s="23"/>
+      <c r="AS10" s="24"/>
+      <c r="AT10" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="AH10" s="61"/>
+      <c r="AW10" s="43"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -2049,12 +2508,50 @@
         <f t="shared" si="7"/>
         <v>0.59055118110236215</v>
       </c>
-      <c r="AF11" s="31" t="s">
+      <c r="AF11" s="23">
+        <v>964</v>
+      </c>
+      <c r="AG11" s="24">
+        <v>1.47</v>
+      </c>
+      <c r="AH11" s="14">
+        <f t="shared" si="8"/>
+        <v>0.58388855239248938</v>
+      </c>
+      <c r="AI11" s="23">
+        <v>988</v>
+      </c>
+      <c r="AJ11" s="24">
+        <v>1.43</v>
+      </c>
+      <c r="AK11" s="14">
+        <f t="shared" si="9"/>
+        <v>0.59842519685039375</v>
+      </c>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="24"/>
+      <c r="AN11" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="23"/>
+      <c r="AP11" s="24"/>
+      <c r="AQ11" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR11" s="23"/>
+      <c r="AS11" s="24"/>
+      <c r="AT11" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="AH11" s="61"/>
+      <c r="AW11" s="43"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
@@ -2156,12 +2653,50 @@
         <f t="shared" si="7"/>
         <v>0.93574846206425155</v>
       </c>
-      <c r="AF12" s="31" t="s">
+      <c r="AF12" s="23">
+        <v>2739</v>
+      </c>
+      <c r="AG12" s="24">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AH12" s="14">
+        <f t="shared" si="8"/>
+        <v>0.93609022556390975</v>
+      </c>
+      <c r="AI12" s="23">
+        <v>2744</v>
+      </c>
+      <c r="AJ12" s="24">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="AK12" s="14">
+        <f t="shared" si="9"/>
+        <v>0.93779904306220097</v>
+      </c>
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="24"/>
+      <c r="AN12" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO12" s="23"/>
+      <c r="AP12" s="24"/>
+      <c r="AQ12" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR12" s="23"/>
+      <c r="AS12" s="24"/>
+      <c r="AT12" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="AH12" s="61"/>
+      <c r="AW12" s="43"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
@@ -2263,12 +2798,50 @@
         <f t="shared" si="7"/>
         <v>0.6205485059353254</v>
       </c>
-      <c r="AF13" s="31" t="s">
+      <c r="AF13" s="23">
+        <v>1494</v>
+      </c>
+      <c r="AG13" s="24">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="AH13" s="14">
+        <f t="shared" si="8"/>
+        <v>0.61154318460908719</v>
+      </c>
+      <c r="AI13" s="23">
+        <v>1503</v>
+      </c>
+      <c r="AJ13" s="24">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="AK13" s="14">
+        <f t="shared" si="9"/>
+        <v>0.61522717969709373</v>
+      </c>
+      <c r="AL13" s="23"/>
+      <c r="AM13" s="24"/>
+      <c r="AN13" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO13" s="23"/>
+      <c r="AP13" s="24"/>
+      <c r="AQ13" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR13" s="23"/>
+      <c r="AS13" s="24"/>
+      <c r="AT13" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU13" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AH13" s="61"/>
+      <c r="AW13" s="43"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
@@ -2370,12 +2943,50 @@
         <f t="shared" si="7"/>
         <v>0.59571788413098237</v>
       </c>
-      <c r="AF14" s="31" t="s">
+      <c r="AF14" s="23">
+        <v>1871</v>
+      </c>
+      <c r="AG14" s="24">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AH14" s="14">
+        <f t="shared" si="8"/>
+        <v>0.58910579345088165</v>
+      </c>
+      <c r="AI14" s="23">
+        <v>1881</v>
+      </c>
+      <c r="AJ14" s="24">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="AK14" s="14">
+        <f t="shared" si="9"/>
+        <v>0.59225440806045337</v>
+      </c>
+      <c r="AL14" s="23"/>
+      <c r="AM14" s="24"/>
+      <c r="AN14" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="24"/>
+      <c r="AQ14" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR14" s="23"/>
+      <c r="AS14" s="24"/>
+      <c r="AT14" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU14" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="AH14" s="61"/>
+      <c r="AW14" s="43"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
@@ -2477,12 +3088,50 @@
         <f t="shared" si="7"/>
         <v>0.66079494128274618</v>
       </c>
-      <c r="AF15" s="31" t="s">
+      <c r="AF15" s="23">
+        <v>1450</v>
+      </c>
+      <c r="AG15" s="24">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AH15" s="14">
+        <f t="shared" si="8"/>
+        <v>0.65492321589882563</v>
+      </c>
+      <c r="AI15" s="23">
+        <v>1444</v>
+      </c>
+      <c r="AJ15" s="24">
+        <v>2.04</v>
+      </c>
+      <c r="AK15" s="14">
+        <f t="shared" si="9"/>
+        <v>0.65221318879855461</v>
+      </c>
+      <c r="AL15" s="23"/>
+      <c r="AM15" s="24"/>
+      <c r="AN15" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO15" s="23"/>
+      <c r="AP15" s="24"/>
+      <c r="AQ15" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR15" s="23"/>
+      <c r="AS15" s="24"/>
+      <c r="AT15" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU15" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="AH15" s="61"/>
+      <c r="AW15" s="43"/>
     </row>
-    <row r="16" spans="1:34" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
@@ -2574,170 +3223,277 @@
         <f t="shared" si="6"/>
         <v>0.82800762417311358</v>
       </c>
-      <c r="AC16" s="59">
+      <c r="AC16" s="41">
         <v>7746</v>
       </c>
-      <c r="AD16" s="60">
+      <c r="AD16" s="42">
         <v>0</v>
       </c>
       <c r="AE16" s="15">
         <f t="shared" si="7"/>
         <v>0.86848301379078374</v>
       </c>
-      <c r="AF16" s="32" t="s">
+      <c r="AF16" s="25">
+        <v>7365</v>
+      </c>
+      <c r="AG16" s="26">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="AH16" s="15">
+        <f t="shared" si="8"/>
+        <v>0.82576522031617894</v>
+      </c>
+      <c r="AI16" s="44">
+        <v>7488</v>
+      </c>
+      <c r="AJ16" s="45">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="AK16" s="15">
+        <f t="shared" si="9"/>
+        <v>0.83955600403632691</v>
+      </c>
+      <c r="AL16" s="44"/>
+      <c r="AM16" s="45"/>
+      <c r="AN16" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AO16" s="44"/>
+      <c r="AP16" s="45"/>
+      <c r="AQ16" s="15">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AR16" s="44"/>
+      <c r="AS16" s="45"/>
+      <c r="AT16" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+    <row r="17" spans="1:50" ht="19" x14ac:dyDescent="0.25">
+      <c r="B17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="48" t="s">
+      <c r="C17" s="70"/>
+      <c r="D17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="48" t="s">
+      <c r="E17" s="70"/>
+      <c r="F17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="55" t="s">
+      <c r="G17" s="70"/>
+      <c r="H17" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="56"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="55" t="s">
+      <c r="K17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="56"/>
+      <c r="L17" s="50"/>
       <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="55" t="s">
+      <c r="N17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="56"/>
+      <c r="O17" s="50"/>
       <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="55" t="s">
+      <c r="Q17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="56"/>
+      <c r="R17" s="50"/>
       <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="55" t="s">
+      <c r="T17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="56"/>
+      <c r="U17" s="50"/>
       <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="W17" s="55" t="s">
+      <c r="W17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="56"/>
+      <c r="X17" s="50"/>
       <c r="Y17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Z17" s="55" t="s">
+      <c r="Z17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AA17" s="56"/>
+      <c r="AA17" s="50"/>
       <c r="AB17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AC17" s="55" t="s">
+      <c r="AC17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AD17" s="56"/>
+      <c r="AD17" s="50"/>
       <c r="AE17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
+      <c r="AF17" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG17" s="50"/>
+      <c r="AH17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI17" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ17" s="50"/>
+      <c r="AK17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL17" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM17" s="50"/>
+      <c r="AN17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO17" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP17" s="50"/>
+      <c r="AQ17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR17" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS17" s="50"/>
+      <c r="AT17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW17" s="43"/>
+      <c r="AX17" s="43"/>
     </row>
-    <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="44">
+    <row r="18" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="65">
         <v>2.52</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="44">
+      <c r="C18" s="66"/>
+      <c r="D18" s="65">
         <v>1.35</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="44">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <v>0.78869999999999996</v>
       </c>
-      <c r="G18" s="45"/>
-      <c r="H18" s="57">
+      <c r="G18" s="66"/>
+      <c r="H18" s="51">
         <v>0.3337</v>
       </c>
-      <c r="I18" s="58"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="27">
         <f>$F$18/H18</f>
         <v>2.3635001498351813</v>
       </c>
-      <c r="K18" s="57">
+      <c r="K18" s="51">
         <v>0.31390000000000001</v>
       </c>
-      <c r="L18" s="58"/>
+      <c r="L18" s="52"/>
       <c r="M18" s="27">
         <f>$F$18/K18</f>
         <v>2.5125836253583942</v>
       </c>
-      <c r="N18" s="57">
+      <c r="N18" s="51">
         <v>0.35489999999999999</v>
       </c>
-      <c r="O18" s="58"/>
+      <c r="O18" s="52"/>
       <c r="P18" s="27">
         <f>$F$18/N18</f>
         <v>2.2223161453930684</v>
       </c>
-      <c r="Q18" s="57">
+      <c r="Q18" s="51">
         <v>0.34489999999999998</v>
       </c>
-      <c r="R18" s="58"/>
+      <c r="R18" s="52"/>
       <c r="S18" s="27">
         <f>$F$18/Q18</f>
         <v>2.2867497825456655</v>
       </c>
-      <c r="T18" s="57">
+      <c r="T18" s="51">
         <v>1.05</v>
       </c>
-      <c r="U18" s="58"/>
+      <c r="U18" s="52"/>
       <c r="V18" s="27">
         <f>$F$18/T18</f>
         <v>0.75114285714285711</v>
       </c>
-      <c r="W18" s="57">
+      <c r="W18" s="51">
         <v>1.1100000000000001</v>
       </c>
-      <c r="X18" s="58"/>
+      <c r="X18" s="52"/>
       <c r="Y18" s="27">
         <f>$F$18/W18</f>
         <v>0.71054054054054039</v>
       </c>
-      <c r="Z18" s="57">
+      <c r="Z18" s="51">
         <v>1.18</v>
       </c>
-      <c r="AA18" s="58"/>
+      <c r="AA18" s="52"/>
       <c r="AB18" s="27">
         <f>$F$18/Z18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AC18" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD18" s="58"/>
+      <c r="AC18" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD18" s="52"/>
       <c r="AE18" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="AF18" s="51">
+        <v>1.18</v>
+      </c>
+      <c r="AG18" s="52"/>
+      <c r="AH18" s="27">
+        <f>$F$18/AF18</f>
+        <v>0.66838983050847456</v>
+      </c>
+      <c r="AI18" s="51">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AJ18" s="52"/>
+      <c r="AK18" s="27">
+        <f>$F$18/AI18</f>
+        <v>0.67991379310344824</v>
+      </c>
+      <c r="AL18" s="51"/>
+      <c r="AM18" s="52"/>
+      <c r="AN18" s="27" t="e">
+        <f>$F$18/AL18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AO18" s="51"/>
+      <c r="AP18" s="52"/>
+      <c r="AQ18" s="27" t="e">
+        <f>$F$18/AO18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR18" s="51"/>
+      <c r="AS18" s="52"/>
+      <c r="AT18" s="27" t="e">
+        <f>$F$18/AR18</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -2749,7 +3505,7 @@
       <c r="E20" s="3"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -2761,7 +3517,7 @@
       <c r="E21" s="3"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -2772,8 +3528,13 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="K22" s="2"/>
+      <c r="AG22" s="46"/>
+      <c r="AH22" s="46"/>
+      <c r="AI22" s="46"/>
+      <c r="AJ22" s="46"/>
+      <c r="AK22" s="46"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2784,8 +3545,13 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="K23" s="2"/>
+      <c r="AG23" s="46"/>
+      <c r="AH23" s="47"/>
+      <c r="AI23" s="46"/>
+      <c r="AJ23" s="48"/>
+      <c r="AK23" s="46"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2796,14 +3562,24 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="K24" s="2"/>
+      <c r="AG24" s="46"/>
+      <c r="AH24" s="47"/>
+      <c r="AI24" s="46"/>
+      <c r="AJ24" s="48"/>
+      <c r="AK24" s="46"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="K25" s="2"/>
+      <c r="AG25" s="46"/>
+      <c r="AH25" s="47"/>
+      <c r="AI25" s="46"/>
+      <c r="AJ25" s="48"/>
+      <c r="AK25" s="46"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -2814,21 +3590,74 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="K26" s="2"/>
+      <c r="AG26" s="46"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="48"/>
+      <c r="AK26" s="46"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
       <c r="K27" s="2"/>
+      <c r="AG27" s="46"/>
+      <c r="AH27" s="47"/>
+      <c r="AI27" s="46"/>
+      <c r="AJ27" s="48"/>
+      <c r="AK27" s="46"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
       <c r="K28" s="2"/>
+      <c r="AG28" s="46"/>
+      <c r="AH28" s="47"/>
+      <c r="AI28" s="46"/>
+      <c r="AJ28" s="48"/>
+      <c r="AK28" s="46"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
       <c r="K29" s="2"/>
+      <c r="AG29" s="46"/>
+      <c r="AH29" s="47"/>
+      <c r="AI29" s="46"/>
+      <c r="AJ29" s="48"/>
+      <c r="AK29" s="46"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
       <c r="K30" s="2"/>
+      <c r="AG30" s="46"/>
+      <c r="AH30" s="47"/>
+      <c r="AI30" s="46"/>
+      <c r="AJ30" s="48"/>
+      <c r="AK30" s="46"/>
+    </row>
+    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="AG31" s="46"/>
+      <c r="AH31" s="47"/>
+      <c r="AI31" s="46"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="46"/>
+    </row>
+    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="AG32" s="46"/>
+      <c r="AH32" s="47"/>
+      <c r="AI32" s="46"/>
+      <c r="AJ32" s="48"/>
+      <c r="AK32" s="46"/>
+    </row>
+    <row r="33" spans="33:37" x14ac:dyDescent="0.2">
+      <c r="AG33" s="46"/>
+      <c r="AH33" s="46"/>
+      <c r="AI33" s="46"/>
+      <c r="AJ33" s="48"/>
+      <c r="AK33" s="46"/>
+    </row>
+    <row r="34" spans="33:37" x14ac:dyDescent="0.2">
+      <c r="AG34" s="46"/>
+      <c r="AH34" s="46"/>
+      <c r="AI34" s="46"/>
+      <c r="AJ34" s="46"/>
+      <c r="AK34" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="73">
     <mergeCell ref="AC3:AE3"/>
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="AC5:AD5"/>
@@ -2877,8 +3706,129 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AI17:AJ17"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AO17:AP17"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AR4:AT4"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AR17:AS17"/>
+    <mergeCell ref="AR18:AS18"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AO5:AP5"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J16">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:M16">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P7:P16">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S7:S16">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V7:V16">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y7:Y16">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB7:AB16">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE7:AE16">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH7:AH16">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2890,7 +3840,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7:M16">
+  <conditionalFormatting sqref="AK7:AK16">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2902,43 +3852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:P16">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S7:S16">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V7:V16">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y7:Y16">
+  <conditionalFormatting sqref="AN7:AN16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2950,7 +3864,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB7:AB16">
+  <conditionalFormatting sqref="AQ7:AQ16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2962,7 +3876,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE7:AE16">
+  <conditionalFormatting sqref="AT7:AT16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2975,6 +3889,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="76" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="42" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add no-ras run to overview
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1B66D-E91C-F846-980A-85ADBB14A817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72920E09-D20D-104E-B642-D9228E989BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -1012,6 +1012,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1024,7 +1042,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1036,47 +1075,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1397,8 +1397,8 @@
   </sheetPr>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="57" workbookViewId="0">
-      <selection activeCell="AL24" sqref="AL24"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,228 +1453,228 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="T3" s="53" t="s">
+      <c r="T3" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53" t="s">
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53" t="s">
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53" t="s">
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53" t="s">
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="53"/>
-      <c r="AN3" s="53"/>
-      <c r="AO3" s="53"/>
-      <c r="AP3" s="53"/>
-      <c r="AQ3" s="53"/>
-      <c r="AR3" s="53"/>
-      <c r="AS3" s="53"/>
-      <c r="AT3" s="53"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="49"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="49"/>
+      <c r="AO3" s="49"/>
+      <c r="AP3" s="49"/>
+      <c r="AQ3" s="49"/>
+      <c r="AR3" s="49"/>
+      <c r="AS3" s="49"/>
+      <c r="AT3" s="49"/>
     </row>
     <row r="4" spans="1:49" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="67" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="67" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="59" t="s">
+      <c r="G4" s="64"/>
+      <c r="H4" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="59" t="s">
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="59" t="s">
+      <c r="L4" s="51"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="59" t="s">
+      <c r="O4" s="51"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="60"/>
-      <c r="S4" s="61"/>
-      <c r="T4" s="59" t="s">
+      <c r="R4" s="51"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="60"/>
-      <c r="V4" s="61"/>
-      <c r="W4" s="59" t="s">
+      <c r="U4" s="51"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="59" t="s">
+      <c r="X4" s="51"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="60"/>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="59" t="s">
+      <c r="AA4" s="51"/>
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="60"/>
-      <c r="AE4" s="61"/>
-      <c r="AF4" s="59" t="s">
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="52"/>
+      <c r="AF4" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="59" t="s">
+      <c r="AG4" s="51"/>
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="AJ4" s="60"/>
-      <c r="AK4" s="61"/>
-      <c r="AL4" s="59" t="s">
+      <c r="AJ4" s="51"/>
+      <c r="AK4" s="52"/>
+      <c r="AL4" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="AM4" s="60"/>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="54" t="s">
+      <c r="AM4" s="51"/>
+      <c r="AN4" s="52"/>
+      <c r="AO4" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="AP4" s="55"/>
-      <c r="AQ4" s="62"/>
-      <c r="AR4" s="54" t="s">
+      <c r="AP4" s="68"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="AS4" s="55"/>
-      <c r="AT4" s="56"/>
+      <c r="AS4" s="68"/>
+      <c r="AT4" s="69"/>
     </row>
     <row r="5" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="63" t="s">
+      <c r="C5" s="66"/>
+      <c r="D5" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="64"/>
-      <c r="F5" s="63" t="s">
+      <c r="E5" s="66"/>
+      <c r="F5" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="64"/>
-      <c r="H5" s="57" t="s">
+      <c r="G5" s="66"/>
+      <c r="H5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="58"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="58"/>
+      <c r="L5" s="54"/>
       <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="57" t="s">
+      <c r="N5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="58"/>
+      <c r="O5" s="54"/>
       <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="57" t="s">
+      <c r="Q5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="58"/>
+      <c r="R5" s="54"/>
       <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="57" t="s">
+      <c r="T5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="58"/>
+      <c r="U5" s="54"/>
       <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="57" t="s">
+      <c r="W5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="58"/>
+      <c r="X5" s="54"/>
       <c r="Y5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Z5" s="57" t="s">
+      <c r="Z5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="58"/>
+      <c r="AA5" s="54"/>
       <c r="AB5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" s="57" t="s">
+      <c r="AC5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="58"/>
+      <c r="AD5" s="54"/>
       <c r="AE5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="57" t="s">
+      <c r="AF5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AG5" s="58"/>
+      <c r="AG5" s="54"/>
       <c r="AH5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AI5" s="57" t="s">
+      <c r="AI5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AJ5" s="58"/>
+      <c r="AJ5" s="54"/>
       <c r="AK5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AL5" s="57" t="s">
+      <c r="AL5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AM5" s="58"/>
+      <c r="AM5" s="54"/>
       <c r="AN5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AO5" s="57" t="s">
+      <c r="AO5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AP5" s="58"/>
+      <c r="AP5" s="54"/>
       <c r="AQ5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AR5" s="57" t="s">
+      <c r="AR5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="AS5" s="58"/>
+      <c r="AS5" s="54"/>
       <c r="AT5" s="16" t="s">
         <v>16</v>
       </c>
@@ -1948,11 +1948,15 @@
         <f>AI7/$F7</f>
         <v>0.68220064724919094</v>
       </c>
-      <c r="AL7" s="21"/>
-      <c r="AM7" s="22"/>
+      <c r="AL7" s="21">
+        <v>2560</v>
+      </c>
+      <c r="AM7" s="22">
+        <v>0.69299999999999995</v>
+      </c>
       <c r="AN7" s="13">
         <f>AL7/$F7</f>
-        <v>0</v>
+        <v>0.82847896440129454</v>
       </c>
       <c r="AO7" s="21"/>
       <c r="AP7" s="22"/>
@@ -2093,11 +2097,15 @@
         <f t="shared" ref="AK8:AK16" si="9">AI8/$F8</f>
         <v>0.53270198283515835</v>
       </c>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="24"/>
+      <c r="AL8" s="23">
+        <v>2383</v>
+      </c>
+      <c r="AM8" s="24">
+        <v>1.67</v>
+      </c>
       <c r="AN8" s="14">
         <f t="shared" ref="AN8:AN16" si="10">AL8/$F8</f>
-        <v>0</v>
+        <v>0.70523823616454573</v>
       </c>
       <c r="AO8" s="23"/>
       <c r="AP8" s="24"/>
@@ -2238,11 +2246,15 @@
         <f t="shared" si="9"/>
         <v>0.78511627906976744</v>
       </c>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="24"/>
+      <c r="AL9" s="23">
+        <v>3061</v>
+      </c>
+      <c r="AM9" s="24">
+        <v>1.54</v>
+      </c>
       <c r="AN9" s="14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.94914728682170546</v>
       </c>
       <c r="AO9" s="23"/>
       <c r="AP9" s="24"/>
@@ -2383,11 +2395,15 @@
         <f t="shared" si="9"/>
         <v>0.64477726574500771</v>
       </c>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="24"/>
+      <c r="AL10" s="23">
+        <v>2396</v>
+      </c>
+      <c r="AM10" s="24">
+        <v>0.68100000000000005</v>
+      </c>
       <c r="AN10" s="14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.92012288786482332</v>
       </c>
       <c r="AO10" s="23"/>
       <c r="AP10" s="24"/>
@@ -2528,11 +2544,15 @@
         <f t="shared" si="9"/>
         <v>0.59842519685039375</v>
       </c>
-      <c r="AL11" s="23"/>
-      <c r="AM11" s="24"/>
+      <c r="AL11" s="23">
+        <v>1399</v>
+      </c>
+      <c r="AM11" s="24">
+        <v>1.01</v>
+      </c>
       <c r="AN11" s="14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.84736523319200485</v>
       </c>
       <c r="AO11" s="23"/>
       <c r="AP11" s="24"/>
@@ -2673,11 +2693,15 @@
         <f t="shared" si="9"/>
         <v>0.93779904306220097</v>
       </c>
-      <c r="AL12" s="23"/>
-      <c r="AM12" s="24"/>
+      <c r="AL12" s="23">
+        <v>2906</v>
+      </c>
+      <c r="AM12" s="24">
+        <v>0.60699999999999998</v>
+      </c>
       <c r="AN12" s="14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.99316473000683525</v>
       </c>
       <c r="AO12" s="23"/>
       <c r="AP12" s="24"/>
@@ -2818,11 +2842,15 @@
         <f t="shared" si="9"/>
         <v>0.61522717969709373</v>
       </c>
-      <c r="AL13" s="23"/>
-      <c r="AM13" s="24"/>
+      <c r="AL13" s="23">
+        <v>2337</v>
+      </c>
+      <c r="AM13" s="24">
+        <v>0.61299999999999999</v>
+      </c>
       <c r="AN13" s="14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.95661072451903395</v>
       </c>
       <c r="AO13" s="23"/>
       <c r="AP13" s="24"/>
@@ -2963,11 +2991,15 @@
         <f t="shared" si="9"/>
         <v>0.59225440806045337</v>
       </c>
-      <c r="AL14" s="23"/>
-      <c r="AM14" s="24"/>
+      <c r="AL14" s="23">
+        <v>2796</v>
+      </c>
+      <c r="AM14" s="24">
+        <v>0.61</v>
+      </c>
       <c r="AN14" s="14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.88035264483627207</v>
       </c>
       <c r="AO14" s="23"/>
       <c r="AP14" s="24"/>
@@ -3108,11 +3140,15 @@
         <f t="shared" si="9"/>
         <v>0.65221318879855461</v>
       </c>
-      <c r="AL15" s="23"/>
-      <c r="AM15" s="24"/>
+      <c r="AL15" s="23">
+        <v>1455</v>
+      </c>
+      <c r="AM15" s="24">
+        <v>2.02</v>
+      </c>
       <c r="AN15" s="14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.65718157181571812</v>
       </c>
       <c r="AO15" s="23"/>
       <c r="AP15" s="24"/>
@@ -3253,11 +3289,15 @@
         <f t="shared" si="9"/>
         <v>0.83955600403632691</v>
       </c>
-      <c r="AL16" s="44"/>
-      <c r="AM16" s="45"/>
+      <c r="AL16" s="44">
+        <v>7620</v>
+      </c>
+      <c r="AM16" s="45">
+        <v>0.81100000000000005</v>
+      </c>
       <c r="AN16" s="15">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.85435586949209552</v>
       </c>
       <c r="AO16" s="44"/>
       <c r="AP16" s="45"/>
@@ -3276,106 +3316,106 @@
       </c>
     </row>
     <row r="17" spans="1:50" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="69" t="s">
+      <c r="C17" s="60"/>
+      <c r="D17" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="70"/>
-      <c r="F17" s="69" t="s">
+      <c r="E17" s="60"/>
+      <c r="F17" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="49" t="s">
+      <c r="G17" s="60"/>
+      <c r="H17" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="50"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="49" t="s">
+      <c r="K17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="50"/>
+      <c r="L17" s="56"/>
       <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="49" t="s">
+      <c r="N17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="50"/>
+      <c r="O17" s="56"/>
       <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="49" t="s">
+      <c r="Q17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="50"/>
+      <c r="R17" s="56"/>
       <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="49" t="s">
+      <c r="T17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="50"/>
+      <c r="U17" s="56"/>
       <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="W17" s="49" t="s">
+      <c r="W17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="50"/>
+      <c r="X17" s="56"/>
       <c r="Y17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Z17" s="49" t="s">
+      <c r="Z17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AA17" s="50"/>
+      <c r="AA17" s="56"/>
       <c r="AB17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AC17" s="49" t="s">
+      <c r="AC17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AD17" s="50"/>
+      <c r="AD17" s="56"/>
       <c r="AE17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AF17" s="49" t="s">
+      <c r="AF17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AG17" s="50"/>
+      <c r="AG17" s="56"/>
       <c r="AH17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AI17" s="49" t="s">
+      <c r="AI17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AJ17" s="50"/>
+      <c r="AJ17" s="56"/>
       <c r="AK17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AL17" s="49" t="s">
+      <c r="AL17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AM17" s="50"/>
+      <c r="AM17" s="56"/>
       <c r="AN17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AO17" s="49" t="s">
+      <c r="AO17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AP17" s="50"/>
+      <c r="AP17" s="56"/>
       <c r="AQ17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AR17" s="49" t="s">
+      <c r="AR17" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="AS17" s="50"/>
+      <c r="AS17" s="56"/>
       <c r="AT17" s="20" t="s">
         <v>31</v>
       </c>
@@ -3383,111 +3423,113 @@
       <c r="AX17" s="43"/>
     </row>
     <row r="18" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="65">
+      <c r="B18" s="61">
         <v>2.52</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="65">
+      <c r="C18" s="62"/>
+      <c r="D18" s="61">
         <v>1.35</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="65">
+      <c r="E18" s="62"/>
+      <c r="F18" s="61">
         <v>0.78869999999999996</v>
       </c>
-      <c r="G18" s="66"/>
-      <c r="H18" s="51">
+      <c r="G18" s="62"/>
+      <c r="H18" s="57">
         <v>0.3337</v>
       </c>
-      <c r="I18" s="52"/>
+      <c r="I18" s="58"/>
       <c r="J18" s="27">
         <f>$F$18/H18</f>
         <v>2.3635001498351813</v>
       </c>
-      <c r="K18" s="51">
+      <c r="K18" s="57">
         <v>0.31390000000000001</v>
       </c>
-      <c r="L18" s="52"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="27">
         <f>$F$18/K18</f>
         <v>2.5125836253583942</v>
       </c>
-      <c r="N18" s="51">
+      <c r="N18" s="57">
         <v>0.35489999999999999</v>
       </c>
-      <c r="O18" s="52"/>
+      <c r="O18" s="58"/>
       <c r="P18" s="27">
         <f>$F$18/N18</f>
         <v>2.2223161453930684</v>
       </c>
-      <c r="Q18" s="51">
+      <c r="Q18" s="57">
         <v>0.34489999999999998</v>
       </c>
-      <c r="R18" s="52"/>
+      <c r="R18" s="58"/>
       <c r="S18" s="27">
         <f>$F$18/Q18</f>
         <v>2.2867497825456655</v>
       </c>
-      <c r="T18" s="51">
+      <c r="T18" s="57">
         <v>1.05</v>
       </c>
-      <c r="U18" s="52"/>
+      <c r="U18" s="58"/>
       <c r="V18" s="27">
         <f>$F$18/T18</f>
         <v>0.75114285714285711</v>
       </c>
-      <c r="W18" s="51">
+      <c r="W18" s="57">
         <v>1.1100000000000001</v>
       </c>
-      <c r="X18" s="52"/>
+      <c r="X18" s="58"/>
       <c r="Y18" s="27">
         <f>$F$18/W18</f>
         <v>0.71054054054054039</v>
       </c>
-      <c r="Z18" s="51">
+      <c r="Z18" s="57">
         <v>1.18</v>
       </c>
-      <c r="AA18" s="52"/>
+      <c r="AA18" s="58"/>
       <c r="AB18" s="27">
         <f>$F$18/Z18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AC18" s="51" t="s">
+      <c r="AC18" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="AD18" s="52"/>
+      <c r="AD18" s="58"/>
       <c r="AE18" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="AF18" s="51">
+      <c r="AF18" s="57">
         <v>1.18</v>
       </c>
-      <c r="AG18" s="52"/>
+      <c r="AG18" s="58"/>
       <c r="AH18" s="27">
         <f>$F$18/AF18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AI18" s="51">
+      <c r="AI18" s="57">
         <v>1.1599999999999999</v>
       </c>
-      <c r="AJ18" s="52"/>
+      <c r="AJ18" s="58"/>
       <c r="AK18" s="27">
         <f>$F$18/AI18</f>
         <v>0.67991379310344824</v>
       </c>
-      <c r="AL18" s="51"/>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="27" t="e">
+      <c r="AL18" s="57">
+        <v>0.92510000000000003</v>
+      </c>
+      <c r="AM18" s="58"/>
+      <c r="AN18" s="27">
         <f>$F$18/AL18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AO18" s="51"/>
-      <c r="AP18" s="52"/>
+        <v>0.85255648038049936</v>
+      </c>
+      <c r="AO18" s="57"/>
+      <c r="AP18" s="58"/>
       <c r="AQ18" s="27" t="e">
         <f>$F$18/AO18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AR18" s="51"/>
-      <c r="AS18" s="52"/>
+      <c r="AR18" s="57"/>
+      <c r="AS18" s="58"/>
       <c r="AT18" s="27" t="e">
         <f>$F$18/AR18</f>
         <v>#DIV/0!</v>
@@ -3658,38 +3700,31 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="AO17:AP17"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AR4:AT4"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AR17:AS17"/>
+    <mergeCell ref="AR18:AS18"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AI17:AJ17"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="W3:Y3"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="B5:C5"/>
@@ -3706,31 +3741,38 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="AI17:AJ17"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="AI18:AJ18"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AO17:AP17"/>
-    <mergeCell ref="AL18:AM18"/>
-    <mergeCell ref="AO18:AP18"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AR4:AT4"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="AR17:AS17"/>
-    <mergeCell ref="AR18:AS18"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AL4:AN4"/>
-    <mergeCell ref="AO4:AQ4"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J16">
     <cfRule type="colorScale" priority="16">

</xml_diff>

<commit_message>
style and fix optimisation comparison figure
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72920E09-D20D-104E-B642-D9228E989BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E6575E-F665-3744-AC58-FB317FDE14C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -1012,9 +1012,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1024,59 +1051,32 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1397,8 +1397,8 @@
   </sheetPr>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="AM21" sqref="AM21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,228 +1453,228 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="T3" s="49" t="s">
+      <c r="T3" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49" t="s">
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49" t="s">
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49" t="s">
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49" t="s">
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="AG3" s="49"/>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-      <c r="AJ3" s="49"/>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="49"/>
-      <c r="AM3" s="49"/>
-      <c r="AN3" s="49"/>
-      <c r="AO3" s="49"/>
-      <c r="AP3" s="49"/>
-      <c r="AQ3" s="49"/>
-      <c r="AR3" s="49"/>
-      <c r="AS3" s="49"/>
-      <c r="AT3" s="49"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="53"/>
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="53"/>
+      <c r="AM3" s="53"/>
+      <c r="AN3" s="53"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="53"/>
+      <c r="AQ3" s="53"/>
+      <c r="AR3" s="53"/>
+      <c r="AS3" s="53"/>
+      <c r="AT3" s="53"/>
     </row>
     <row r="4" spans="1:49" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="63" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="63" t="s">
+      <c r="E4" s="68"/>
+      <c r="F4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="50" t="s">
+      <c r="G4" s="68"/>
+      <c r="H4" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="50" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="50" t="s">
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="50" t="s">
+      <c r="O4" s="60"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="51"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="50" t="s">
+      <c r="R4" s="60"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="51"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="50" t="s">
+      <c r="U4" s="60"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="50" t="s">
+      <c r="X4" s="60"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="50" t="s">
+      <c r="AA4" s="60"/>
+      <c r="AB4" s="61"/>
+      <c r="AC4" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="51"/>
-      <c r="AE4" s="52"/>
-      <c r="AF4" s="50" t="s">
+      <c r="AD4" s="60"/>
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="AG4" s="51"/>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="50" t="s">
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="AJ4" s="51"/>
-      <c r="AK4" s="52"/>
-      <c r="AL4" s="50" t="s">
+      <c r="AJ4" s="60"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="AM4" s="51"/>
-      <c r="AN4" s="52"/>
-      <c r="AO4" s="67" t="s">
+      <c r="AM4" s="60"/>
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="AP4" s="68"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="67" t="s">
+      <c r="AP4" s="55"/>
+      <c r="AQ4" s="62"/>
+      <c r="AR4" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="AS4" s="68"/>
-      <c r="AT4" s="69"/>
+      <c r="AS4" s="55"/>
+      <c r="AT4" s="56"/>
     </row>
     <row r="5" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="65" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="65" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="66"/>
-      <c r="H5" s="53" t="s">
+      <c r="G5" s="64"/>
+      <c r="H5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="54"/>
+      <c r="I5" s="58"/>
       <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="54"/>
+      <c r="L5" s="58"/>
       <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="53" t="s">
+      <c r="N5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="54"/>
+      <c r="O5" s="58"/>
       <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="53" t="s">
+      <c r="Q5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="54"/>
+      <c r="R5" s="58"/>
       <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="53" t="s">
+      <c r="T5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="54"/>
+      <c r="U5" s="58"/>
       <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="53" t="s">
+      <c r="W5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="54"/>
+      <c r="X5" s="58"/>
       <c r="Y5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Z5" s="53" t="s">
+      <c r="Z5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="54"/>
+      <c r="AA5" s="58"/>
       <c r="AB5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" s="53" t="s">
+      <c r="AC5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="54"/>
+      <c r="AD5" s="58"/>
       <c r="AE5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="53" t="s">
+      <c r="AF5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AG5" s="54"/>
+      <c r="AG5" s="58"/>
       <c r="AH5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AI5" s="53" t="s">
+      <c r="AI5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AJ5" s="54"/>
+      <c r="AJ5" s="58"/>
       <c r="AK5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AL5" s="53" t="s">
+      <c r="AL5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AM5" s="54"/>
+      <c r="AM5" s="58"/>
       <c r="AN5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AO5" s="53" t="s">
+      <c r="AO5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AP5" s="54"/>
+      <c r="AP5" s="58"/>
       <c r="AQ5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AR5" s="53" t="s">
+      <c r="AR5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AS5" s="54"/>
+      <c r="AS5" s="58"/>
       <c r="AT5" s="16" t="s">
         <v>16</v>
       </c>
@@ -3316,106 +3316,106 @@
       </c>
     </row>
     <row r="17" spans="1:50" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="59" t="s">
+      <c r="C17" s="70"/>
+      <c r="D17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="59" t="s">
+      <c r="E17" s="70"/>
+      <c r="F17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="55" t="s">
+      <c r="G17" s="70"/>
+      <c r="H17" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="56"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="55" t="s">
+      <c r="K17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="56"/>
+      <c r="L17" s="50"/>
       <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="55" t="s">
+      <c r="N17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="56"/>
+      <c r="O17" s="50"/>
       <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="55" t="s">
+      <c r="Q17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="56"/>
+      <c r="R17" s="50"/>
       <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="55" t="s">
+      <c r="T17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="56"/>
+      <c r="U17" s="50"/>
       <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="W17" s="55" t="s">
+      <c r="W17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="56"/>
+      <c r="X17" s="50"/>
       <c r="Y17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Z17" s="55" t="s">
+      <c r="Z17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AA17" s="56"/>
+      <c r="AA17" s="50"/>
       <c r="AB17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AC17" s="55" t="s">
+      <c r="AC17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AD17" s="56"/>
+      <c r="AD17" s="50"/>
       <c r="AE17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AF17" s="55" t="s">
+      <c r="AF17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AG17" s="56"/>
+      <c r="AG17" s="50"/>
       <c r="AH17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AI17" s="55" t="s">
+      <c r="AI17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AJ17" s="56"/>
+      <c r="AJ17" s="50"/>
       <c r="AK17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AL17" s="55" t="s">
+      <c r="AL17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AM17" s="56"/>
+      <c r="AM17" s="50"/>
       <c r="AN17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AO17" s="55" t="s">
+      <c r="AO17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AP17" s="56"/>
+      <c r="AP17" s="50"/>
       <c r="AQ17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AR17" s="55" t="s">
+      <c r="AR17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AS17" s="56"/>
+      <c r="AS17" s="50"/>
       <c r="AT17" s="20" t="s">
         <v>31</v>
       </c>
@@ -3423,113 +3423,113 @@
       <c r="AX17" s="43"/>
     </row>
     <row r="18" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="61">
+      <c r="B18" s="65">
         <v>2.52</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="61">
+      <c r="C18" s="66"/>
+      <c r="D18" s="65">
         <v>1.35</v>
       </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="61">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <v>0.78869999999999996</v>
       </c>
-      <c r="G18" s="62"/>
-      <c r="H18" s="57">
+      <c r="G18" s="66"/>
+      <c r="H18" s="51">
         <v>0.3337</v>
       </c>
-      <c r="I18" s="58"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="27">
         <f>$F$18/H18</f>
         <v>2.3635001498351813</v>
       </c>
-      <c r="K18" s="57">
+      <c r="K18" s="51">
         <v>0.31390000000000001</v>
       </c>
-      <c r="L18" s="58"/>
+      <c r="L18" s="52"/>
       <c r="M18" s="27">
         <f>$F$18/K18</f>
         <v>2.5125836253583942</v>
       </c>
-      <c r="N18" s="57">
+      <c r="N18" s="51">
         <v>0.35489999999999999</v>
       </c>
-      <c r="O18" s="58"/>
+      <c r="O18" s="52"/>
       <c r="P18" s="27">
         <f>$F$18/N18</f>
         <v>2.2223161453930684</v>
       </c>
-      <c r="Q18" s="57">
+      <c r="Q18" s="51">
         <v>0.34489999999999998</v>
       </c>
-      <c r="R18" s="58"/>
+      <c r="R18" s="52"/>
       <c r="S18" s="27">
         <f>$F$18/Q18</f>
         <v>2.2867497825456655</v>
       </c>
-      <c r="T18" s="57">
+      <c r="T18" s="51">
         <v>1.05</v>
       </c>
-      <c r="U18" s="58"/>
+      <c r="U18" s="52"/>
       <c r="V18" s="27">
         <f>$F$18/T18</f>
         <v>0.75114285714285711</v>
       </c>
-      <c r="W18" s="57">
+      <c r="W18" s="51">
         <v>1.1100000000000001</v>
       </c>
-      <c r="X18" s="58"/>
+      <c r="X18" s="52"/>
       <c r="Y18" s="27">
         <f>$F$18/W18</f>
         <v>0.71054054054054039</v>
       </c>
-      <c r="Z18" s="57">
+      <c r="Z18" s="51">
         <v>1.18</v>
       </c>
-      <c r="AA18" s="58"/>
+      <c r="AA18" s="52"/>
       <c r="AB18" s="27">
         <f>$F$18/Z18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AC18" s="57" t="s">
+      <c r="AC18" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AD18" s="58"/>
+      <c r="AD18" s="52"/>
       <c r="AE18" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="AF18" s="57">
+      <c r="AF18" s="51">
         <v>1.18</v>
       </c>
-      <c r="AG18" s="58"/>
+      <c r="AG18" s="52"/>
       <c r="AH18" s="27">
         <f>$F$18/AF18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AI18" s="57">
+      <c r="AI18" s="51">
         <v>1.1599999999999999</v>
       </c>
-      <c r="AJ18" s="58"/>
+      <c r="AJ18" s="52"/>
       <c r="AK18" s="27">
         <f>$F$18/AI18</f>
         <v>0.67991379310344824</v>
       </c>
-      <c r="AL18" s="57">
+      <c r="AL18" s="51">
         <v>0.92510000000000003</v>
       </c>
-      <c r="AM18" s="58"/>
+      <c r="AM18" s="52"/>
       <c r="AN18" s="27">
         <f>$F$18/AL18</f>
         <v>0.85255648038049936</v>
       </c>
-      <c r="AO18" s="57"/>
-      <c r="AP18" s="58"/>
+      <c r="AO18" s="51"/>
+      <c r="AP18" s="52"/>
       <c r="AQ18" s="27" t="e">
         <f>$F$18/AO18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AR18" s="57"/>
-      <c r="AS18" s="58"/>
+      <c r="AR18" s="51"/>
+      <c r="AS18" s="52"/>
       <c r="AT18" s="27" t="e">
         <f>$F$18/AR18</f>
         <v>#DIV/0!</v>
@@ -3558,6 +3558,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="K21" s="2"/>
+      <c r="AL21" s="43"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -3700,31 +3701,38 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="AO17:AP17"/>
-    <mergeCell ref="AL18:AM18"/>
-    <mergeCell ref="AO18:AP18"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AR4:AT4"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="AR17:AS17"/>
-    <mergeCell ref="AR18:AS18"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AL4:AN4"/>
-    <mergeCell ref="AO4:AQ4"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="AI17:AJ17"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="AI18:AJ18"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="W3:Y3"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="B5:C5"/>
@@ -3741,38 +3749,31 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AI17:AJ17"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AO17:AP17"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AR4:AT4"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AR17:AS17"/>
+    <mergeCell ref="AR18:AS18"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AO5:AP5"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J16">
     <cfRule type="colorScale" priority="16">

</xml_diff>

<commit_message>
add none-run results to paper, various fixes
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B080FE56-F3F5-5C42-AA04-B9C9DC40804C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A248C3B6-4C6E-7F45-B483-7FE6D9B43DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19780" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="61">
   <si>
     <t>Benchmark</t>
   </si>
@@ -459,7 +459,10 @@
     </r>
   </si>
   <si>
-    <t>INVALID</t>
+    <t>Average Ratio</t>
+  </si>
+  <si>
+    <t>Factor to optimized</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -923,11 +926,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1015,9 +1027,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,23 +1066,26 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1051,35 +1093,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1400,8 +1430,8 @@
   </sheetPr>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="AK8" sqref="AK8"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="AR15" sqref="AR15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,10 +1455,10 @@
     <col min="32" max="40" width="13.33203125" customWidth="1"/>
     <col min="41" max="41" width="15.5" customWidth="1"/>
     <col min="42" max="42" width="15.6640625" customWidth="1"/>
-    <col min="43" max="43" width="16.5" customWidth="1"/>
+    <col min="43" max="43" width="16" customWidth="1"/>
     <col min="44" max="44" width="12.5" customWidth="1"/>
     <col min="45" max="45" width="13.33203125" customWidth="1"/>
-    <col min="46" max="46" width="12.1640625" customWidth="1"/>
+    <col min="46" max="46" width="13.83203125" customWidth="1"/>
     <col min="47" max="47" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1456,229 +1486,229 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="T3" s="49" t="s">
+      <c r="T3" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49" t="s">
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49" t="s">
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49" t="s">
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="49" t="s">
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="AG3" s="49"/>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-      <c r="AJ3" s="49"/>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="49"/>
-      <c r="AM3" s="49"/>
-      <c r="AN3" s="49"/>
-      <c r="AO3" s="49"/>
-      <c r="AP3" s="49"/>
-      <c r="AQ3" s="49"/>
-      <c r="AR3" s="49"/>
-      <c r="AS3" s="49"/>
-      <c r="AT3" s="49"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="53"/>
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="53"/>
+      <c r="AM3" s="53"/>
+      <c r="AN3" s="53"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="53"/>
+      <c r="AQ3" s="53"/>
+      <c r="AR3" s="53"/>
+      <c r="AS3" s="53"/>
+      <c r="AT3" s="53"/>
     </row>
     <row r="4" spans="1:49" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="63" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="63" t="s">
+      <c r="E4" s="68"/>
+      <c r="F4" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="50" t="s">
+      <c r="G4" s="68"/>
+      <c r="H4" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="50" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="50" t="s">
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="50" t="s">
+      <c r="O4" s="60"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="51"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="50" t="s">
+      <c r="R4" s="60"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="51"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="50" t="s">
+      <c r="U4" s="60"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="50" t="s">
+      <c r="X4" s="60"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="50" t="s">
+      <c r="AA4" s="60"/>
+      <c r="AB4" s="61"/>
+      <c r="AC4" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="51"/>
-      <c r="AE4" s="52"/>
-      <c r="AF4" s="50" t="s">
+      <c r="AD4" s="60"/>
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="AG4" s="51"/>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="50" t="s">
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="AJ4" s="51"/>
-      <c r="AK4" s="52"/>
-      <c r="AL4" s="50" t="s">
+      <c r="AJ4" s="60"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="AM4" s="51"/>
-      <c r="AN4" s="52"/>
-      <c r="AO4" s="67" t="s">
+      <c r="AM4" s="60"/>
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="AP4" s="68"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="67" t="s">
+      <c r="AP4" s="55"/>
+      <c r="AQ4" s="62"/>
+      <c r="AR4" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="AS4" s="68"/>
-      <c r="AT4" s="69"/>
+      <c r="AS4" s="55"/>
+      <c r="AT4" s="56"/>
     </row>
     <row r="5" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="65" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="65" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="66"/>
-      <c r="H5" s="53" t="s">
+      <c r="G5" s="64"/>
+      <c r="H5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="54"/>
+      <c r="I5" s="58"/>
       <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="54"/>
+      <c r="L5" s="58"/>
       <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="53" t="s">
+      <c r="N5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="54"/>
+      <c r="O5" s="58"/>
       <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="53" t="s">
+      <c r="Q5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="54"/>
+      <c r="R5" s="58"/>
       <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="53" t="s">
+      <c r="T5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="54"/>
+      <c r="U5" s="58"/>
       <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="53" t="s">
+      <c r="W5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="54"/>
+      <c r="X5" s="58"/>
       <c r="Y5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Z5" s="53" t="s">
+      <c r="Z5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="54"/>
+      <c r="AA5" s="58"/>
       <c r="AB5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" s="53" t="s">
+      <c r="AC5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="54"/>
+      <c r="AD5" s="58"/>
       <c r="AE5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="53" t="s">
+      <c r="AF5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="16" t="s">
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AI5" s="53" t="s">
+      <c r="AI5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AJ5" s="54"/>
-      <c r="AK5" s="16" t="s">
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AL5" s="53" t="s">
+      <c r="AL5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AM5" s="54"/>
-      <c r="AN5" s="16" t="s">
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AO5" s="53" t="s">
+      <c r="AO5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AP5" s="54"/>
-      <c r="AQ5" s="16" t="s">
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AR5" s="53" t="s">
+      <c r="AR5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="AS5" s="54"/>
-      <c r="AT5" s="16" t="s">
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="76" t="s">
         <v>16</v>
       </c>
       <c r="AU5" s="28" t="s">
@@ -2128,11 +2158,15 @@
         <f t="shared" ref="AQ8:AQ16" si="11">AO8/$F8</f>
         <v>0.81828943474400706</v>
       </c>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="24"/>
+      <c r="AR8" s="23">
+        <v>14072</v>
+      </c>
+      <c r="AS8" s="24">
+        <v>0.28299999999999997</v>
+      </c>
       <c r="AT8" s="14">
         <f t="shared" ref="AT8:AT16" si="12">AR8/$F8</f>
-        <v>0</v>
+        <v>4.1645457235868601</v>
       </c>
       <c r="AU8" s="31" t="s">
         <v>4</v>
@@ -2281,11 +2315,15 @@
         <f t="shared" si="11"/>
         <v>0.94232558139534883</v>
       </c>
-      <c r="AR9" s="23"/>
-      <c r="AS9" s="24"/>
+      <c r="AR9" s="23">
+        <v>9127</v>
+      </c>
+      <c r="AS9" s="24">
+        <v>0.51700000000000002</v>
+      </c>
       <c r="AT9" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2.8300775193798451</v>
       </c>
       <c r="AU9" s="31" t="s">
         <v>5</v>
@@ -2434,11 +2472,15 @@
         <f t="shared" si="11"/>
         <v>1.0238095238095237</v>
       </c>
-      <c r="AR10" s="23"/>
-      <c r="AS10" s="24"/>
+      <c r="AR10" s="23">
+        <v>8557</v>
+      </c>
+      <c r="AS10" s="24">
+        <v>0.191</v>
+      </c>
       <c r="AT10" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.2860983102918588</v>
       </c>
       <c r="AU10" s="31" t="s">
         <v>6</v>
@@ -2744,11 +2786,15 @@
         <f t="shared" si="11"/>
         <v>0.99350649350649356</v>
       </c>
-      <c r="AR12" s="23"/>
-      <c r="AS12" s="24"/>
+      <c r="AR12" s="23">
+        <v>6750</v>
+      </c>
+      <c r="AS12" s="24">
+        <v>0.26100000000000001</v>
+      </c>
       <c r="AT12" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2.3069036226930963</v>
       </c>
       <c r="AU12" s="31" t="s">
         <v>8</v>
@@ -2897,11 +2943,15 @@
         <f t="shared" si="11"/>
         <v>0.95333606221858369</v>
       </c>
-      <c r="AR13" s="23"/>
-      <c r="AS13" s="24"/>
+      <c r="AR13" s="23">
+        <v>11064</v>
+      </c>
+      <c r="AS13" s="24">
+        <v>0.13</v>
+      </c>
       <c r="AT13" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.5288579615227178</v>
       </c>
       <c r="AU13" s="31" t="s">
         <v>9</v>
@@ -3050,11 +3100,15 @@
         <f t="shared" si="11"/>
         <v>0.88916876574307302</v>
       </c>
-      <c r="AR14" s="23"/>
-      <c r="AS14" s="24"/>
+      <c r="AR14" s="23">
+        <v>10375</v>
+      </c>
+      <c r="AS14" s="24">
+        <v>0.16400000000000001</v>
+      </c>
       <c r="AT14" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.2666876574307304</v>
       </c>
       <c r="AU14" s="31" t="s">
         <v>10</v>
@@ -3367,106 +3421,106 @@
       </c>
     </row>
     <row r="17" spans="1:50" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="59" t="s">
+      <c r="C17" s="70"/>
+      <c r="D17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="59" t="s">
+      <c r="E17" s="70"/>
+      <c r="F17" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="60"/>
-      <c r="H17" s="55" t="s">
+      <c r="G17" s="70"/>
+      <c r="H17" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="56"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="55" t="s">
+      <c r="K17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="56"/>
+      <c r="L17" s="50"/>
       <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="55" t="s">
+      <c r="N17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="56"/>
+      <c r="O17" s="50"/>
       <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="55" t="s">
+      <c r="Q17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="56"/>
+      <c r="R17" s="50"/>
       <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="55" t="s">
+      <c r="T17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="56"/>
+      <c r="U17" s="50"/>
       <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="W17" s="55" t="s">
+      <c r="W17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="56"/>
+      <c r="X17" s="50"/>
       <c r="Y17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Z17" s="55" t="s">
+      <c r="Z17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AA17" s="56"/>
+      <c r="AA17" s="50"/>
       <c r="AB17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AC17" s="55" t="s">
+      <c r="AC17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AD17" s="56"/>
+      <c r="AD17" s="50"/>
       <c r="AE17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AF17" s="55" t="s">
+      <c r="AF17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AG17" s="56"/>
+      <c r="AG17" s="50"/>
       <c r="AH17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AI17" s="55" t="s">
+      <c r="AI17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AJ17" s="56"/>
+      <c r="AJ17" s="50"/>
       <c r="AK17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AL17" s="55" t="s">
+      <c r="AL17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AM17" s="56"/>
+      <c r="AM17" s="50"/>
       <c r="AN17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AO17" s="55" t="s">
+      <c r="AO17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AP17" s="56"/>
+      <c r="AP17" s="50"/>
       <c r="AQ17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AR17" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="AS17" s="56"/>
+      <c r="AR17" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS17" s="50"/>
       <c r="AT17" s="20" t="s">
         <v>31</v>
       </c>
@@ -3474,152 +3528,199 @@
       <c r="AX17" s="43"/>
     </row>
     <row r="18" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="61">
+      <c r="B18" s="65">
         <v>2.52</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="61">
+      <c r="C18" s="66"/>
+      <c r="D18" s="65">
         <v>1.35</v>
       </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="61">
+      <c r="E18" s="66"/>
+      <c r="F18" s="65">
         <v>0.78869999999999996</v>
       </c>
-      <c r="G18" s="62"/>
-      <c r="H18" s="57">
+      <c r="G18" s="66"/>
+      <c r="H18" s="51">
         <v>0.3337</v>
       </c>
-      <c r="I18" s="58"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="27">
         <f>$F$18/H18</f>
         <v>2.3635001498351813</v>
       </c>
-      <c r="K18" s="57">
+      <c r="K18" s="51">
         <v>0.31390000000000001</v>
       </c>
-      <c r="L18" s="58"/>
+      <c r="L18" s="52"/>
       <c r="M18" s="27">
         <f>$F$18/K18</f>
         <v>2.5125836253583942</v>
       </c>
-      <c r="N18" s="57">
+      <c r="N18" s="51">
         <v>0.35489999999999999</v>
       </c>
-      <c r="O18" s="58"/>
+      <c r="O18" s="52"/>
       <c r="P18" s="27">
         <f>$F$18/N18</f>
         <v>2.2223161453930684</v>
       </c>
-      <c r="Q18" s="57">
+      <c r="Q18" s="51">
         <v>0.34489999999999998</v>
       </c>
-      <c r="R18" s="58"/>
+      <c r="R18" s="52"/>
       <c r="S18" s="27">
         <f>$F$18/Q18</f>
         <v>2.2867497825456655</v>
       </c>
-      <c r="T18" s="57">
+      <c r="T18" s="51">
         <v>1.05</v>
       </c>
-      <c r="U18" s="58"/>
+      <c r="U18" s="52"/>
       <c r="V18" s="27">
         <f>$F$18/T18</f>
         <v>0.75114285714285711</v>
       </c>
-      <c r="W18" s="57">
+      <c r="W18" s="51">
         <v>1.1100000000000001</v>
       </c>
-      <c r="X18" s="58"/>
+      <c r="X18" s="52"/>
       <c r="Y18" s="27">
         <f>$F$18/W18</f>
         <v>0.71054054054054039</v>
       </c>
-      <c r="Z18" s="57">
+      <c r="Z18" s="51">
         <v>1.18</v>
       </c>
-      <c r="AA18" s="58"/>
+      <c r="AA18" s="52"/>
       <c r="AB18" s="27">
         <f>$F$18/Z18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AC18" s="57" t="s">
+      <c r="AC18" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AD18" s="58"/>
+      <c r="AD18" s="52"/>
       <c r="AE18" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="AF18" s="57">
+      <c r="AF18" s="51">
         <v>1.18</v>
       </c>
-      <c r="AG18" s="58"/>
+      <c r="AG18" s="52"/>
       <c r="AH18" s="27">
         <f>$F$18/AF18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AI18" s="57">
+      <c r="AI18" s="51">
         <v>1.1599999999999999</v>
       </c>
-      <c r="AJ18" s="58"/>
+      <c r="AJ18" s="52"/>
       <c r="AK18" s="27">
         <f>$F$18/AI18</f>
         <v>0.67991379310344824</v>
       </c>
-      <c r="AL18" s="57">
+      <c r="AL18" s="51">
         <v>0.92510000000000003</v>
       </c>
-      <c r="AM18" s="58"/>
+      <c r="AM18" s="52"/>
       <c r="AN18" s="27">
         <f>$F$18/AL18</f>
         <v>0.85255648038049936</v>
       </c>
-      <c r="AO18" s="57">
+      <c r="AO18" s="51">
         <v>0.89019999999999999</v>
       </c>
-      <c r="AP18" s="58"/>
+      <c r="AP18" s="52"/>
       <c r="AQ18" s="27">
         <f>$F$18/AO18</f>
         <v>0.88598067849921358</v>
       </c>
-      <c r="AR18" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS18" s="58"/>
-      <c r="AT18" s="27" t="s">
-        <v>59</v>
+      <c r="AR18" s="71">
+        <f>AVERAGE(AS7:AS16)</f>
+        <v>0.23224999999999998</v>
+      </c>
+      <c r="AS18" s="52"/>
+      <c r="AT18" s="27">
+        <f>AVERAGE(G7:G16)/AR18</f>
+        <v>3.6374596340150696</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
+    <row r="19" spans="1:50" ht="19" x14ac:dyDescent="0.25">
+      <c r="AF19" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG19" s="72"/>
+      <c r="AH19" s="73"/>
+      <c r="AI19" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ19" s="72"/>
+      <c r="AK19" s="73"/>
+      <c r="AL19" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM19" s="72"/>
+      <c r="AN19" s="73"/>
+      <c r="AO19" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP19" s="72"/>
+      <c r="AQ19" s="73"/>
+      <c r="AR19" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS19" s="72"/>
+      <c r="AT19" s="73"/>
+    </row>
+    <row r="20" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="K20" s="2"/>
+      <c r="AF20" s="71">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="74"/>
+      <c r="AH20" s="75"/>
+      <c r="AI20" s="71">
+        <f>$AF$18/AI18</f>
+        <v>1.0172413793103448</v>
+      </c>
+      <c r="AJ20" s="74"/>
+      <c r="AK20" s="75"/>
+      <c r="AL20" s="71">
+        <f>$AF$18/AL18</f>
+        <v>1.2755377796994918</v>
+      </c>
+      <c r="AM20" s="74"/>
+      <c r="AN20" s="75"/>
+      <c r="AO20" s="71">
+        <f>$AF$18/AO18</f>
+        <v>1.325544821388452</v>
+      </c>
+      <c r="AP20" s="74"/>
+      <c r="AQ20" s="75"/>
+      <c r="AR20" s="71">
+        <f>AVERAGE(AG7:AG16)/AR18</f>
+        <v>5.5341227125941872</v>
+      </c>
+      <c r="AS20" s="74"/>
+      <c r="AT20" s="75"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="K21" s="2"/>
+      <c r="AG21" s="43"/>
       <c r="AL21" s="43"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -3633,10 +3734,10 @@
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -3650,10 +3751,10 @@
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -3666,8 +3767,11 @@
       <c r="AK24" s="46"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="K25" s="2"/>
       <c r="AG25" s="46"/>
@@ -3678,10 +3782,10 @@
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -3694,6 +3798,9 @@
       <c r="AK26" s="46"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="AG27" s="46"/>
       <c r="AH27" s="47"/>
@@ -3702,6 +3809,12 @@
       <c r="AK27" s="46"/>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
       <c r="K28" s="2"/>
       <c r="AG28" s="46"/>
       <c r="AH28" s="47"/>
@@ -3754,32 +3867,49 @@
       <c r="AK34" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="AO17:AP17"/>
-    <mergeCell ref="AL18:AM18"/>
-    <mergeCell ref="AO18:AP18"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AR4:AT4"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="AR17:AS17"/>
-    <mergeCell ref="AR18:AS18"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AL4:AN4"/>
-    <mergeCell ref="AO4:AQ4"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="AI17:AJ17"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="AI18:AJ18"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AI5:AJ5"/>
+  <mergeCells count="83">
+    <mergeCell ref="AL19:AN19"/>
+    <mergeCell ref="AL20:AN20"/>
+    <mergeCell ref="AI19:AK19"/>
+    <mergeCell ref="AI20:AK20"/>
+    <mergeCell ref="AF19:AH19"/>
+    <mergeCell ref="AF20:AH20"/>
+    <mergeCell ref="AR19:AT19"/>
+    <mergeCell ref="AR20:AT20"/>
+    <mergeCell ref="AO19:AQ19"/>
+    <mergeCell ref="AO20:AQ20"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="W3:Y3"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="B5:C5"/>
@@ -3796,38 +3926,31 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AI17:AJ17"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AO17:AP17"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AR4:AT4"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AR17:AS17"/>
+    <mergeCell ref="AR18:AS18"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AO5:AP5"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J16">
     <cfRule type="colorScale" priority="16">

</xml_diff>

<commit_message>
add remaining benchmark results
</commit_message>
<xml_diff>
--- a/documentation/spec/results/results.xlsx
+++ b/documentation/spec/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flo/Dropbox/Universität/TUM Informatik BSc/2 - SoSe 20/d - ERA-GP/eragp-dbt-2020/documentation/spec/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A248C3B6-4C6E-7F45-B483-7FE6D9B43DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C102DD9D-A812-1048-91CE-41970CA25624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19780" xr2:uid="{3B1D7D53-693A-CC4B-99C9-F7AE6D80617F}"/>
   </bookViews>
@@ -352,9 +352,6 @@
     </r>
   </si>
   <si>
-    <t>finalized…</t>
-  </si>
-  <si>
     <r>
       <t>v1.3.1</t>
     </r>
@@ -463,6 +460,9 @@
   </si>
   <si>
     <t>Factor to optimized</t>
+  </si>
+  <si>
+    <t>Final version…</t>
   </si>
 </sst>
 </file>
@@ -1027,6 +1027,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1039,7 +1075,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1051,65 +1108,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1431,7 +1431,7 @@
   <dimension ref="A1:AX34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="AR15" sqref="AR15"/>
+      <selection activeCell="AF4" sqref="AF4:AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1486,229 +1486,229 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="T3" s="53" t="s">
+      <c r="T3" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53" t="s">
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53" t="s">
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53" t="s">
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="53"/>
-      <c r="AN3" s="53"/>
-      <c r="AO3" s="53"/>
-      <c r="AP3" s="53"/>
-      <c r="AQ3" s="53"/>
-      <c r="AR3" s="53"/>
-      <c r="AS3" s="53"/>
-      <c r="AT3" s="53"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG3" s="56"/>
+      <c r="AH3" s="56"/>
+      <c r="AI3" s="56"/>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="56"/>
+      <c r="AP3" s="56"/>
+      <c r="AQ3" s="56"/>
+      <c r="AR3" s="56"/>
+      <c r="AS3" s="56"/>
+      <c r="AT3" s="56"/>
     </row>
     <row r="4" spans="1:49" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="67" t="s">
+      <c r="C4" s="70"/>
+      <c r="D4" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="67" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="59" t="s">
+      <c r="G4" s="70"/>
+      <c r="H4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="59" t="s">
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="59" t="s">
+      <c r="L4" s="58"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="59" t="s">
+      <c r="O4" s="58"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="60"/>
-      <c r="S4" s="61"/>
-      <c r="T4" s="59" t="s">
+      <c r="R4" s="58"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="60"/>
-      <c r="V4" s="61"/>
-      <c r="W4" s="59" t="s">
+      <c r="U4" s="58"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="59" t="s">
+      <c r="X4" s="58"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="60"/>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="59" t="s">
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="60"/>
-      <c r="AE4" s="61"/>
-      <c r="AF4" s="59" t="s">
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="59" t="s">
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="59"/>
+      <c r="AI4" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ4" s="58"/>
+      <c r="AK4" s="59"/>
+      <c r="AL4" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="AJ4" s="60"/>
-      <c r="AK4" s="61"/>
-      <c r="AL4" s="59" t="s">
+      <c r="AM4" s="58"/>
+      <c r="AN4" s="59"/>
+      <c r="AO4" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="AM4" s="60"/>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="54" t="s">
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="AP4" s="55"/>
-      <c r="AQ4" s="62"/>
-      <c r="AR4" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS4" s="55"/>
-      <c r="AT4" s="56"/>
+      <c r="AS4" s="74"/>
+      <c r="AT4" s="75"/>
     </row>
     <row r="5" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="63" t="s">
+      <c r="C5" s="72"/>
+      <c r="D5" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="64"/>
-      <c r="F5" s="63" t="s">
+      <c r="E5" s="72"/>
+      <c r="F5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="64"/>
-      <c r="H5" s="57" t="s">
+      <c r="G5" s="72"/>
+      <c r="H5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="58"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="58"/>
+      <c r="L5" s="60"/>
       <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="57" t="s">
+      <c r="N5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="58"/>
+      <c r="O5" s="60"/>
       <c r="P5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="57" t="s">
+      <c r="Q5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="58"/>
+      <c r="R5" s="60"/>
       <c r="S5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="57" t="s">
+      <c r="T5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="58"/>
+      <c r="U5" s="60"/>
       <c r="V5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="57" t="s">
+      <c r="W5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="58"/>
+      <c r="X5" s="60"/>
       <c r="Y5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Z5" s="57" t="s">
+      <c r="Z5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="58"/>
+      <c r="AA5" s="60"/>
       <c r="AB5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" s="57" t="s">
+      <c r="AC5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="58"/>
+      <c r="AD5" s="60"/>
       <c r="AE5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="57" t="s">
+      <c r="AF5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AG5" s="58"/>
-      <c r="AH5" s="76" t="s">
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AI5" s="57" t="s">
+      <c r="AI5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AJ5" s="58"/>
-      <c r="AK5" s="76" t="s">
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AL5" s="57" t="s">
+      <c r="AL5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="76" t="s">
+      <c r="AM5" s="60"/>
+      <c r="AN5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AO5" s="57" t="s">
+      <c r="AO5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AP5" s="58"/>
-      <c r="AQ5" s="76" t="s">
+      <c r="AP5" s="60"/>
+      <c r="AQ5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AR5" s="57" t="s">
+      <c r="AR5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AS5" s="58"/>
-      <c r="AT5" s="76" t="s">
+      <c r="AS5" s="60"/>
+      <c r="AT5" s="49" t="s">
         <v>16</v>
       </c>
       <c r="AU5" s="28" t="s">
@@ -3257,11 +3257,15 @@
         <f t="shared" si="11"/>
         <v>0.65808491418247517</v>
       </c>
-      <c r="AR15" s="23"/>
-      <c r="AS15" s="24"/>
+      <c r="AR15" s="23">
+        <v>12630</v>
+      </c>
+      <c r="AS15" s="24">
+        <v>0.23300000000000001</v>
+      </c>
       <c r="AT15" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5.7046070460704605</v>
       </c>
       <c r="AU15" s="31" t="s">
         <v>11</v>
@@ -3410,117 +3414,121 @@
         <f t="shared" si="11"/>
         <v>0.85816795604888441</v>
       </c>
-      <c r="AR16" s="44"/>
-      <c r="AS16" s="45"/>
+      <c r="AR16" s="44">
+        <v>30085</v>
+      </c>
+      <c r="AS16" s="45">
+        <v>0.20499999999999999</v>
+      </c>
       <c r="AT16" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.3731360017939229</v>
       </c>
       <c r="AU16" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:50" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="69" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="70"/>
-      <c r="F17" s="69" t="s">
+      <c r="E17" s="66"/>
+      <c r="F17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="49" t="s">
+      <c r="G17" s="66"/>
+      <c r="H17" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="50"/>
+      <c r="I17" s="62"/>
       <c r="J17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="49" t="s">
+      <c r="K17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="50"/>
+      <c r="L17" s="62"/>
       <c r="M17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="N17" s="49" t="s">
+      <c r="N17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="O17" s="50"/>
+      <c r="O17" s="62"/>
       <c r="P17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="49" t="s">
+      <c r="Q17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="50"/>
+      <c r="R17" s="62"/>
       <c r="S17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="49" t="s">
+      <c r="T17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="50"/>
+      <c r="U17" s="62"/>
       <c r="V17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="W17" s="49" t="s">
+      <c r="W17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="50"/>
+      <c r="X17" s="62"/>
       <c r="Y17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Z17" s="49" t="s">
+      <c r="Z17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="AA17" s="50"/>
+      <c r="AA17" s="62"/>
       <c r="AB17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AC17" s="49" t="s">
+      <c r="AC17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="AD17" s="50"/>
+      <c r="AD17" s="62"/>
       <c r="AE17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AF17" s="49" t="s">
+      <c r="AF17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="AG17" s="50"/>
+      <c r="AG17" s="62"/>
       <c r="AH17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AI17" s="49" t="s">
+      <c r="AI17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="AJ17" s="50"/>
+      <c r="AJ17" s="62"/>
       <c r="AK17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AL17" s="49" t="s">
+      <c r="AL17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="AM17" s="50"/>
+      <c r="AM17" s="62"/>
       <c r="AN17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AO17" s="49" t="s">
+      <c r="AO17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="AP17" s="50"/>
+      <c r="AP17" s="62"/>
       <c r="AQ17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AR17" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS17" s="50"/>
+      <c r="AR17" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS17" s="62"/>
       <c r="AT17" s="20" t="s">
         <v>31</v>
       </c>
@@ -3528,184 +3536,184 @@
       <c r="AX17" s="43"/>
     </row>
     <row r="18" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="65">
+      <c r="B18" s="67">
         <v>2.52</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="65">
+      <c r="C18" s="68"/>
+      <c r="D18" s="67">
         <v>1.35</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="65">
+      <c r="E18" s="68"/>
+      <c r="F18" s="67">
         <v>0.78869999999999996</v>
       </c>
-      <c r="G18" s="66"/>
-      <c r="H18" s="51">
+      <c r="G18" s="68"/>
+      <c r="H18" s="63">
         <v>0.3337</v>
       </c>
-      <c r="I18" s="52"/>
+      <c r="I18" s="64"/>
       <c r="J18" s="27">
         <f>$F$18/H18</f>
         <v>2.3635001498351813</v>
       </c>
-      <c r="K18" s="51">
+      <c r="K18" s="63">
         <v>0.31390000000000001</v>
       </c>
-      <c r="L18" s="52"/>
+      <c r="L18" s="64"/>
       <c r="M18" s="27">
         <f>$F$18/K18</f>
         <v>2.5125836253583942</v>
       </c>
-      <c r="N18" s="51">
+      <c r="N18" s="63">
         <v>0.35489999999999999</v>
       </c>
-      <c r="O18" s="52"/>
+      <c r="O18" s="64"/>
       <c r="P18" s="27">
         <f>$F$18/N18</f>
         <v>2.2223161453930684</v>
       </c>
-      <c r="Q18" s="51">
+      <c r="Q18" s="63">
         <v>0.34489999999999998</v>
       </c>
-      <c r="R18" s="52"/>
+      <c r="R18" s="64"/>
       <c r="S18" s="27">
         <f>$F$18/Q18</f>
         <v>2.2867497825456655</v>
       </c>
-      <c r="T18" s="51">
+      <c r="T18" s="63">
         <v>1.05</v>
       </c>
-      <c r="U18" s="52"/>
+      <c r="U18" s="64"/>
       <c r="V18" s="27">
         <f>$F$18/T18</f>
         <v>0.75114285714285711</v>
       </c>
-      <c r="W18" s="51">
+      <c r="W18" s="63">
         <v>1.1100000000000001</v>
       </c>
-      <c r="X18" s="52"/>
+      <c r="X18" s="64"/>
       <c r="Y18" s="27">
         <f>$F$18/W18</f>
         <v>0.71054054054054039</v>
       </c>
-      <c r="Z18" s="51">
+      <c r="Z18" s="63">
         <v>1.18</v>
       </c>
-      <c r="AA18" s="52"/>
+      <c r="AA18" s="64"/>
       <c r="AB18" s="27">
         <f>$F$18/Z18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AC18" s="51" t="s">
+      <c r="AC18" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="AD18" s="52"/>
+      <c r="AD18" s="64"/>
       <c r="AE18" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="AF18" s="51">
+      <c r="AF18" s="63">
         <v>1.18</v>
       </c>
-      <c r="AG18" s="52"/>
+      <c r="AG18" s="64"/>
       <c r="AH18" s="27">
         <f>$F$18/AF18</f>
         <v>0.66838983050847456</v>
       </c>
-      <c r="AI18" s="51">
+      <c r="AI18" s="63">
         <v>1.1599999999999999</v>
       </c>
-      <c r="AJ18" s="52"/>
+      <c r="AJ18" s="64"/>
       <c r="AK18" s="27">
         <f>$F$18/AI18</f>
         <v>0.67991379310344824</v>
       </c>
-      <c r="AL18" s="51">
+      <c r="AL18" s="63">
         <v>0.92510000000000003</v>
       </c>
-      <c r="AM18" s="52"/>
+      <c r="AM18" s="64"/>
       <c r="AN18" s="27">
         <f>$F$18/AL18</f>
         <v>0.85255648038049936</v>
       </c>
-      <c r="AO18" s="51">
+      <c r="AO18" s="63">
         <v>0.89019999999999999</v>
       </c>
-      <c r="AP18" s="52"/>
+      <c r="AP18" s="64"/>
       <c r="AQ18" s="27">
         <f>$F$18/AO18</f>
         <v>0.88598067849921358</v>
       </c>
-      <c r="AR18" s="71">
+      <c r="AR18" s="53">
         <f>AVERAGE(AS7:AS16)</f>
-        <v>0.23224999999999998</v>
-      </c>
-      <c r="AS18" s="52"/>
+        <v>0.22959999999999997</v>
+      </c>
+      <c r="AS18" s="64"/>
       <c r="AT18" s="27">
         <f>AVERAGE(G7:G16)/AR18</f>
-        <v>3.6374596340150696</v>
+        <v>3.6794425087108014</v>
       </c>
     </row>
     <row r="19" spans="1:50" ht="19" x14ac:dyDescent="0.25">
-      <c r="AF19" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG19" s="72"/>
-      <c r="AH19" s="73"/>
-      <c r="AI19" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ19" s="72"/>
-      <c r="AK19" s="73"/>
-      <c r="AL19" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM19" s="72"/>
-      <c r="AN19" s="73"/>
-      <c r="AO19" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP19" s="72"/>
-      <c r="AQ19" s="73"/>
-      <c r="AR19" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="AS19" s="72"/>
-      <c r="AT19" s="73"/>
+      <c r="AF19" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="52"/>
+      <c r="AI19" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ19" s="51"/>
+      <c r="AK19" s="52"/>
+      <c r="AL19" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM19" s="51"/>
+      <c r="AN19" s="52"/>
+      <c r="AO19" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP19" s="51"/>
+      <c r="AQ19" s="52"/>
+      <c r="AR19" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS19" s="51"/>
+      <c r="AT19" s="52"/>
     </row>
     <row r="20" spans="1:50" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="K20" s="2"/>
-      <c r="AF20" s="71">
+      <c r="AF20" s="53">
         <v>1</v>
       </c>
-      <c r="AG20" s="74"/>
-      <c r="AH20" s="75"/>
-      <c r="AI20" s="71">
+      <c r="AG20" s="54"/>
+      <c r="AH20" s="55"/>
+      <c r="AI20" s="53">
         <f>$AF$18/AI18</f>
         <v>1.0172413793103448</v>
       </c>
-      <c r="AJ20" s="74"/>
-      <c r="AK20" s="75"/>
-      <c r="AL20" s="71">
+      <c r="AJ20" s="54"/>
+      <c r="AK20" s="55"/>
+      <c r="AL20" s="53">
         <f>$AF$18/AL18</f>
         <v>1.2755377796994918</v>
       </c>
-      <c r="AM20" s="74"/>
-      <c r="AN20" s="75"/>
-      <c r="AO20" s="71">
+      <c r="AM20" s="54"/>
+      <c r="AN20" s="55"/>
+      <c r="AO20" s="53">
         <f>$AF$18/AO18</f>
         <v>1.325544821388452</v>
       </c>
-      <c r="AP20" s="74"/>
-      <c r="AQ20" s="75"/>
-      <c r="AR20" s="71">
+      <c r="AP20" s="54"/>
+      <c r="AQ20" s="55"/>
+      <c r="AR20" s="53">
         <f>AVERAGE(AG7:AG16)/AR18</f>
-        <v>5.5341227125941872</v>
-      </c>
-      <c r="AS20" s="74"/>
-      <c r="AT20" s="75"/>
+        <v>5.5979965156794425</v>
+      </c>
+      <c r="AS20" s="54"/>
+      <c r="AT20" s="55"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.2">
       <c r="C21" s="3"/>
@@ -3868,48 +3876,24 @@
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="AL19:AN19"/>
-    <mergeCell ref="AL20:AN20"/>
-    <mergeCell ref="AI19:AK19"/>
-    <mergeCell ref="AI20:AK20"/>
-    <mergeCell ref="AF19:AH19"/>
-    <mergeCell ref="AF20:AH20"/>
-    <mergeCell ref="AR19:AT19"/>
-    <mergeCell ref="AR20:AT20"/>
-    <mergeCell ref="AO19:AQ19"/>
-    <mergeCell ref="AO20:AQ20"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="AO17:AP17"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AO18:AP18"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AR4:AT4"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AR17:AS17"/>
+    <mergeCell ref="AR18:AS18"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AO4:AQ4"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="W3:Y3"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="B5:C5"/>
@@ -3926,6 +3910,42 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="AR19:AT19"/>
+    <mergeCell ref="AR20:AT20"/>
+    <mergeCell ref="AO19:AQ19"/>
+    <mergeCell ref="AO20:AQ20"/>
+    <mergeCell ref="AC3:AE3"/>
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
     <mergeCell ref="AF17:AG17"/>
     <mergeCell ref="AI17:AJ17"/>
     <mergeCell ref="AF18:AG18"/>
@@ -3933,24 +3953,12 @@
     <mergeCell ref="AL3:AN3"/>
     <mergeCell ref="AL17:AM17"/>
     <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AF4:AH4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AO17:AP17"/>
-    <mergeCell ref="AL18:AM18"/>
-    <mergeCell ref="AO18:AP18"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AR4:AT4"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="AR17:AS17"/>
-    <mergeCell ref="AR18:AS18"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AL4:AN4"/>
-    <mergeCell ref="AO4:AQ4"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AL19:AN19"/>
+    <mergeCell ref="AL20:AN20"/>
+    <mergeCell ref="AI19:AK19"/>
+    <mergeCell ref="AI20:AK20"/>
+    <mergeCell ref="AF19:AH19"/>
+    <mergeCell ref="AF20:AH20"/>
   </mergeCells>
   <conditionalFormatting sqref="J7:J16">
     <cfRule type="colorScale" priority="16">

</xml_diff>